<commit_message>
Create function to assess dumpsite scores
</commit_message>
<xml_diff>
--- a/data/lookup_tables.xlsx
+++ b/data/lookup_tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\srucker\Documents\GitHub\SCI\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0C1EA98-09B1-4786-9A6D-8C67792D785B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DB99BD2-0229-4434-841B-1962CFE22845}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{FC8AAFAA-1B2E-4A6F-8639-F15C3BC242A6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{FC8AAFAA-1B2E-4A6F-8639-F15C3BC242A6}"/>
   </bookViews>
   <sheets>
     <sheet name="dumpsite_score" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="68">
   <si>
     <t>max_sites_per_mile</t>
   </si>
@@ -47,9 +47,6 @@
     <t>score</t>
   </si>
   <si>
-    <t>impact</t>
-  </si>
-  <si>
     <t>severe</t>
   </si>
   <si>
@@ -240,6 +237,12 @@
   </si>
   <si>
     <t>mainstem_connectivity_status</t>
+  </si>
+  <si>
+    <t>d_impact</t>
+  </si>
+  <si>
+    <t>none</t>
   </si>
 </sst>
 </file>
@@ -694,44 +697,52 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF0D815C-FD9D-4123-9D9D-AD3295A2835E}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="B1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2">
-        <v>3</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -751,7 +762,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -759,7 +770,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2">
         <v>10</v>
@@ -767,7 +778,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3">
         <v>7</v>
@@ -775,7 +786,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4">
         <v>4</v>
@@ -783,7 +794,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -798,8 +809,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B281CBBA-5423-42AE-9693-0C69866CF5CE}">
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -811,13 +822,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" t="s">
         <v>65</v>
-      </c>
-      <c r="B1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C1" t="s">
-        <v>66</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -825,13 +836,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D2">
         <v>10</v>
@@ -839,13 +850,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
         <v>13</v>
       </c>
-      <c r="B3" t="s">
-        <v>14</v>
-      </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D3">
         <v>10</v>
@@ -853,13 +864,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
         <v>15</v>
       </c>
-      <c r="B4" t="s">
-        <v>16</v>
-      </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D4">
         <v>10</v>
@@ -867,13 +878,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
         <v>17</v>
       </c>
-      <c r="B5" t="s">
-        <v>18</v>
-      </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D5">
         <v>10</v>
@@ -881,13 +892,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
         <v>19</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>20</v>
-      </c>
-      <c r="C6" t="s">
-        <v>21</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -895,13 +906,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" t="s">
         <v>22</v>
       </c>
-      <c r="B7" t="s">
-        <v>23</v>
-      </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D7">
         <v>10</v>
@@ -909,13 +920,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" t="s">
         <v>24</v>
       </c>
-      <c r="B8" t="s">
-        <v>25</v>
-      </c>
       <c r="C8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -923,13 +934,13 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" t="s">
         <v>26</v>
       </c>
-      <c r="B9" t="s">
-        <v>27</v>
-      </c>
       <c r="C9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -937,13 +948,13 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" t="s">
         <v>28</v>
       </c>
-      <c r="B10" t="s">
-        <v>29</v>
-      </c>
       <c r="C10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -951,13 +962,13 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" t="s">
         <v>30</v>
       </c>
-      <c r="B11" t="s">
-        <v>31</v>
-      </c>
       <c r="C11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -965,13 +976,13 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" t="s">
         <v>32</v>
       </c>
-      <c r="B12" t="s">
-        <v>33</v>
-      </c>
       <c r="C12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D12">
         <v>10</v>
@@ -979,13 +990,13 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" t="s">
         <v>34</v>
       </c>
-      <c r="B13" t="s">
-        <v>35</v>
-      </c>
       <c r="C13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -993,13 +1004,13 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" t="s">
         <v>36</v>
       </c>
-      <c r="B14" t="s">
-        <v>37</v>
-      </c>
       <c r="C14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D14">
         <v>10</v>
@@ -1007,13 +1018,13 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" t="s">
         <v>38</v>
       </c>
-      <c r="B15" t="s">
-        <v>39</v>
-      </c>
       <c r="C15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D15">
         <v>10</v>
@@ -1021,13 +1032,13 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" t="s">
         <v>40</v>
       </c>
-      <c r="B16" t="s">
-        <v>41</v>
-      </c>
       <c r="C16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D16">
         <v>10</v>
@@ -1035,13 +1046,13 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" t="s">
         <v>42</v>
       </c>
-      <c r="B17" t="s">
-        <v>43</v>
-      </c>
       <c r="C17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D17">
         <v>10</v>
@@ -1049,13 +1060,13 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" t="s">
         <v>44</v>
       </c>
-      <c r="B18" t="s">
-        <v>45</v>
-      </c>
       <c r="C18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D18">
         <v>10</v>
@@ -1063,13 +1074,13 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" t="s">
         <v>46</v>
       </c>
-      <c r="B19" t="s">
-        <v>47</v>
-      </c>
       <c r="C19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D19">
         <v>10</v>
@@ -1077,13 +1088,13 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" t="s">
         <v>48</v>
       </c>
-      <c r="B20" t="s">
-        <v>49</v>
-      </c>
       <c r="C20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D20">
         <v>10</v>
@@ -1091,13 +1102,13 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" t="s">
         <v>50</v>
       </c>
-      <c r="B21" t="s">
-        <v>51</v>
-      </c>
       <c r="C21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -1105,13 +1116,13 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22" t="s">
         <v>52</v>
       </c>
-      <c r="B22" t="s">
-        <v>53</v>
-      </c>
       <c r="C22" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D22">
         <v>10</v>
@@ -1119,13 +1130,13 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
+        <v>53</v>
+      </c>
+      <c r="B23" t="s">
         <v>54</v>
       </c>
-      <c r="B23" t="s">
-        <v>55</v>
-      </c>
       <c r="C23" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D23">
         <v>10</v>
@@ -1133,13 +1144,13 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
+        <v>55</v>
+      </c>
+      <c r="B24" t="s">
         <v>56</v>
       </c>
-      <c r="B24" t="s">
-        <v>57</v>
-      </c>
       <c r="C24" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D24">
         <v>10</v>
@@ -1147,13 +1158,13 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
+        <v>57</v>
+      </c>
+      <c r="B25" t="s">
         <v>58</v>
       </c>
-      <c r="B25" t="s">
-        <v>59</v>
-      </c>
       <c r="C25" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D25">
         <v>10</v>
@@ -1161,13 +1172,13 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
+        <v>59</v>
+      </c>
+      <c r="B26" t="s">
         <v>60</v>
       </c>
-      <c r="B26" t="s">
-        <v>61</v>
-      </c>
       <c r="C26" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D26">
         <v>1</v>
@@ -1175,13 +1186,13 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
+        <v>61</v>
+      </c>
+      <c r="B27" t="s">
         <v>62</v>
       </c>
-      <c r="B27" t="s">
-        <v>63</v>
-      </c>
       <c r="C27" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D27">
         <v>10</v>

</xml_diff>

<commit_message>
Summarize EIA subshed area; Impervious area not included
</commit_message>
<xml_diff>
--- a/data/lookup_tables.xlsx
+++ b/data/lookup_tables.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\srucker\Documents\GitHub\SCI\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DB99BD2-0229-4434-841B-1962CFE22845}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B0465A6-38C2-4160-B5F8-1DCB09D734C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{FC8AAFAA-1B2E-4A6F-8639-F15C3BC242A6}"/>
+    <workbookView xWindow="28680" yWindow="-12225" windowWidth="25440" windowHeight="15390" activeTab="4" xr2:uid="{FC8AAFAA-1B2E-4A6F-8639-F15C3BC242A6}"/>
   </bookViews>
   <sheets>
     <sheet name="dumpsite_score" sheetId="1" r:id="rId1"/>
     <sheet name="dumpsite_weight" sheetId="2" r:id="rId2"/>
     <sheet name="trash_score" sheetId="3" r:id="rId3"/>
     <sheet name="connectivity_score" sheetId="4" r:id="rId4"/>
+    <sheet name="eia_area" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="100">
   <si>
     <t>max_sites_per_mile</t>
   </si>
@@ -243,6 +244,102 @@
   </si>
   <si>
     <t>none</t>
+  </si>
+  <si>
+    <t>Rock Creek - Upper - MS4 - Portal Branch</t>
+  </si>
+  <si>
+    <t>Rock Creek - Lower - MS4 - Dumbarton Oaks</t>
+  </si>
+  <si>
+    <t>Rock Creek - Lower - MS4 - Klingle Valley Run</t>
+  </si>
+  <si>
+    <t>Rock Creek - Lower - MS4 - Melvin Hazen Valley Branch</t>
+  </si>
+  <si>
+    <t>Rock Creek - Lower - MS4 - Normanstone Creek</t>
+  </si>
+  <si>
+    <t>Potomac River - Upper - MS4 - Battery Kemble Creek</t>
+  </si>
+  <si>
+    <t>Anacostia River - Upper - MS4 - Fort Davis Tributary</t>
+  </si>
+  <si>
+    <t>Anacostia River - Upper - MS4 - Texas Avenue Tributary</t>
+  </si>
+  <si>
+    <t>Anacostia River - Lower - MS4 - Fort Stanton Tributary</t>
+  </si>
+  <si>
+    <t>Potomac River - Upper - MS4 - Dalecarlia Tributary</t>
+  </si>
+  <si>
+    <t>Anacostia River - Upper - MS4 - Pope Branch</t>
+  </si>
+  <si>
+    <t>Anacostia River - Upper - MS4 - Fort Chaplin Tributary</t>
+  </si>
+  <si>
+    <t>Anacostia River - Upper - MS4 - Fort Dupont Tributary</t>
+  </si>
+  <si>
+    <t>Rock Creek - Upper - MS4 - Soapstone Creek</t>
+  </si>
+  <si>
+    <t>Anacostia River - Upper - MS4 - Nash Run</t>
+  </si>
+  <si>
+    <t>Rock Creek - Upper - MS4 - Luzon Branch</t>
+  </si>
+  <si>
+    <t>Rock Creek - Upper - MS4 - Pinehurst Branch</t>
+  </si>
+  <si>
+    <t>Rock Creek - Upper - MS4 - Fenwick Branch</t>
+  </si>
+  <si>
+    <t>Anacostia River - Upper - MS4 - Hickey Run</t>
+  </si>
+  <si>
+    <t>Potomac River - Upper - MS4 - Foundry Branch</t>
+  </si>
+  <si>
+    <t>Rock Creek - Upper - MS4 - Broad Branch</t>
+  </si>
+  <si>
+    <t>Rock Creek - Lower - CSS - Rock Creek</t>
+  </si>
+  <si>
+    <t>TWB06</t>
+  </si>
+  <si>
+    <t>Anacostia River - Upper - MS4 - Watts Branch - Upper</t>
+  </si>
+  <si>
+    <t>TWB05</t>
+  </si>
+  <si>
+    <t>Anacostia River - Upper - MS4 - Watts Branch - Lower</t>
+  </si>
+  <si>
+    <t>Rock Creek - Lower - MS4 - Piney Branch</t>
+  </si>
+  <si>
+    <t>Potomac River - Lower - MS4 - Oxon Run</t>
+  </si>
+  <si>
+    <t>RCR05</t>
+  </si>
+  <si>
+    <t>Rock Creek - Upper - MS4 - Rock Creek</t>
+  </si>
+  <si>
+    <t>Rock Creek - Lower - MS4 - Rock Creek</t>
+  </si>
+  <si>
+    <t>segment_lookup</t>
   </si>
 </sst>
 </file>
@@ -298,9 +395,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -338,7 +435,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -444,7 +541,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -586,7 +683,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -600,12 +697,12 @@
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -613,7 +710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>10</v>
       </c>
@@ -621,7 +718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>9</v>
       </c>
@@ -629,7 +726,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>8</v>
       </c>
@@ -637,7 +734,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>7</v>
       </c>
@@ -645,7 +742,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>6</v>
       </c>
@@ -653,7 +750,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>5</v>
       </c>
@@ -661,7 +758,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>4</v>
       </c>
@@ -669,7 +766,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>3</v>
       </c>
@@ -677,7 +774,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>2</v>
       </c>
@@ -685,7 +782,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>1</v>
       </c>
@@ -699,13 +796,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF0D815C-FD9D-4123-9D9D-AD3295A2835E}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>66</v>
       </c>
@@ -713,7 +810,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -721,7 +818,7 @@
         <v>-3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -729,7 +826,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -737,7 +834,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>67</v>
       </c>
@@ -758,9 +855,9 @@
       <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -768,7 +865,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -776,7 +873,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -784,7 +881,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -792,7 +889,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -810,17 +907,17 @@
   <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>64</v>
       </c>
@@ -834,7 +931,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -848,7 +945,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -862,7 +959,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -876,7 +973,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -890,7 +987,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -904,7 +1001,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -918,7 +1015,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -932,7 +1029,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -946,7 +1043,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -960,7 +1057,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -974,7 +1071,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>31</v>
       </c>
@@ -988,7 +1085,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>33</v>
       </c>
@@ -1002,7 +1099,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>35</v>
       </c>
@@ -1016,7 +1113,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>37</v>
       </c>
@@ -1030,7 +1127,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>39</v>
       </c>
@@ -1044,7 +1141,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>41</v>
       </c>
@@ -1058,7 +1155,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>43</v>
       </c>
@@ -1072,7 +1169,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>45</v>
       </c>
@@ -1086,7 +1183,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>47</v>
       </c>
@@ -1100,7 +1197,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>49</v>
       </c>
@@ -1114,7 +1211,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>51</v>
       </c>
@@ -1128,7 +1225,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>53</v>
       </c>
@@ -1142,7 +1239,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>55</v>
       </c>
@@ -1156,7 +1253,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>57</v>
       </c>
@@ -1170,7 +1267,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>59</v>
       </c>
@@ -1184,7 +1281,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>61</v>
       </c>
@@ -1196,6 +1293,257 @@
       </c>
       <c r="D27">
         <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50FDDFB2-57CD-4186-8745-C34C09AB75A5}">
+  <dimension ref="A1:B29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="48.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.36328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>75</v>
+      </c>
+      <c r="B9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>76</v>
+      </c>
+      <c r="B10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>77</v>
+      </c>
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>78</v>
+      </c>
+      <c r="B12" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>79</v>
+      </c>
+      <c r="B13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>80</v>
+      </c>
+      <c r="B14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>81</v>
+      </c>
+      <c r="B15" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>82</v>
+      </c>
+      <c r="B16" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>83</v>
+      </c>
+      <c r="B17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>84</v>
+      </c>
+      <c r="B18" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>85</v>
+      </c>
+      <c r="B19" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>86</v>
+      </c>
+      <c r="B20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>87</v>
+      </c>
+      <c r="B21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>88</v>
+      </c>
+      <c r="B22" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>89</v>
+      </c>
+      <c r="B23" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>91</v>
+      </c>
+      <c r="B24" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>93</v>
+      </c>
+      <c r="B25" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>94</v>
+      </c>
+      <c r="B26" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>95</v>
+      </c>
+      <c r="B27" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>97</v>
+      </c>
+      <c r="B28" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>98</v>
+      </c>
+      <c r="B29" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add BMP data for EIA calculation
</commit_message>
<xml_diff>
--- a/data/lookup_tables.xlsx
+++ b/data/lookup_tables.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\srucker\Documents\GitHub\SCI\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B0465A6-38C2-4160-B5F8-1DCB09D734C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B98CE36-78D7-40E7-AEA5-CE8284BE37F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-12225" windowWidth="25440" windowHeight="15390" activeTab="4" xr2:uid="{FC8AAFAA-1B2E-4A6F-8639-F15C3BC242A6}"/>
+    <workbookView xWindow="28680" yWindow="-12225" windowWidth="25440" windowHeight="15390" activeTab="5" xr2:uid="{FC8AAFAA-1B2E-4A6F-8639-F15C3BC242A6}"/>
   </bookViews>
   <sheets>
     <sheet name="dumpsite_score" sheetId="1" r:id="rId1"/>
     <sheet name="dumpsite_weight" sheetId="2" r:id="rId2"/>
     <sheet name="trash_score" sheetId="3" r:id="rId3"/>
     <sheet name="connectivity_score" sheetId="4" r:id="rId4"/>
-    <sheet name="eia_area" sheetId="5" r:id="rId5"/>
+    <sheet name="eia_location_id" sheetId="5" r:id="rId5"/>
+    <sheet name="eia_area" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="103">
   <si>
     <t>max_sites_per_mile</t>
   </si>
@@ -340,6 +341,15 @@
   </si>
   <si>
     <t>segment_lookup</t>
+  </si>
+  <si>
+    <t>sqft</t>
+  </si>
+  <si>
+    <t>Impervious_sqft</t>
+  </si>
+  <si>
+    <t>acres</t>
   </si>
 </sst>
 </file>
@@ -1304,8 +1314,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50FDDFB2-57CD-4186-8745-C34C09AB75A5}">
   <dimension ref="A1:B29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1549,4 +1559,430 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74512946-BFD5-4355-975E-7040C988669E}">
+  <dimension ref="A1:D29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="6.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2">
+        <v>71.444418330000005</v>
+      </c>
+      <c r="C2">
+        <v>5906012.3820000002</v>
+      </c>
+      <c r="D2">
+        <v>2675408.4810000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3">
+        <v>136.07334739999999</v>
+      </c>
+      <c r="C3">
+        <v>5927331.3049999997</v>
+      </c>
+      <c r="D3">
+        <v>1625421.122</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4">
+        <v>171.85245789999999</v>
+      </c>
+      <c r="C4">
+        <v>7485863.1229999997</v>
+      </c>
+      <c r="D4">
+        <v>2819719.7179999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5">
+        <v>174.32630649999999</v>
+      </c>
+      <c r="C5">
+        <v>7593623.5350000001</v>
+      </c>
+      <c r="D5">
+        <v>2576687.5819999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6">
+        <v>217.7788955</v>
+      </c>
+      <c r="C6">
+        <v>9486410.7420000006</v>
+      </c>
+      <c r="D6">
+        <v>3660210.128</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7">
+        <v>231.58095510000001</v>
+      </c>
+      <c r="C7">
+        <v>10087626.050000001</v>
+      </c>
+      <c r="D7">
+        <v>2137233.2710000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8">
+        <v>234.09865740000001</v>
+      </c>
+      <c r="C8">
+        <v>10197296.73</v>
+      </c>
+      <c r="D8">
+        <v>3478720.3960000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9">
+        <v>249.2998709</v>
+      </c>
+      <c r="C9">
+        <v>10859458.939999999</v>
+      </c>
+      <c r="D9">
+        <v>4057289.39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10">
+        <v>276.8609783</v>
+      </c>
+      <c r="C10">
+        <v>12060015.970000001</v>
+      </c>
+      <c r="D10">
+        <v>5035429.9689999996</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11">
+        <v>270.26444609999999</v>
+      </c>
+      <c r="C11">
+        <v>12104505.98</v>
+      </c>
+      <c r="D11">
+        <v>3150624.395</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12">
+        <v>280.45176459999999</v>
+      </c>
+      <c r="C12">
+        <v>12216430</v>
+      </c>
+      <c r="D12">
+        <v>3607941.4730000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13">
+        <v>291.45618960000002</v>
+      </c>
+      <c r="C13">
+        <v>12695780.83</v>
+      </c>
+      <c r="D13">
+        <v>4527052.1179999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14">
+        <v>409.25697700000001</v>
+      </c>
+      <c r="C14">
+        <v>17827162.609999999</v>
+      </c>
+      <c r="D14">
+        <v>1609838.871</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>58</v>
+      </c>
+      <c r="B15">
+        <v>516.37507649999998</v>
+      </c>
+      <c r="C15">
+        <v>22493208.359999999</v>
+      </c>
+      <c r="D15">
+        <v>10075179</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16">
+        <v>472.15890439999998</v>
+      </c>
+      <c r="C16">
+        <v>28262408.210000001</v>
+      </c>
+      <c r="D16">
+        <v>10428891.060000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17">
+        <v>643.53066860000001</v>
+      </c>
+      <c r="C17">
+        <v>28811482.870000001</v>
+      </c>
+      <c r="D17">
+        <v>14779080.73</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18">
+        <v>449.3504049</v>
+      </c>
+      <c r="C18">
+        <v>28934650.41</v>
+      </c>
+      <c r="D18">
+        <v>7336519.3689999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19">
+        <v>220.8060729</v>
+      </c>
+      <c r="C19">
+        <v>41747880.719999999</v>
+      </c>
+      <c r="D19">
+        <v>18710988.010000002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20">
+        <v>1103.8468869999999</v>
+      </c>
+      <c r="C20">
+        <v>48083378.079999998</v>
+      </c>
+      <c r="D20">
+        <v>20152081.27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21">
+        <v>1134.548792</v>
+      </c>
+      <c r="C21">
+        <v>49420747.68</v>
+      </c>
+      <c r="D21">
+        <v>18262208.25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22">
+        <v>1148.451286</v>
+      </c>
+      <c r="C22">
+        <v>51304948.560000002</v>
+      </c>
+      <c r="D22">
+        <v>17934581.789999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23">
+        <v>1603.223352</v>
+      </c>
+      <c r="C23">
+        <v>69836129.849999994</v>
+      </c>
+      <c r="D23">
+        <v>50051478.759999998</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>90</v>
+      </c>
+      <c r="B24">
+        <v>848.33045019999997</v>
+      </c>
+      <c r="C24">
+        <v>90723670.299999997</v>
+      </c>
+      <c r="D24">
+        <v>32039217.879999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>92</v>
+      </c>
+      <c r="B25">
+        <v>410.63448010000002</v>
+      </c>
+      <c r="C25">
+        <v>108610836.7</v>
+      </c>
+      <c r="D25">
+        <v>38050077.590000004</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>56</v>
+      </c>
+      <c r="B26">
+        <v>158.9618614</v>
+      </c>
+      <c r="C26">
+        <v>109878251</v>
+      </c>
+      <c r="D26">
+        <v>57375195.619999997</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>48</v>
+      </c>
+      <c r="B27">
+        <v>2171.0271550000002</v>
+      </c>
+      <c r="C27">
+        <v>414641447.69999999</v>
+      </c>
+      <c r="D27">
+        <v>145300487.90000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>96</v>
+      </c>
+      <c r="B28">
+        <v>1335.459206</v>
+      </c>
+      <c r="C28">
+        <v>797091117.29999995</v>
+      </c>
+      <c r="D28">
+        <v>266505068.69999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>13</v>
+      </c>
+      <c r="B29">
+        <v>925.03015310000001</v>
+      </c>
+      <c r="C29">
+        <v>1033762101</v>
+      </c>
+      <c r="D29">
+        <v>393938764.89999998</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Handle qualifiers in WQ results field
</commit_message>
<xml_diff>
--- a/data/lookup_tables.xlsx
+++ b/data/lookup_tables.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\srucker\Documents\GitHub\SCI\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B98CE36-78D7-40E7-AEA5-CE8284BE37F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3034960-1A62-4757-B79B-06FE19071CAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-12225" windowWidth="25440" windowHeight="15390" activeTab="5" xr2:uid="{FC8AAFAA-1B2E-4A6F-8639-F15C3BC242A6}"/>
+    <workbookView xWindow="28680" yWindow="-12225" windowWidth="25440" windowHeight="15390" xr2:uid="{FC8AAFAA-1B2E-4A6F-8639-F15C3BC242A6}"/>
   </bookViews>
   <sheets>
-    <sheet name="dumpsite_score" sheetId="1" r:id="rId1"/>
-    <sheet name="dumpsite_weight" sheetId="2" r:id="rId2"/>
-    <sheet name="trash_score" sheetId="3" r:id="rId3"/>
-    <sheet name="connectivity_score" sheetId="4" r:id="rId4"/>
-    <sheet name="eia_location_id" sheetId="5" r:id="rId5"/>
-    <sheet name="eia_area" sheetId="6" r:id="rId6"/>
+    <sheet name="location" sheetId="7" r:id="rId1"/>
+    <sheet name="dumpsite_score" sheetId="1" r:id="rId2"/>
+    <sheet name="dumpsite_weight" sheetId="2" r:id="rId3"/>
+    <sheet name="trash_score" sheetId="3" r:id="rId4"/>
+    <sheet name="connectivity_score" sheetId="4" r:id="rId5"/>
+    <sheet name="eia_location_id" sheetId="5" r:id="rId6"/>
+    <sheet name="eia_area" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="105">
   <si>
     <t>max_sites_per_mile</t>
   </si>
@@ -350,6 +351,12 @@
   </si>
   <si>
     <t>acres</t>
+  </si>
+  <si>
+    <t>Watts Branch - Upper</t>
+  </si>
+  <si>
+    <t>location_name</t>
   </si>
 </sst>
 </file>
@@ -700,6 +707,249 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8059EA70-FEB1-4761-8449-3A8139D2BAE4}">
+  <dimension ref="A1:B28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>54</v>
+      </c>
+      <c r="B23" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>56</v>
+      </c>
+      <c r="B24" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>58</v>
+      </c>
+      <c r="B25" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>60</v>
+      </c>
+      <c r="B26" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>62</v>
+      </c>
+      <c r="B27" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>92</v>
+      </c>
+      <c r="B28" t="s">
+        <v>103</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEE4E2E0-88CD-471E-9F5A-AB0C2722050D}">
   <dimension ref="A1:B11"/>
   <sheetViews>
@@ -802,7 +1052,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF0D815C-FD9D-4123-9D9D-AD3295A2835E}">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -857,7 +1107,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BC52232-62A1-4046-A953-F434B4285A01}">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -912,13 +1162,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B281CBBA-5423-42AE-9693-0C69866CF5CE}">
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1310,7 +1558,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50FDDFB2-57CD-4186-8745-C34C09AB75A5}">
   <dimension ref="A1:B29"/>
   <sheetViews>
@@ -1561,17 +1809,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74512946-BFD5-4355-975E-7040C988669E}">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="6.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.36328125" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="11.81640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.26953125" customWidth="1"/>
   </cols>

</xml_diff>

<commit_message>
Create calculations for pH
</commit_message>
<xml_diff>
--- a/data/lookup_tables.xlsx
+++ b/data/lookup_tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\srucker\Documents\GitHub\SCI\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3034960-1A62-4757-B79B-06FE19071CAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9EB4FFF-EDBC-4AD6-BB0A-D160ABA3C082}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-12225" windowWidth="25440" windowHeight="15390" xr2:uid="{FC8AAFAA-1B2E-4A6F-8639-F15C3BC242A6}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{FC8AAFAA-1B2E-4A6F-8639-F15C3BC242A6}"/>
   </bookViews>
   <sheets>
     <sheet name="location" sheetId="7" r:id="rId1"/>
@@ -710,7 +710,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8059EA70-FEB1-4761-8449-3A8139D2BAE4}">
   <dimension ref="A1:B28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
       <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Create function for nitrogen and phosphorus calculations
</commit_message>
<xml_diff>
--- a/data/lookup_tables.xlsx
+++ b/data/lookup_tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\srucker\Documents\GitHub\SCI\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9EB4FFF-EDBC-4AD6-BB0A-D160ABA3C082}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DC42158-8692-438B-A345-A6CC6108B823}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{FC8AAFAA-1B2E-4A6F-8639-F15C3BC242A6}"/>
+    <workbookView xWindow="28680" yWindow="-345" windowWidth="29040" windowHeight="15840" xr2:uid="{FC8AAFAA-1B2E-4A6F-8639-F15C3BC242A6}"/>
   </bookViews>
   <sheets>
     <sheet name="location" sheetId="7" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="108">
   <si>
     <t>max_sites_per_mile</t>
   </si>
@@ -357,6 +357,15 @@
   </si>
   <si>
     <t>location_name</t>
+  </si>
+  <si>
+    <t>Piedmont</t>
+  </si>
+  <si>
+    <t>Coastal Plain</t>
+  </si>
+  <si>
+    <t>ecoregion</t>
   </si>
 </sst>
 </file>
@@ -708,139 +717,185 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8059EA70-FEB1-4761-8449-3A8139D2BAE4}">
-  <dimension ref="A1:B28"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>63</v>
       </c>
       <c r="B1" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
       <c r="B3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
       <c r="B4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>17</v>
       </c>
       <c r="B5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>19</v>
       </c>
       <c r="B6" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C6" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>22</v>
       </c>
       <c r="B7" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C7" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>24</v>
       </c>
       <c r="B8" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C8" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>26</v>
       </c>
       <c r="B9" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C9" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>28</v>
       </c>
       <c r="B10" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C10" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>30</v>
       </c>
       <c r="B11" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C11" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>32</v>
       </c>
       <c r="B12" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C12" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>34</v>
       </c>
       <c r="B13" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C13" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>36</v>
       </c>
       <c r="B14" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C14" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>38</v>
       </c>
       <c r="B15" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C15" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>40</v>
       </c>
@@ -848,100 +903,136 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>42</v>
       </c>
       <c r="B17" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C17" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>44</v>
       </c>
       <c r="B18" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C18" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>46</v>
       </c>
       <c r="B19" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C19" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>48</v>
       </c>
       <c r="B20" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C20" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>50</v>
       </c>
       <c r="B21" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C21" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>52</v>
       </c>
       <c r="B22" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C22" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>54</v>
       </c>
       <c r="B23" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C23" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>56</v>
       </c>
       <c r="B24" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C24" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>58</v>
       </c>
       <c r="B25" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C25" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>60</v>
       </c>
       <c r="B26" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C26" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>62</v>
       </c>
       <c r="B27" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C27" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>92</v>
       </c>
       <c r="B28" t="s">
         <v>103</v>
+      </c>
+      <c r="C28" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -957,12 +1048,12 @@
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -970,7 +1061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>10</v>
       </c>
@@ -978,7 +1069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>9</v>
       </c>
@@ -986,7 +1077,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>8</v>
       </c>
@@ -994,7 +1085,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>7</v>
       </c>
@@ -1002,7 +1093,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>6</v>
       </c>
@@ -1010,7 +1101,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1018,7 +1109,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4</v>
       </c>
@@ -1026,7 +1117,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>3</v>
       </c>
@@ -1034,7 +1125,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2</v>
       </c>
@@ -1042,7 +1133,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1</v>
       </c>
@@ -1060,9 +1151,9 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>66</v>
       </c>
@@ -1070,7 +1161,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1078,7 +1169,7 @@
         <v>-3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1086,7 +1177,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1094,7 +1185,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>67</v>
       </c>
@@ -1115,9 +1206,9 @@
       <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -1125,7 +1216,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1133,7 +1224,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1141,7 +1232,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1149,7 +1240,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1168,14 +1259,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>64</v>
       </c>
@@ -1189,7 +1280,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -1203,7 +1294,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -1217,7 +1308,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -1231,7 +1322,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -1245,7 +1336,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -1259,7 +1350,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -1273,7 +1364,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -1287,7 +1378,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -1301,7 +1392,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -1315,7 +1406,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -1329,7 +1420,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>31</v>
       </c>
@@ -1343,7 +1434,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>33</v>
       </c>
@@ -1357,7 +1448,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>35</v>
       </c>
@@ -1371,7 +1462,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>37</v>
       </c>
@@ -1385,7 +1476,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>39</v>
       </c>
@@ -1399,7 +1490,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>41</v>
       </c>
@@ -1413,7 +1504,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>43</v>
       </c>
@@ -1427,7 +1518,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>45</v>
       </c>
@@ -1441,7 +1532,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>47</v>
       </c>
@@ -1455,7 +1546,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>49</v>
       </c>
@@ -1469,7 +1560,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>51</v>
       </c>
@@ -1483,7 +1574,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>53</v>
       </c>
@@ -1497,7 +1588,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>55</v>
       </c>
@@ -1511,7 +1602,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>57</v>
       </c>
@@ -1525,7 +1616,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>59</v>
       </c>
@@ -1539,7 +1630,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>61</v>
       </c>
@@ -1566,13 +1657,13 @@
       <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="48.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="48.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>99</v>
       </c>
@@ -1580,7 +1671,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>68</v>
       </c>
@@ -1588,7 +1679,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>69</v>
       </c>
@@ -1596,7 +1687,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>70</v>
       </c>
@@ -1604,7 +1695,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>71</v>
       </c>
@@ -1612,7 +1703,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>72</v>
       </c>
@@ -1620,7 +1711,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>73</v>
       </c>
@@ -1628,7 +1719,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>74</v>
       </c>
@@ -1636,7 +1727,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>75</v>
       </c>
@@ -1644,7 +1735,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>76</v>
       </c>
@@ -1652,7 +1743,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>77</v>
       </c>
@@ -1660,7 +1751,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>78</v>
       </c>
@@ -1668,7 +1759,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>79</v>
       </c>
@@ -1676,7 +1767,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>80</v>
       </c>
@@ -1684,7 +1775,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>81</v>
       </c>
@@ -1692,7 +1783,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>82</v>
       </c>
@@ -1700,7 +1791,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>83</v>
       </c>
@@ -1708,7 +1799,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>84</v>
       </c>
@@ -1716,7 +1807,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>85</v>
       </c>
@@ -1724,7 +1815,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>86</v>
       </c>
@@ -1732,7 +1823,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>87</v>
       </c>
@@ -1740,7 +1831,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>88</v>
       </c>
@@ -1748,7 +1839,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>89</v>
       </c>
@@ -1756,7 +1847,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>91</v>
       </c>
@@ -1764,7 +1855,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>93</v>
       </c>
@@ -1772,7 +1863,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>94</v>
       </c>
@@ -1780,7 +1871,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>95</v>
       </c>
@@ -1788,7 +1879,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>97</v>
       </c>
@@ -1796,7 +1887,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>98</v>
       </c>
@@ -1817,14 +1908,14 @@
       <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.26953125" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>63</v>
       </c>
@@ -1838,7 +1929,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>54</v>
       </c>
@@ -1852,7 +1943,7 @@
         <v>2675408.4810000001</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -1866,7 +1957,7 @@
         <v>1625421.122</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -1880,7 +1971,7 @@
         <v>2819719.7179999999</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>42</v>
       </c>
@@ -1894,7 +1985,7 @@
         <v>2576687.5819999999</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>46</v>
       </c>
@@ -1908,7 +1999,7 @@
         <v>3660210.128</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -1922,7 +2013,7 @@
         <v>2137233.2710000002</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -1936,7 +2027,7 @@
         <v>3478720.3960000002</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>60</v>
       </c>
@@ -1950,7 +2041,7 @@
         <v>4057289.39</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>34</v>
       </c>
@@ -1964,7 +2055,7 @@
         <v>5035429.9689999996</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -1978,7 +2069,7 @@
         <v>3150624.395</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>50</v>
       </c>
@@ -1992,7 +2083,7 @@
         <v>3607941.4730000002</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -2006,7 +2097,7 @@
         <v>4527052.1179999998</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -2020,7 +2111,7 @@
         <v>1609838.871</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>58</v>
       </c>
@@ -2034,7 +2125,7 @@
         <v>10075179</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>44</v>
       </c>
@@ -2048,7 +2139,7 @@
         <v>10428891.060000001</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>40</v>
       </c>
@@ -2062,7 +2153,7 @@
         <v>14779080.73</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>52</v>
       </c>
@@ -2076,7 +2167,7 @@
         <v>7336519.3689999999</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>32</v>
       </c>
@@ -2090,7 +2181,7 @@
         <v>18710988.010000002</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>36</v>
       </c>
@@ -2104,7 +2195,7 @@
         <v>20152081.27</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>26</v>
       </c>
@@ -2118,7 +2209,7 @@
         <v>18262208.25</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>17</v>
       </c>
@@ -2132,7 +2223,7 @@
         <v>17934581.789999999</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>10</v>
       </c>
@@ -2146,7 +2237,7 @@
         <v>50051478.759999998</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>90</v>
       </c>
@@ -2160,7 +2251,7 @@
         <v>32039217.879999999</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>92</v>
       </c>
@@ -2174,7 +2265,7 @@
         <v>38050077.590000004</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>56</v>
       </c>
@@ -2188,7 +2279,7 @@
         <v>57375195.619999997</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>48</v>
       </c>
@@ -2202,7 +2293,7 @@
         <v>145300487.90000001</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>96</v>
       </c>
@@ -2216,7 +2307,7 @@
         <v>266505068.69999999</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>13</v>
       </c>

</xml_diff>

<commit_message>
Pull aquatic biology static results from lookup table
</commit_message>
<xml_diff>
--- a/data/lookup_tables.xlsx
+++ b/data/lookup_tables.xlsx
@@ -1,25 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\srucker\Documents\GitHub\SCI\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://limnotech-my.sharepoint.com/personal/srucker_limno_com/Documents/Documents/GitHub/SCI/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DC42158-8692-438B-A345-A6CC6108B823}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="64" documentId="13_ncr:1_{113EE769-9AD3-4243-97B3-520451D281E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DB808233-E373-48D7-BBFF-5921BB008E34}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-345" windowWidth="29040" windowHeight="15840" xr2:uid="{FC8AAFAA-1B2E-4A6F-8639-F15C3BC242A6}"/>
+    <workbookView xWindow="28680" yWindow="-12225" windowWidth="25440" windowHeight="15390" firstSheet="3" activeTab="6" xr2:uid="{FC8AAFAA-1B2E-4A6F-8639-F15C3BC242A6}"/>
   </bookViews>
   <sheets>
     <sheet name="location" sheetId="7" r:id="rId1"/>
     <sheet name="dumpsite_score" sheetId="1" r:id="rId2"/>
     <sheet name="dumpsite_weight" sheetId="2" r:id="rId3"/>
     <sheet name="trash_score" sheetId="3" r:id="rId4"/>
-    <sheet name="connectivity_score" sheetId="4" r:id="rId5"/>
-    <sheet name="eia_location_id" sheetId="5" r:id="rId6"/>
-    <sheet name="eia_area" sheetId="6" r:id="rId7"/>
+    <sheet name="connectivity_summary" sheetId="4" r:id="rId5"/>
+    <sheet name="fish_summary" sheetId="8" r:id="rId6"/>
+    <sheet name="habitat_summary" sheetId="11" r:id="rId7"/>
+    <sheet name="macroinvertebrate_summary" sheetId="12" r:id="rId8"/>
+    <sheet name="eia_location_id" sheetId="5" r:id="rId9"/>
+    <sheet name="eia_area" sheetId="6" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="114">
   <si>
     <t>max_sites_per_mile</t>
   </si>
@@ -353,19 +356,37 @@
     <t>acres</t>
   </si>
   <si>
+    <t>location_name</t>
+  </si>
+  <si>
+    <t>Piedmont</t>
+  </si>
+  <si>
+    <t>Coastal Plain</t>
+  </si>
+  <si>
+    <t>ecoregion</t>
+  </si>
+  <si>
+    <t>Rock Creek</t>
+  </si>
+  <si>
+    <t>Watts Branch</t>
+  </si>
+  <si>
     <t>Watts Branch - Upper</t>
   </si>
   <si>
-    <t>location_name</t>
-  </si>
-  <si>
-    <t>Piedmont</t>
-  </si>
-  <si>
-    <t>Coastal Plain</t>
-  </si>
-  <si>
-    <t>ecoregion</t>
+    <t>no fish</t>
+  </si>
+  <si>
+    <t>fish_ibi_data</t>
+  </si>
+  <si>
+    <t>habitat_phi_data</t>
+  </si>
+  <si>
+    <t>macroinvertebrate_hbi_data</t>
   </si>
 </sst>
 </file>
@@ -717,31 +738,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8059EA70-FEB1-4761-8449-3A8139D2BAE4}">
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>63</v>
       </c>
       <c r="B1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+      <c r="D1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -749,10 +774,13 @@
         <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+      <c r="D2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -760,10 +788,13 @@
         <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+      <c r="D3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -771,10 +802,13 @@
         <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -782,10 +816,13 @@
         <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -793,10 +830,13 @@
         <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="D6" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -804,10 +844,13 @@
         <v>21</v>
       </c>
       <c r="C7" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="D7" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -815,10 +858,13 @@
         <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="D8" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -826,10 +872,13 @@
         <v>25</v>
       </c>
       <c r="C9" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="D9" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -837,10 +886,13 @@
         <v>27</v>
       </c>
       <c r="C10" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="D10" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -848,10 +900,13 @@
         <v>29</v>
       </c>
       <c r="C11" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="D11" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>32</v>
       </c>
@@ -859,10 +914,13 @@
         <v>31</v>
       </c>
       <c r="C12" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="D12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>34</v>
       </c>
@@ -870,10 +928,13 @@
         <v>33</v>
       </c>
       <c r="C13" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="D13" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>36</v>
       </c>
@@ -881,10 +942,13 @@
         <v>35</v>
       </c>
       <c r="C14" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="D14" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>38</v>
       </c>
@@ -892,18 +956,24 @@
         <v>37</v>
       </c>
       <c r="C15" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+      <c r="D15" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>40</v>
       </c>
       <c r="B16" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>42</v>
       </c>
@@ -911,10 +981,13 @@
         <v>41</v>
       </c>
       <c r="C17" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+      <c r="D17" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>44</v>
       </c>
@@ -922,10 +995,13 @@
         <v>43</v>
       </c>
       <c r="C18" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+      <c r="D18" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>46</v>
       </c>
@@ -933,10 +1009,13 @@
         <v>45</v>
       </c>
       <c r="C19" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="D19" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>48</v>
       </c>
@@ -944,10 +1023,13 @@
         <v>47</v>
       </c>
       <c r="C20" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+      <c r="D20" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>50</v>
       </c>
@@ -955,10 +1037,13 @@
         <v>49</v>
       </c>
       <c r="C21" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="D21" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>52</v>
       </c>
@@ -966,10 +1051,13 @@
         <v>51</v>
       </c>
       <c r="C22" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+      <c r="D22" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>54</v>
       </c>
@@ -977,10 +1065,13 @@
         <v>53</v>
       </c>
       <c r="C23" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+      <c r="D23" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>56</v>
       </c>
@@ -988,10 +1079,13 @@
         <v>55</v>
       </c>
       <c r="C24" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="D24" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>58</v>
       </c>
@@ -999,10 +1093,13 @@
         <v>57</v>
       </c>
       <c r="C25" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+      <c r="D25" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>60</v>
       </c>
@@ -1010,10 +1107,13 @@
         <v>59</v>
       </c>
       <c r="C26" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+      <c r="D26" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>62</v>
       </c>
@@ -1021,18 +1121,464 @@
         <v>61</v>
       </c>
       <c r="C27" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+      <c r="D27" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>92</v>
       </c>
       <c r="B28" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="C28" t="s">
-        <v>106</v>
+        <v>108</v>
+      </c>
+      <c r="D28" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>90</v>
+      </c>
+      <c r="B29" t="s">
+        <v>109</v>
+      </c>
+      <c r="C29" t="s">
+        <v>108</v>
+      </c>
+      <c r="D29" t="s">
+        <v>105</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74512946-BFD5-4355-975E-7040C988669E}">
+  <dimension ref="A1:D29"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2">
+        <v>71.444418330000005</v>
+      </c>
+      <c r="C2">
+        <v>5906012.3820000002</v>
+      </c>
+      <c r="D2">
+        <v>2675408.4810000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3">
+        <v>136.07334739999999</v>
+      </c>
+      <c r="C3">
+        <v>5927331.3049999997</v>
+      </c>
+      <c r="D3">
+        <v>1625421.122</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4">
+        <v>171.85245789999999</v>
+      </c>
+      <c r="C4">
+        <v>7485863.1229999997</v>
+      </c>
+      <c r="D4">
+        <v>2819719.7179999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5">
+        <v>174.32630649999999</v>
+      </c>
+      <c r="C5">
+        <v>7593623.5350000001</v>
+      </c>
+      <c r="D5">
+        <v>2576687.5819999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6">
+        <v>217.7788955</v>
+      </c>
+      <c r="C6">
+        <v>9486410.7420000006</v>
+      </c>
+      <c r="D6">
+        <v>3660210.128</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7">
+        <v>231.58095510000001</v>
+      </c>
+      <c r="C7">
+        <v>10087626.050000001</v>
+      </c>
+      <c r="D7">
+        <v>2137233.2710000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8">
+        <v>234.09865740000001</v>
+      </c>
+      <c r="C8">
+        <v>10197296.73</v>
+      </c>
+      <c r="D8">
+        <v>3478720.3960000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9">
+        <v>249.2998709</v>
+      </c>
+      <c r="C9">
+        <v>10859458.939999999</v>
+      </c>
+      <c r="D9">
+        <v>4057289.39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10">
+        <v>276.8609783</v>
+      </c>
+      <c r="C10">
+        <v>12060015.970000001</v>
+      </c>
+      <c r="D10">
+        <v>5035429.9689999996</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11">
+        <v>270.26444609999999</v>
+      </c>
+      <c r="C11">
+        <v>12104505.98</v>
+      </c>
+      <c r="D11">
+        <v>3150624.395</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12">
+        <v>280.45176459999999</v>
+      </c>
+      <c r="C12">
+        <v>12216430</v>
+      </c>
+      <c r="D12">
+        <v>3607941.4730000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13">
+        <v>291.45618960000002</v>
+      </c>
+      <c r="C13">
+        <v>12695780.83</v>
+      </c>
+      <c r="D13">
+        <v>4527052.1179999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14">
+        <v>409.25697700000001</v>
+      </c>
+      <c r="C14">
+        <v>17827162.609999999</v>
+      </c>
+      <c r="D14">
+        <v>1609838.871</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>58</v>
+      </c>
+      <c r="B15">
+        <v>516.37507649999998</v>
+      </c>
+      <c r="C15">
+        <v>22493208.359999999</v>
+      </c>
+      <c r="D15">
+        <v>10075179</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16">
+        <v>472.15890439999998</v>
+      </c>
+      <c r="C16">
+        <v>28262408.210000001</v>
+      </c>
+      <c r="D16">
+        <v>10428891.060000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17">
+        <v>643.53066860000001</v>
+      </c>
+      <c r="C17">
+        <v>28811482.870000001</v>
+      </c>
+      <c r="D17">
+        <v>14779080.73</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18">
+        <v>449.3504049</v>
+      </c>
+      <c r="C18">
+        <v>28934650.41</v>
+      </c>
+      <c r="D18">
+        <v>7336519.3689999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19">
+        <v>220.8060729</v>
+      </c>
+      <c r="C19">
+        <v>41747880.719999999</v>
+      </c>
+      <c r="D19">
+        <v>18710988.010000002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20">
+        <v>1103.8468869999999</v>
+      </c>
+      <c r="C20">
+        <v>48083378.079999998</v>
+      </c>
+      <c r="D20">
+        <v>20152081.27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21">
+        <v>1134.548792</v>
+      </c>
+      <c r="C21">
+        <v>49420747.68</v>
+      </c>
+      <c r="D21">
+        <v>18262208.25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22">
+        <v>1148.451286</v>
+      </c>
+      <c r="C22">
+        <v>51304948.560000002</v>
+      </c>
+      <c r="D22">
+        <v>17934581.789999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23">
+        <v>1603.223352</v>
+      </c>
+      <c r="C23">
+        <v>69836129.849999994</v>
+      </c>
+      <c r="D23">
+        <v>50051478.759999998</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>90</v>
+      </c>
+      <c r="B24">
+        <v>848.33045019999997</v>
+      </c>
+      <c r="C24">
+        <v>90723670.299999997</v>
+      </c>
+      <c r="D24">
+        <v>32039217.879999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>92</v>
+      </c>
+      <c r="B25">
+        <v>410.63448010000002</v>
+      </c>
+      <c r="C25">
+        <v>108610836.7</v>
+      </c>
+      <c r="D25">
+        <v>38050077.590000004</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>56</v>
+      </c>
+      <c r="B26">
+        <v>158.9618614</v>
+      </c>
+      <c r="C26">
+        <v>109878251</v>
+      </c>
+      <c r="D26">
+        <v>57375195.619999997</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>48</v>
+      </c>
+      <c r="B27">
+        <v>2171.0271550000002</v>
+      </c>
+      <c r="C27">
+        <v>414641447.69999999</v>
+      </c>
+      <c r="D27">
+        <v>145300487.90000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>96</v>
+      </c>
+      <c r="B28">
+        <v>1335.459206</v>
+      </c>
+      <c r="C28">
+        <v>797091117.29999995</v>
+      </c>
+      <c r="D28">
+        <v>266505068.69999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>13</v>
+      </c>
+      <c r="B29">
+        <v>925.03015310000001</v>
+      </c>
+      <c r="C29">
+        <v>1033762101</v>
+      </c>
+      <c r="D29">
+        <v>393938764.89999998</v>
       </c>
     </row>
   </sheetData>
@@ -1048,12 +1594,12 @@
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1061,7 +1607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>10</v>
       </c>
@@ -1069,7 +1615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>9</v>
       </c>
@@ -1077,7 +1623,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>8</v>
       </c>
@@ -1085,7 +1631,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>7</v>
       </c>
@@ -1093,7 +1639,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>6</v>
       </c>
@@ -1101,7 +1647,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1109,7 +1655,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>4</v>
       </c>
@@ -1117,7 +1663,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>3</v>
       </c>
@@ -1125,7 +1671,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2</v>
       </c>
@@ -1133,7 +1679,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1</v>
       </c>
@@ -1148,12 +1694,12 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>66</v>
       </c>
@@ -1161,7 +1707,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1169,7 +1715,7 @@
         <v>-3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1177,7 +1723,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1185,7 +1731,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>67</v>
       </c>
@@ -1206,9 +1752,9 @@
       <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -1216,7 +1762,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1224,7 +1770,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1232,7 +1778,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1240,7 +1786,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1255,18 +1801,20 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B281CBBA-5423-42AE-9693-0C69866CF5CE}">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>64</v>
       </c>
@@ -1280,12 +1828,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>107</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s">
         <v>11</v>
@@ -1294,12 +1842,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
         <v>11</v>
@@ -1308,12 +1856,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
         <v>11</v>
@@ -1322,54 +1870,54 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" t="s">
         <v>11</v>
       </c>
-      <c r="D5">
+      <c r="D6">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" t="s">
         <v>20</v>
       </c>
-      <c r="D6">
+      <c r="D7">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C8" t="s">
         <v>20</v>
@@ -1378,12 +1926,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C9" t="s">
         <v>20</v>
@@ -1392,12 +1940,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C10" t="s">
         <v>20</v>
@@ -1406,54 +1954,54 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" t="s">
         <v>20</v>
       </c>
-      <c r="D11">
+      <c r="D12">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12" t="s">
-        <v>32</v>
-      </c>
-      <c r="C12" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" t="s">
         <v>11</v>
       </c>
-      <c r="D12">
+      <c r="D13">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>33</v>
-      </c>
-      <c r="B13" t="s">
-        <v>34</v>
-      </c>
-      <c r="C13" t="s">
-        <v>20</v>
-      </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B14" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C14" t="s">
         <v>11</v>
@@ -1462,12 +2010,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B15" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C15" t="s">
         <v>11</v>
@@ -1476,12 +2024,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B16" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C16" t="s">
         <v>11</v>
@@ -1490,12 +2038,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B17" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C17" t="s">
         <v>11</v>
@@ -1504,12 +2052,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B18" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C18" t="s">
         <v>11</v>
@@ -1518,12 +2066,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B19" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C19" t="s">
         <v>11</v>
@@ -1532,40 +2080,40 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B20" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C20" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>51</v>
+      </c>
+      <c r="B21" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21" t="s">
         <v>11</v>
       </c>
-      <c r="D20">
+      <c r="D21">
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>49</v>
-      </c>
-      <c r="B21" t="s">
-        <v>50</v>
-      </c>
-      <c r="C21" t="s">
-        <v>20</v>
-      </c>
-      <c r="D21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B22" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C22" t="s">
         <v>11</v>
@@ -1574,12 +2122,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B23" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C23" t="s">
         <v>11</v>
@@ -1588,12 +2136,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B24" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C24" t="s">
         <v>11</v>
@@ -1602,45 +2150,31 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B25" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C25" t="s">
+        <v>20</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>108</v>
+      </c>
+      <c r="B26" t="s">
+        <v>62</v>
+      </c>
+      <c r="C26" t="s">
         <v>11</v>
       </c>
-      <c r="D25">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>59</v>
-      </c>
-      <c r="B26" t="s">
-        <v>60</v>
-      </c>
-      <c r="C26" t="s">
-        <v>20</v>
-      </c>
       <c r="D26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>61</v>
-      </c>
-      <c r="B27" t="s">
-        <v>62</v>
-      </c>
-      <c r="C27" t="s">
-        <v>11</v>
-      </c>
-      <c r="D27">
         <v>10</v>
       </c>
     </row>
@@ -1650,6 +2184,1154 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AE2FD76-BC91-45B2-B5B8-525E322D787E}">
+  <dimension ref="A1:D26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="25.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2">
+        <v>2.64</v>
+      </c>
+      <c r="D2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3">
+        <v>1.8</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5">
+        <v>1.4</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6">
+        <v>1.8</v>
+      </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7">
+        <v>1.67</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" t="s">
+        <v>110</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" t="s">
+        <v>110</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" t="s">
+        <v>110</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" t="s">
+        <v>110</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13">
+        <v>3.3</v>
+      </c>
+      <c r="D13">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17">
+        <v>3</v>
+      </c>
+      <c r="D17">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18">
+        <v>1.8</v>
+      </c>
+      <c r="D18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>49</v>
+      </c>
+      <c r="B20" t="s">
+        <v>50</v>
+      </c>
+      <c r="C20">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="D20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>51</v>
+      </c>
+      <c r="B21" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21">
+        <v>1.4</v>
+      </c>
+      <c r="D21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22" t="s">
+        <v>54</v>
+      </c>
+      <c r="C22" t="s">
+        <v>110</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>55</v>
+      </c>
+      <c r="B23" t="s">
+        <v>56</v>
+      </c>
+      <c r="C23">
+        <v>1.67</v>
+      </c>
+      <c r="D23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>57</v>
+      </c>
+      <c r="B24" t="s">
+        <v>58</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>59</v>
+      </c>
+      <c r="B25" t="s">
+        <v>60</v>
+      </c>
+      <c r="C25" t="s">
+        <v>110</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>108</v>
+      </c>
+      <c r="B26" t="s">
+        <v>62</v>
+      </c>
+      <c r="C26">
+        <v>2.17</v>
+      </c>
+      <c r="D26">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B442153-1068-48BB-9E2A-4ABB5CD9BD58}">
+  <dimension ref="A1:D26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="25.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2">
+        <v>62.85</v>
+      </c>
+      <c r="D2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3">
+        <v>64.180000000000007</v>
+      </c>
+      <c r="D3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4">
+        <v>57.73</v>
+      </c>
+      <c r="D4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5">
+        <v>55.18</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6">
+        <v>66.290000000000006</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7">
+        <v>57.56</v>
+      </c>
+      <c r="D7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8">
+        <v>61.44</v>
+      </c>
+      <c r="D8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9">
+        <v>62.52</v>
+      </c>
+      <c r="D9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10">
+        <v>65.59</v>
+      </c>
+      <c r="D10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11">
+        <v>53.18</v>
+      </c>
+      <c r="D11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12">
+        <v>55.02</v>
+      </c>
+      <c r="D12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13">
+        <v>47.94</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14">
+        <v>55.46</v>
+      </c>
+      <c r="D14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15">
+        <v>55.1</v>
+      </c>
+      <c r="D15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16">
+        <v>78.7</v>
+      </c>
+      <c r="D16">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17">
+        <v>66.36</v>
+      </c>
+      <c r="D17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18">
+        <v>54.84</v>
+      </c>
+      <c r="D18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19">
+        <v>62.97</v>
+      </c>
+      <c r="D19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>49</v>
+      </c>
+      <c r="B20" t="s">
+        <v>50</v>
+      </c>
+      <c r="C20">
+        <v>73.84</v>
+      </c>
+      <c r="D20">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>51</v>
+      </c>
+      <c r="B21" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21">
+        <v>60.77</v>
+      </c>
+      <c r="D21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22" t="s">
+        <v>54</v>
+      </c>
+      <c r="C22">
+        <v>55.67</v>
+      </c>
+      <c r="D22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>55</v>
+      </c>
+      <c r="B23" t="s">
+        <v>56</v>
+      </c>
+      <c r="C23">
+        <v>47.4</v>
+      </c>
+      <c r="D23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>57</v>
+      </c>
+      <c r="B24" t="s">
+        <v>58</v>
+      </c>
+      <c r="C24">
+        <v>56.63</v>
+      </c>
+      <c r="D24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>59</v>
+      </c>
+      <c r="B25" t="s">
+        <v>60</v>
+      </c>
+      <c r="C25">
+        <v>65.17</v>
+      </c>
+      <c r="D25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>108</v>
+      </c>
+      <c r="B26" t="s">
+        <v>62</v>
+      </c>
+      <c r="C26">
+        <v>54.15</v>
+      </c>
+      <c r="D26">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{200F6E0C-51C0-4CFC-8295-6BC9A0CB5165}">
+  <dimension ref="A1:D26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="25.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2">
+        <v>6.86</v>
+      </c>
+      <c r="D2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3">
+        <v>5.28</v>
+      </c>
+      <c r="D3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4">
+        <v>6.41</v>
+      </c>
+      <c r="D4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5">
+        <v>5.88</v>
+      </c>
+      <c r="D5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7">
+        <v>6.24</v>
+      </c>
+      <c r="D7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9">
+        <v>9.14</v>
+      </c>
+      <c r="D9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10">
+        <v>7.39</v>
+      </c>
+      <c r="D10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11">
+        <v>6.28</v>
+      </c>
+      <c r="D11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12">
+        <v>5.39</v>
+      </c>
+      <c r="D12">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13">
+        <v>7.9</v>
+      </c>
+      <c r="D13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14">
+        <v>5.99</v>
+      </c>
+      <c r="D14">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15">
+        <v>6.49</v>
+      </c>
+      <c r="D15">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16">
+        <v>5.32</v>
+      </c>
+      <c r="D16">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17">
+        <v>8.06</v>
+      </c>
+      <c r="D17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18">
+        <v>5.88</v>
+      </c>
+      <c r="D18">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19">
+        <v>7.67</v>
+      </c>
+      <c r="D19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>49</v>
+      </c>
+      <c r="B20" t="s">
+        <v>50</v>
+      </c>
+      <c r="C20">
+        <v>4.45</v>
+      </c>
+      <c r="D20">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>51</v>
+      </c>
+      <c r="B21" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21">
+        <v>6.82</v>
+      </c>
+      <c r="D21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22" t="s">
+        <v>54</v>
+      </c>
+      <c r="C22">
+        <v>5.93</v>
+      </c>
+      <c r="D22">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>55</v>
+      </c>
+      <c r="B23" t="s">
+        <v>56</v>
+      </c>
+      <c r="C23">
+        <v>7.6</v>
+      </c>
+      <c r="D23">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>57</v>
+      </c>
+      <c r="B24" t="s">
+        <v>58</v>
+      </c>
+      <c r="C24">
+        <v>6.22</v>
+      </c>
+      <c r="D24">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>59</v>
+      </c>
+      <c r="B25" t="s">
+        <v>60</v>
+      </c>
+      <c r="C25">
+        <v>9.3800000000000008</v>
+      </c>
+      <c r="D25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>108</v>
+      </c>
+      <c r="B26" t="s">
+        <v>62</v>
+      </c>
+      <c r="C26">
+        <v>6.46</v>
+      </c>
+      <c r="D26">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50FDDFB2-57CD-4186-8745-C34C09AB75A5}">
   <dimension ref="A1:B29"/>
   <sheetViews>
@@ -1657,13 +3339,13 @@
       <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="48.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="48.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>99</v>
       </c>
@@ -1671,7 +3353,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>68</v>
       </c>
@@ -1679,7 +3361,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>69</v>
       </c>
@@ -1687,7 +3369,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>70</v>
       </c>
@@ -1695,7 +3377,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>71</v>
       </c>
@@ -1703,7 +3385,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>72</v>
       </c>
@@ -1711,7 +3393,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>73</v>
       </c>
@@ -1719,7 +3401,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>74</v>
       </c>
@@ -1727,7 +3409,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>75</v>
       </c>
@@ -1735,7 +3417,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>76</v>
       </c>
@@ -1743,7 +3425,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>77</v>
       </c>
@@ -1751,7 +3433,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>78</v>
       </c>
@@ -1759,7 +3441,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>79</v>
       </c>
@@ -1767,7 +3449,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>80</v>
       </c>
@@ -1775,7 +3457,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>81</v>
       </c>
@@ -1783,7 +3465,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>82</v>
       </c>
@@ -1791,7 +3473,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>83</v>
       </c>
@@ -1799,7 +3481,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>84</v>
       </c>
@@ -1807,7 +3489,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>85</v>
       </c>
@@ -1815,7 +3497,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>86</v>
       </c>
@@ -1823,7 +3505,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>87</v>
       </c>
@@ -1831,7 +3513,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>88</v>
       </c>
@@ -1839,7 +3521,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>89</v>
       </c>
@@ -1847,7 +3529,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>91</v>
       </c>
@@ -1855,7 +3537,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>93</v>
       </c>
@@ -1863,7 +3545,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>94</v>
       </c>
@@ -1871,7 +3553,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>95</v>
       </c>
@@ -1879,7 +3561,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>97</v>
       </c>
@@ -1887,438 +3569,12 @@
         <v>96</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>98</v>
       </c>
       <c r="B29" t="s">
         <v>13</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74512946-BFD5-4355-975E-7040C988669E}">
-  <dimension ref="A1:D29"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B2">
-        <v>71.444418330000005</v>
-      </c>
-      <c r="C2">
-        <v>5906012.3820000002</v>
-      </c>
-      <c r="D2">
-        <v>2675408.4810000001</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3">
-        <v>136.07334739999999</v>
-      </c>
-      <c r="C3">
-        <v>5927331.3049999997</v>
-      </c>
-      <c r="D3">
-        <v>1625421.122</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B4">
-        <v>171.85245789999999</v>
-      </c>
-      <c r="C4">
-        <v>7485863.1229999997</v>
-      </c>
-      <c r="D4">
-        <v>2819719.7179999999</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>42</v>
-      </c>
-      <c r="B5">
-        <v>174.32630649999999</v>
-      </c>
-      <c r="C5">
-        <v>7593623.5350000001</v>
-      </c>
-      <c r="D5">
-        <v>2576687.5819999999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>46</v>
-      </c>
-      <c r="B6">
-        <v>217.7788955</v>
-      </c>
-      <c r="C6">
-        <v>9486410.7420000006</v>
-      </c>
-      <c r="D6">
-        <v>3660210.128</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7">
-        <v>231.58095510000001</v>
-      </c>
-      <c r="C7">
-        <v>10087626.050000001</v>
-      </c>
-      <c r="D7">
-        <v>2137233.2710000002</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>30</v>
-      </c>
-      <c r="B8">
-        <v>234.09865740000001</v>
-      </c>
-      <c r="C8">
-        <v>10197296.73</v>
-      </c>
-      <c r="D8">
-        <v>3478720.3960000002</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>60</v>
-      </c>
-      <c r="B9">
-        <v>249.2998709</v>
-      </c>
-      <c r="C9">
-        <v>10859458.939999999</v>
-      </c>
-      <c r="D9">
-        <v>4057289.39</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>34</v>
-      </c>
-      <c r="B10">
-        <v>276.8609783</v>
-      </c>
-      <c r="C10">
-        <v>12060015.970000001</v>
-      </c>
-      <c r="D10">
-        <v>5035429.9689999996</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11">
-        <v>270.26444609999999</v>
-      </c>
-      <c r="C11">
-        <v>12104505.98</v>
-      </c>
-      <c r="D11">
-        <v>3150624.395</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>50</v>
-      </c>
-      <c r="B12">
-        <v>280.45176459999999</v>
-      </c>
-      <c r="C12">
-        <v>12216430</v>
-      </c>
-      <c r="D12">
-        <v>3607941.4730000002</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>28</v>
-      </c>
-      <c r="B13">
-        <v>291.45618960000002</v>
-      </c>
-      <c r="C13">
-        <v>12695780.83</v>
-      </c>
-      <c r="D13">
-        <v>4527052.1179999998</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14">
-        <v>409.25697700000001</v>
-      </c>
-      <c r="C14">
-        <v>17827162.609999999</v>
-      </c>
-      <c r="D14">
-        <v>1609838.871</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>58</v>
-      </c>
-      <c r="B15">
-        <v>516.37507649999998</v>
-      </c>
-      <c r="C15">
-        <v>22493208.359999999</v>
-      </c>
-      <c r="D15">
-        <v>10075179</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>44</v>
-      </c>
-      <c r="B16">
-        <v>472.15890439999998</v>
-      </c>
-      <c r="C16">
-        <v>28262408.210000001</v>
-      </c>
-      <c r="D16">
-        <v>10428891.060000001</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>40</v>
-      </c>
-      <c r="B17">
-        <v>643.53066860000001</v>
-      </c>
-      <c r="C17">
-        <v>28811482.870000001</v>
-      </c>
-      <c r="D17">
-        <v>14779080.73</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>52</v>
-      </c>
-      <c r="B18">
-        <v>449.3504049</v>
-      </c>
-      <c r="C18">
-        <v>28934650.41</v>
-      </c>
-      <c r="D18">
-        <v>7336519.3689999999</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>32</v>
-      </c>
-      <c r="B19">
-        <v>220.8060729</v>
-      </c>
-      <c r="C19">
-        <v>41747880.719999999</v>
-      </c>
-      <c r="D19">
-        <v>18710988.010000002</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>36</v>
-      </c>
-      <c r="B20">
-        <v>1103.8468869999999</v>
-      </c>
-      <c r="C20">
-        <v>48083378.079999998</v>
-      </c>
-      <c r="D20">
-        <v>20152081.27</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>26</v>
-      </c>
-      <c r="B21">
-        <v>1134.548792</v>
-      </c>
-      <c r="C21">
-        <v>49420747.68</v>
-      </c>
-      <c r="D21">
-        <v>18262208.25</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>17</v>
-      </c>
-      <c r="B22">
-        <v>1148.451286</v>
-      </c>
-      <c r="C22">
-        <v>51304948.560000002</v>
-      </c>
-      <c r="D22">
-        <v>17934581.789999999</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>10</v>
-      </c>
-      <c r="B23">
-        <v>1603.223352</v>
-      </c>
-      <c r="C23">
-        <v>69836129.849999994</v>
-      </c>
-      <c r="D23">
-        <v>50051478.759999998</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>90</v>
-      </c>
-      <c r="B24">
-        <v>848.33045019999997</v>
-      </c>
-      <c r="C24">
-        <v>90723670.299999997</v>
-      </c>
-      <c r="D24">
-        <v>32039217.879999999</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>92</v>
-      </c>
-      <c r="B25">
-        <v>410.63448010000002</v>
-      </c>
-      <c r="C25">
-        <v>108610836.7</v>
-      </c>
-      <c r="D25">
-        <v>38050077.590000004</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>56</v>
-      </c>
-      <c r="B26">
-        <v>158.9618614</v>
-      </c>
-      <c r="C26">
-        <v>109878251</v>
-      </c>
-      <c r="D26">
-        <v>57375195.619999997</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>48</v>
-      </c>
-      <c r="B27">
-        <v>2171.0271550000002</v>
-      </c>
-      <c r="C27">
-        <v>414641447.69999999</v>
-      </c>
-      <c r="D27">
-        <v>145300487.90000001</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>96</v>
-      </c>
-      <c r="B28">
-        <v>1335.459206</v>
-      </c>
-      <c r="C28">
-        <v>797091117.29999995</v>
-      </c>
-      <c r="D28">
-        <v>266505068.69999999</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>13</v>
-      </c>
-      <c r="B29">
-        <v>925.03015310000001</v>
-      </c>
-      <c r="C29">
-        <v>1033762101</v>
-      </c>
-      <c r="D29">
-        <v>393938764.89999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Calculate EIA impervious treated area
May need to do GIS intersection with impervious layer and subshed layer to confirm correct numbers. Should all layers be referencing the DC open data subshed layer instead of the typical LTI subshed layer?
</commit_message>
<xml_diff>
--- a/data/lookup_tables.xlsx
+++ b/data/lookup_tables.xlsx
@@ -8,9 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://limnotech-my.sharepoint.com/personal/srucker_limno_com/Documents/Documents/GitHub/SCI/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="79" documentId="13_ncr:1_{113EE769-9AD3-4243-97B3-520451D281E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{77183DE4-219A-4F73-9DD6-E01075055CA8}"/>
+  <xr:revisionPtr revIDLastSave="160" documentId="13_ncr:1_{113EE769-9AD3-4243-97B3-520451D281E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7A3FEAB9-E603-446E-A223-07385343E2BF}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" firstSheet="5" activeTab="8" xr2:uid="{FC8AAFAA-1B2E-4A6F-8639-F15C3BC242A6}"/>
+    <workbookView xWindow="28680" yWindow="-345" windowWidth="29040" windowHeight="15840" tabRatio="721" firstSheet="4" activeTab="9" xr2:uid="{FC8AAFAA-1B2E-4A6F-8639-F15C3BC242A6}"/>
+    <workbookView xWindow="28680" yWindow="-345" windowWidth="29040" windowHeight="15840" firstSheet="5" activeTab="9" xr2:uid="{23697FDE-567D-4570-AE33-F8F65584BB36}"/>
   </bookViews>
   <sheets>
     <sheet name="location" sheetId="7" r:id="rId1"/>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="116">
   <si>
     <t>max_sites_per_mile</t>
   </si>
@@ -384,6 +385,15 @@
   </si>
   <si>
     <t>Potomac Lower - MS4 - Oxon Run</t>
+  </si>
+  <si>
+    <t>mainstem_lookup</t>
+  </si>
+  <si>
+    <t>subshed_lookup</t>
+  </si>
+  <si>
+    <t>watts_lookup</t>
   </si>
 </sst>
 </file>
@@ -737,9 +747,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8059EA70-FEB1-4761-8449-3A8139D2BAE4}">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1161,9 +1172,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74512946-BFD5-4355-975E-7040C988669E}">
   <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T9" sqref="T9"/>
     </sheetView>
+    <sheetView tabSelected="1" workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1501,6 +1513,7 @@
     <sheetView workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1604,6 +1617,7 @@
     <sheetView workbookViewId="0">
       <selection activeCell="G32" sqref="G32"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -1659,6 +1673,7 @@
     <sheetView workbookViewId="0">
       <selection activeCell="L27" sqref="L27"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -1714,6 +1729,7 @@
     <sheetView workbookViewId="0">
       <selection activeCell="E31" sqref="E31"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2098,6 +2114,7 @@
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2483,6 +2500,7 @@
     <sheetView workbookViewId="0">
       <selection activeCell="F30" sqref="F30"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2867,6 +2885,7 @@
     <sheetView workbookViewId="0">
       <selection activeCell="F28" sqref="F28"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -3241,248 +3260,458 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50FDDFB2-57CD-4186-8745-C34C09AB75A5}">
-  <dimension ref="A1:B29"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q18" sqref="Q18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="53.6640625" customWidth="1"/>
     <col min="2" max="2" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.44140625" customWidth="1"/>
+    <col min="4" max="4" width="32" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="45.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="39.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>71</v>
       </c>
       <c r="B1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D1" t="s">
+        <v>113</v>
+      </c>
+      <c r="E1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>85</v>
       </c>
       <c r="B2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C2">
+        <f>COUNTIF(location!$A$2:$A$29,eia_location_id!B2)</f>
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>92</v>
       </c>
       <c r="B3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C3">
+        <f>COUNTIF(location!$A$2:$A$29,eia_location_id!B3)</f>
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>93</v>
       </c>
       <c r="B4" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C4">
+        <f>COUNTIF(location!$A$2:$A$29,eia_location_id!B4)</f>
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>94</v>
       </c>
       <c r="B5" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C5">
+        <f>COUNTIF(location!$A$2:$A$29,eia_location_id!B5)</f>
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>95</v>
       </c>
       <c r="B6" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C6">
+        <f>COUNTIF(location!$A$2:$A$29,eia_location_id!B6)</f>
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>99</v>
       </c>
       <c r="B7" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C7">
+        <f>COUNTIF(location!$A$2:$A$29,eia_location_id!B7)</f>
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>100</v>
       </c>
       <c r="B8" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C8">
+        <f>COUNTIF(location!$A$2:$A$29,eia_location_id!B8)</f>
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>101</v>
       </c>
       <c r="B9" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C9">
+        <f>COUNTIF(location!$A$2:$A$29,eia_location_id!B9)</f>
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>102</v>
       </c>
       <c r="B10" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C10">
+        <f>COUNTIF(location!$A$2:$A$29,eia_location_id!B10)</f>
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>103</v>
       </c>
       <c r="B11" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C11">
+        <f>COUNTIF(location!$A$2:$A$29,eia_location_id!B11)</f>
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>104</v>
       </c>
       <c r="B12" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C12">
+        <f>COUNTIF(location!$A$2:$A$29,eia_location_id!B12)</f>
+        <v>1</v>
+      </c>
+      <c r="E12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>105</v>
       </c>
       <c r="B13" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C13">
+        <f>COUNTIF(location!$A$2:$A$29,eia_location_id!B13)</f>
+        <v>1</v>
+      </c>
+      <c r="E13" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>106</v>
       </c>
       <c r="B14" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C14">
+        <f>COUNTIF(location!$A$2:$A$29,eia_location_id!B14)</f>
+        <v>1</v>
+      </c>
+      <c r="E14" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>86</v>
       </c>
       <c r="B15" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C15">
+        <f>COUNTIF(location!$A$2:$A$29,eia_location_id!B15)</f>
+        <v>1</v>
+      </c>
+      <c r="E15" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>107</v>
       </c>
       <c r="B16" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C16">
+        <f>COUNTIF(location!$A$2:$A$29,eia_location_id!B16)</f>
+        <v>1</v>
+      </c>
+      <c r="E16" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>87</v>
       </c>
       <c r="B17" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C17">
+        <f>COUNTIF(location!$A$2:$A$29,eia_location_id!B17)</f>
+        <v>1</v>
+      </c>
+      <c r="E17" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>88</v>
       </c>
       <c r="B18" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C18">
+        <f>COUNTIF(location!$A$2:$A$29,eia_location_id!B18)</f>
+        <v>1</v>
+      </c>
+      <c r="E18" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>89</v>
       </c>
       <c r="B19" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C19">
+        <f>COUNTIF(location!$A$2:$A$29,eia_location_id!B19)</f>
+        <v>1</v>
+      </c>
+      <c r="E19" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>108</v>
       </c>
       <c r="B20" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C20">
+        <f>COUNTIF(location!$A$2:$A$29,eia_location_id!B20)</f>
+        <v>1</v>
+      </c>
+      <c r="E20" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>109</v>
       </c>
       <c r="B21" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C21">
+        <f>COUNTIF(location!$A$2:$A$29,eia_location_id!B21)</f>
+        <v>1</v>
+      </c>
+      <c r="E21" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>90</v>
       </c>
       <c r="B22" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C22">
+        <f>COUNTIF(location!$A$2:$A$29,eia_location_id!B22)</f>
+        <v>1</v>
+      </c>
+      <c r="E22" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>96</v>
       </c>
       <c r="B23" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C23">
+        <f>COUNTIF(location!$A$2:$A$29,eia_location_id!B23)</f>
+        <v>1</v>
+      </c>
+      <c r="D23" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>110</v>
       </c>
       <c r="B24" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C24">
+        <f>COUNTIF(location!$A$2:$A$29,eia_location_id!B24)</f>
+        <v>1</v>
+      </c>
+      <c r="F24" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>111</v>
       </c>
       <c r="B25" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C25">
+        <f>COUNTIF(location!$A$2:$A$29,eia_location_id!B25)</f>
+        <v>1</v>
+      </c>
+      <c r="F25" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>97</v>
       </c>
       <c r="B26" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C26">
+        <f>COUNTIF(location!$A$2:$A$29,eia_location_id!B26)</f>
+        <v>1</v>
+      </c>
+      <c r="E26" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>112</v>
       </c>
       <c r="B27" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C27">
+        <f>COUNTIF(location!$A$2:$A$29,eia_location_id!B27)</f>
+        <v>1</v>
+      </c>
+      <c r="E27" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>91</v>
       </c>
       <c r="B28" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C28">
+        <f>COUNTIF(location!$A$2:$A$29,eia_location_id!B28)</f>
+        <v>0</v>
+      </c>
+      <c r="D28" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>98</v>
       </c>
       <c r="B29" t="s">
         <v>13</v>
+      </c>
+      <c r="C29">
+        <f>COUNTIF(location!$A$2:$A$29,eia_location_id!B29)</f>
+        <v>1</v>
+      </c>
+      <c r="D29" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add new lookup tables for EIA
See tabs: eia_subsheds and eia_rock_creek
</commit_message>
<xml_diff>
--- a/data/lookup_tables.xlsx
+++ b/data/lookup_tables.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://limnotech-my.sharepoint.com/personal/srucker_limno_com/Documents/Documents/GitHub/SCI/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="160" documentId="13_ncr:1_{113EE769-9AD3-4243-97B3-520451D281E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7A3FEAB9-E603-446E-A223-07385343E2BF}"/>
+  <xr:revisionPtr revIDLastSave="214" documentId="13_ncr:1_{113EE769-9AD3-4243-97B3-520451D281E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{80E80562-B639-4D4F-A9FE-A05305510E33}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-345" windowWidth="29040" windowHeight="15840" tabRatio="721" firstSheet="4" activeTab="9" xr2:uid="{FC8AAFAA-1B2E-4A6F-8639-F15C3BC242A6}"/>
-    <workbookView xWindow="28680" yWindow="-345" windowWidth="29040" windowHeight="15840" firstSheet="5" activeTab="9" xr2:uid="{23697FDE-567D-4570-AE33-F8F65584BB36}"/>
+    <workbookView xWindow="28680" yWindow="-12225" windowWidth="25440" windowHeight="15390" tabRatio="721" firstSheet="5" activeTab="10" xr2:uid="{FC8AAFAA-1B2E-4A6F-8639-F15C3BC242A6}"/>
+    <workbookView xWindow="28680" yWindow="-12225" windowWidth="25440" windowHeight="15390" firstSheet="5" activeTab="11" xr2:uid="{23697FDE-567D-4570-AE33-F8F65584BB36}"/>
   </bookViews>
   <sheets>
     <sheet name="location" sheetId="7" r:id="rId1"/>
@@ -23,7 +23,9 @@
     <sheet name="habitat_summary" sheetId="11" r:id="rId7"/>
     <sheet name="macroinvertebrate_summary" sheetId="12" r:id="rId8"/>
     <sheet name="eia_location_id" sheetId="5" r:id="rId9"/>
-    <sheet name="eia_area" sheetId="6" r:id="rId10"/>
+    <sheet name="eia_subsheds" sheetId="13" r:id="rId10"/>
+    <sheet name="eia_rock_creek" sheetId="14" r:id="rId11"/>
+    <sheet name="eia_area" sheetId="6" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -46,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="135">
   <si>
     <t>max_sites_per_mile</t>
   </si>
@@ -394,6 +396,63 @@
   </si>
   <si>
     <t>watts_lookup</t>
+  </si>
+  <si>
+    <t>WATERSHED</t>
+  </si>
+  <si>
+    <t>SUBSHED</t>
+  </si>
+  <si>
+    <t>SEWER_SYST</t>
+  </si>
+  <si>
+    <t>sci_watershed</t>
+  </si>
+  <si>
+    <t>Normanstone Creek</t>
+  </si>
+  <si>
+    <t>Watershed</t>
+  </si>
+  <si>
+    <t>Subshed</t>
+  </si>
+  <si>
+    <t>Sewer System</t>
+  </si>
+  <si>
+    <t>Potomac River</t>
+  </si>
+  <si>
+    <t>MS4</t>
+  </si>
+  <si>
+    <t>Anacostia River</t>
+  </si>
+  <si>
+    <t>CSS</t>
+  </si>
+  <si>
+    <t>Rock Creek / Piney Branch</t>
+  </si>
+  <si>
+    <t>Bingham Run</t>
+  </si>
+  <si>
+    <t>Milkhouse Run</t>
+  </si>
+  <si>
+    <t>Blagden Run</t>
+  </si>
+  <si>
+    <t>treated_sqft</t>
+  </si>
+  <si>
+    <t>impervious_sqft</t>
+  </si>
+  <si>
+    <t>subshed_sqft</t>
   </si>
 </sst>
 </file>
@@ -409,12 +468,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -429,8 +494,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -748,7 +814,7 @@
   <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>
@@ -768,7 +834,7 @@
         <v>74</v>
       </c>
       <c r="C1" t="s">
-        <v>64</v>
+        <v>119</v>
       </c>
       <c r="D1" t="s">
         <v>77</v>
@@ -1017,7 +1083,7 @@
         <v>45</v>
       </c>
       <c r="C19" t="s">
-        <v>45</v>
+        <v>120</v>
       </c>
       <c r="D19" t="s">
         <v>75</v>
@@ -1169,335 +1235,1337 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74512946-BFD5-4355-975E-7040C988669E}">
-  <dimension ref="A1:C29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5527F1A5-7D36-461C-966C-101E89F52B4E}">
+  <dimension ref="A1:H27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E2"/>
+    </sheetView>
+    <sheetView workbookViewId="1"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="25.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F1" t="s">
+        <v>134</v>
+      </c>
+      <c r="G1" t="s">
+        <v>133</v>
+      </c>
+      <c r="H1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E2" t="str">
+        <f>B2 &amp;" - "&amp;D2&amp;" - "&amp;C2</f>
+        <v>Potomac River - MS4 - Battery Kemble Creek</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>125</v>
+      </c>
+      <c r="E3" t="str">
+        <f t="shared" ref="E3:E27" si="0">B3 &amp;" - "&amp;D3&amp;" - "&amp;C3</f>
+        <v>Rock Creek - MS4 - Broad Branch</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
+        <v>125</v>
+      </c>
+      <c r="E4" t="str">
+        <f t="shared" si="0"/>
+        <v>Potomac River - MS4 - Dalecarlia Tributary</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" t="s">
+        <v>125</v>
+      </c>
+      <c r="E5" t="str">
+        <f t="shared" si="0"/>
+        <v>Rock Creek - MS4 - Dumbarton Oaks</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" t="s">
+        <v>125</v>
+      </c>
+      <c r="E6" t="str">
+        <f t="shared" si="0"/>
+        <v>Rock Creek - MS4 - Fenwick Branch</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" t="s">
+        <v>126</v>
+      </c>
+      <c r="C7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" t="s">
+        <v>125</v>
+      </c>
+      <c r="E7" t="str">
+        <f t="shared" si="0"/>
+        <v>Anacostia River - MS4 - Fort Chaplin Tributary</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" t="s">
+        <v>126</v>
+      </c>
+      <c r="C8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" t="s">
+        <v>125</v>
+      </c>
+      <c r="E8" t="str">
+        <f t="shared" si="0"/>
+        <v>Anacostia River - MS4 - Fort Davis Tributary</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" t="s">
+        <v>126</v>
+      </c>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" t="s">
+        <v>125</v>
+      </c>
+      <c r="E9" t="str">
+        <f t="shared" si="0"/>
+        <v>Anacostia River - MS4 - Fort Dupont Tributary</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" t="s">
+        <v>126</v>
+      </c>
+      <c r="C10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" t="s">
+        <v>125</v>
+      </c>
+      <c r="E10" t="str">
+        <f t="shared" si="0"/>
+        <v>Anacostia River - MS4 - Fort Stanton Tributary</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" t="s">
+        <v>124</v>
+      </c>
+      <c r="C11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" t="s">
+        <v>125</v>
+      </c>
+      <c r="E11" t="str">
+        <f t="shared" si="0"/>
+        <v>Potomac River - MS4 - Foundry Branch</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" t="s">
+        <v>126</v>
+      </c>
+      <c r="C12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" t="s">
+        <v>125</v>
+      </c>
+      <c r="E12" t="str">
+        <f t="shared" si="0"/>
+        <v>Anacostia River - MS4 - Hickey Run</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" t="s">
+        <v>78</v>
+      </c>
+      <c r="C13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" t="s">
+        <v>125</v>
+      </c>
+      <c r="E13" t="str">
+        <f t="shared" si="0"/>
+        <v>Rock Creek - MS4 - Klingle Valley Run</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" t="s">
+        <v>78</v>
+      </c>
+      <c r="C14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" t="s">
+        <v>125</v>
+      </c>
+      <c r="E14" t="str">
+        <f t="shared" si="0"/>
+        <v>Rock Creek - MS4 - Luzon Branch</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" t="s">
+        <v>78</v>
+      </c>
+      <c r="C15" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" t="s">
+        <v>125</v>
+      </c>
+      <c r="E15" t="str">
+        <f t="shared" si="0"/>
+        <v>Rock Creek - MS4 - Melvin Hazen Valley Branch</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" t="s">
+        <v>126</v>
+      </c>
+      <c r="C16" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" t="s">
+        <v>125</v>
+      </c>
+      <c r="E16" t="str">
+        <f t="shared" si="0"/>
+        <v>Anacostia River - MS4 - Nash Run</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>120</v>
+      </c>
+      <c r="B17" t="s">
+        <v>78</v>
+      </c>
+      <c r="C17" t="s">
+        <v>120</v>
+      </c>
+      <c r="D17" t="s">
+        <v>125</v>
+      </c>
+      <c r="E17" t="str">
+        <f t="shared" si="0"/>
+        <v>Rock Creek - MS4 - Normanstone Creek</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" t="s">
+        <v>124</v>
+      </c>
+      <c r="C18" t="s">
+        <v>47</v>
+      </c>
+      <c r="D18" t="s">
+        <v>125</v>
+      </c>
+      <c r="E18" t="str">
+        <f t="shared" si="0"/>
+        <v>Potomac River - MS4 - Oxon Run</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" t="s">
+        <v>78</v>
+      </c>
+      <c r="C19" t="s">
+        <v>51</v>
+      </c>
+      <c r="D19" t="s">
+        <v>125</v>
+      </c>
+      <c r="E19" t="str">
+        <f t="shared" si="0"/>
+        <v>Rock Creek - MS4 - Pinehurst Branch</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E20" t="str">
+        <f t="shared" si="0"/>
+        <v>Rock Creek - MS4 - Piney Branch</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" t="s">
+        <v>126</v>
+      </c>
+      <c r="C21" t="s">
+        <v>49</v>
+      </c>
+      <c r="D21" t="s">
+        <v>125</v>
+      </c>
+      <c r="E21" t="str">
+        <f t="shared" si="0"/>
+        <v>Anacostia River - MS4 - Pope Branch</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22" t="s">
+        <v>78</v>
+      </c>
+      <c r="C22" t="s">
+        <v>53</v>
+      </c>
+      <c r="D22" t="s">
+        <v>125</v>
+      </c>
+      <c r="E22" t="str">
+        <f t="shared" si="0"/>
+        <v>Rock Creek - MS4 - Portal Branch</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="E23" t="str">
+        <f t="shared" si="0"/>
+        <v>Rock Creek - CSS - Rock Creek / Piney Branch</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>57</v>
+      </c>
+      <c r="B24" t="s">
+        <v>78</v>
+      </c>
+      <c r="C24" t="s">
+        <v>57</v>
+      </c>
+      <c r="D24" t="s">
+        <v>125</v>
+      </c>
+      <c r="E24" t="str">
+        <f t="shared" si="0"/>
+        <v>Rock Creek - MS4 - Soapstone Creek</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>59</v>
+      </c>
+      <c r="B25" t="s">
+        <v>126</v>
+      </c>
+      <c r="C25" t="s">
+        <v>59</v>
+      </c>
+      <c r="D25" t="s">
+        <v>125</v>
+      </c>
+      <c r="E25" t="str">
+        <f t="shared" si="0"/>
+        <v>Anacostia River - MS4 - Texas Avenue Tributary</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>79</v>
+      </c>
+      <c r="B26" t="s">
+        <v>126</v>
+      </c>
+      <c r="C26" t="s">
+        <v>61</v>
+      </c>
+      <c r="D26" t="s">
+        <v>125</v>
+      </c>
+      <c r="E26" t="str">
+        <f t="shared" si="0"/>
+        <v>Anacostia River - MS4 - Watts Branch - Lower</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>79</v>
+      </c>
+      <c r="B27" t="s">
+        <v>126</v>
+      </c>
+      <c r="C27" t="s">
+        <v>80</v>
+      </c>
+      <c r="D27" t="s">
+        <v>125</v>
+      </c>
+      <c r="E27" t="str">
+        <f t="shared" si="0"/>
+        <v>Anacostia River - MS4 - Watts Branch - Upper</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FCF3A67-4696-4690-90E1-1249EF121DBC}">
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T9" sqref="T9"/>
+      <selection activeCell="E21" sqref="E21"/>
+    </sheetView>
+    <sheetView workbookViewId="1"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="25.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="41.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F1" t="s">
+        <v>134</v>
+      </c>
+      <c r="G1" t="s">
+        <v>133</v>
+      </c>
+      <c r="H1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D2" t="s">
+        <v>127</v>
+      </c>
+      <c r="E2" t="str">
+        <f>B2 &amp;" - "&amp;D2&amp;" - "&amp;C2</f>
+        <v>Rock Creek - CSS - Rock Creek / Piney Branch</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D3" t="s">
+        <v>127</v>
+      </c>
+      <c r="E3" t="str">
+        <f t="shared" ref="E3:E18" si="0">B3 &amp;" - "&amp;D3&amp;" - "&amp;C3</f>
+        <v>Rock Creek - CSS - Rock Creek</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D4" t="s">
+        <v>125</v>
+      </c>
+      <c r="E4" t="str">
+        <f t="shared" si="0"/>
+        <v>Rock Creek - MS4 - Rock Creek</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D5" t="s">
+        <v>125</v>
+      </c>
+      <c r="E5" t="str">
+        <f t="shared" si="0"/>
+        <v>Rock Creek - MS4 - Piney Branch</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" t="s">
+        <v>125</v>
+      </c>
+      <c r="E6" t="str">
+        <f t="shared" si="0"/>
+        <v>Rock Creek - MS4 - Klingle Valley Run</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>78</v>
+      </c>
+      <c r="B7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D7" t="s">
+        <v>125</v>
+      </c>
+      <c r="E7" t="str">
+        <f t="shared" si="0"/>
+        <v>Rock Creek - MS4 - Soapstone Creek</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" t="s">
+        <v>125</v>
+      </c>
+      <c r="E8" t="str">
+        <f t="shared" si="0"/>
+        <v>Rock Creek - MS4 - Melvin Hazen Valley Branch</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>78</v>
+      </c>
+      <c r="B9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" t="s">
+        <v>125</v>
+      </c>
+      <c r="E9" t="str">
+        <f t="shared" si="0"/>
+        <v>Rock Creek - MS4 - Fenwick Branch</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>78</v>
+      </c>
+      <c r="B10" t="s">
+        <v>78</v>
+      </c>
+      <c r="C10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" t="s">
+        <v>125</v>
+      </c>
+      <c r="E10" t="str">
+        <f t="shared" si="0"/>
+        <v>Rock Creek - MS4 - Portal Branch</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>78</v>
+      </c>
+      <c r="B11" t="s">
+        <v>78</v>
+      </c>
+      <c r="C11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" t="s">
+        <v>125</v>
+      </c>
+      <c r="E11" t="str">
+        <f t="shared" si="0"/>
+        <v>Rock Creek - MS4 - Luzon Branch</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>78</v>
+      </c>
+      <c r="B12" t="s">
+        <v>78</v>
+      </c>
+      <c r="C12" t="s">
+        <v>51</v>
+      </c>
+      <c r="D12" t="s">
+        <v>125</v>
+      </c>
+      <c r="E12" t="str">
+        <f t="shared" si="0"/>
+        <v>Rock Creek - MS4 - Pinehurst Branch</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>78</v>
+      </c>
+      <c r="B13" t="s">
+        <v>78</v>
+      </c>
+      <c r="C13" t="s">
+        <v>129</v>
+      </c>
+      <c r="D13" t="s">
+        <v>125</v>
+      </c>
+      <c r="E13" t="str">
+        <f t="shared" si="0"/>
+        <v>Rock Creek - MS4 - Bingham Run</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>78</v>
+      </c>
+      <c r="B14" t="s">
+        <v>78</v>
+      </c>
+      <c r="C14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" t="s">
+        <v>125</v>
+      </c>
+      <c r="E14" t="str">
+        <f t="shared" si="0"/>
+        <v>Rock Creek - MS4 - Broad Branch</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>78</v>
+      </c>
+      <c r="B15" t="s">
+        <v>78</v>
+      </c>
+      <c r="C15" t="s">
+        <v>130</v>
+      </c>
+      <c r="D15" t="s">
+        <v>125</v>
+      </c>
+      <c r="E15" t="str">
+        <f t="shared" si="0"/>
+        <v>Rock Creek - MS4 - Milkhouse Run</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>78</v>
+      </c>
+      <c r="B16" t="s">
+        <v>78</v>
+      </c>
+      <c r="C16" t="s">
+        <v>120</v>
+      </c>
+      <c r="D16" t="s">
+        <v>125</v>
+      </c>
+      <c r="E16" t="str">
+        <f t="shared" si="0"/>
+        <v>Rock Creek - MS4 - Normanstone Creek</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>78</v>
+      </c>
+      <c r="B17" t="s">
+        <v>78</v>
+      </c>
+      <c r="C17" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" t="s">
+        <v>125</v>
+      </c>
+      <c r="E17" t="str">
+        <f t="shared" si="0"/>
+        <v>Rock Creek - MS4 - Dumbarton Oaks</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>78</v>
+      </c>
+      <c r="B18" t="s">
+        <v>78</v>
+      </c>
+      <c r="C18" t="s">
+        <v>131</v>
+      </c>
+      <c r="D18" t="s">
+        <v>125</v>
+      </c>
+      <c r="E18" t="str">
+        <f t="shared" si="0"/>
+        <v>Rock Creek - MS4 - Blagden Run</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74512946-BFD5-4355-975E-7040C988669E}">
+  <dimension ref="A1:G29"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:G1"/>
     </sheetView>
     <sheetView tabSelected="1" workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.33203125" customWidth="1"/>
+    <col min="1" max="1" width="25.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="25.21875" customWidth="1"/>
+    <col min="5" max="5" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>119</v>
+      </c>
       <c r="B1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F1" t="s">
         <v>72</v>
       </c>
-      <c r="C1" t="s">
+      <c r="G1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="str">
+        <f>VLOOKUP(E2,location!$A$2:$C$29,3,FALSE)</f>
+        <v>Rock Creek</v>
+      </c>
+      <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c r="B2">
+      <c r="F2">
         <v>69836129.849999994</v>
       </c>
-      <c r="C2">
+      <c r="G2">
         <v>50051478.759999998</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="e">
+        <f>VLOOKUP(E3,location!$A$2:$C$29,3,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E3" t="s">
         <v>70</v>
       </c>
-      <c r="B3">
+      <c r="F3">
         <v>797091117.29999995</v>
       </c>
-      <c r="C3">
+      <c r="G3">
         <v>266505068.69999999</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="str">
+        <f>VLOOKUP(E4,location!$A$2:$C$29,3,FALSE)</f>
+        <v>Rock Creek</v>
+      </c>
+      <c r="E4" t="s">
         <v>13</v>
       </c>
-      <c r="B4">
+      <c r="F4">
         <v>1033762101</v>
       </c>
-      <c r="C4">
+      <c r="G4">
         <v>393938764.89999998</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="str">
+        <f>VLOOKUP(E5,location!$A$2:$C$29,3,FALSE)</f>
+        <v>Battery Kemble Creek</v>
+      </c>
+      <c r="E5" t="s">
         <v>15</v>
       </c>
-      <c r="B5">
+      <c r="F5">
         <v>10087626.050000001</v>
       </c>
-      <c r="C5">
+      <c r="G5">
         <v>2137233.2710000002</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" t="str">
+        <f>VLOOKUP(E6,location!$A$2:$C$29,3,FALSE)</f>
+        <v>Broad Branch</v>
+      </c>
+      <c r="E6" t="s">
         <v>17</v>
       </c>
-      <c r="B6">
+      <c r="F6">
         <v>51304948.560000002</v>
       </c>
-      <c r="C6">
+      <c r="G6">
         <v>17934581.789999999</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" t="str">
+        <f>VLOOKUP(E7,location!$A$2:$C$29,3,FALSE)</f>
+        <v>Dalecarlia Tributary</v>
+      </c>
+      <c r="E7" t="s">
         <v>19</v>
       </c>
-      <c r="B7">
+      <c r="F7">
         <v>12104505.98</v>
       </c>
-      <c r="C7">
+      <c r="G7">
         <v>3150624.395</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" t="str">
+        <f>VLOOKUP(E8,location!$A$2:$C$29,3,FALSE)</f>
+        <v>Dumbarton Oaks</v>
+      </c>
+      <c r="E8" t="s">
         <v>22</v>
       </c>
-      <c r="B8">
+      <c r="F8">
         <v>5927331.3049999997</v>
       </c>
-      <c r="C8">
+      <c r="G8">
         <v>1625421.122</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" t="str">
+        <f>VLOOKUP(E9,location!$A$2:$C$29,3,FALSE)</f>
+        <v>Fort Dupont Tributary</v>
+      </c>
+      <c r="E9" t="s">
         <v>24</v>
       </c>
-      <c r="B9">
+      <c r="F9">
         <v>17827162.609999999</v>
       </c>
-      <c r="C9">
+      <c r="G9">
         <v>1609838.871</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" t="str">
+        <f>VLOOKUP(E10,location!$A$2:$C$29,3,FALSE)</f>
+        <v>Foundry Branch</v>
+      </c>
+      <c r="E10" t="s">
         <v>26</v>
       </c>
-      <c r="B10">
+      <c r="F10">
         <v>49420747.68</v>
       </c>
-      <c r="C10">
+      <c r="G10">
         <v>18262208.25</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" t="str">
+        <f>VLOOKUP(E11,location!$A$2:$C$29,3,FALSE)</f>
+        <v>Fort Chaplin Tributary</v>
+      </c>
+      <c r="E11" t="s">
         <v>28</v>
       </c>
-      <c r="B11">
+      <c r="F11">
         <v>12695780.83</v>
       </c>
-      <c r="C11">
+      <c r="G11">
         <v>4527052.1179999998</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" t="str">
+        <f>VLOOKUP(E12,location!$A$2:$C$29,3,FALSE)</f>
+        <v>Fort Davis Tributary</v>
+      </c>
+      <c r="E12" t="s">
         <v>30</v>
       </c>
-      <c r="B12">
+      <c r="F12">
         <v>10197296.73</v>
       </c>
-      <c r="C12">
+      <c r="G12">
         <v>3478720.3960000002</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" t="str">
+        <f>VLOOKUP(E13,location!$A$2:$C$29,3,FALSE)</f>
+        <v>Fenwick Branch</v>
+      </c>
+      <c r="E13" t="s">
         <v>32</v>
       </c>
-      <c r="B13">
+      <c r="F13">
         <v>41747880.719999999</v>
       </c>
-      <c r="C13">
+      <c r="G13">
         <v>18710988.010000002</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" t="str">
+        <f>VLOOKUP(E14,location!$A$2:$C$29,3,FALSE)</f>
+        <v>Fort Stanton Tributary</v>
+      </c>
+      <c r="E14" t="s">
         <v>34</v>
       </c>
-      <c r="B14">
+      <c r="F14">
         <v>12060015.970000001</v>
       </c>
-      <c r="C14">
+      <c r="G14">
         <v>5035429.9689999996</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" t="str">
+        <f>VLOOKUP(E15,location!$A$2:$C$29,3,FALSE)</f>
+        <v>Hickey Run</v>
+      </c>
+      <c r="E15" t="s">
         <v>36</v>
       </c>
-      <c r="B15">
+      <c r="F15">
         <v>48083378.079999998</v>
       </c>
-      <c r="C15">
+      <c r="G15">
         <v>20152081.27</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" t="str">
+        <f>VLOOKUP(E16,location!$A$2:$C$29,3,FALSE)</f>
+        <v>Klingle Valley Run</v>
+      </c>
+      <c r="E16" t="s">
         <v>38</v>
       </c>
-      <c r="B16">
+      <c r="F16">
         <v>7485863.1229999997</v>
       </c>
-      <c r="C16">
+      <c r="G16">
         <v>2819719.7179999999</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" t="str">
+        <f>VLOOKUP(E17,location!$A$2:$C$29,3,FALSE)</f>
+        <v>Luzon Branch</v>
+      </c>
+      <c r="E17" t="s">
         <v>40</v>
       </c>
-      <c r="B17">
+      <c r="F17">
         <v>28811482.870000001</v>
       </c>
-      <c r="C17">
+      <c r="G17">
         <v>14779080.73</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" t="str">
+        <f>VLOOKUP(E18,location!$A$2:$C$29,3,FALSE)</f>
+        <v>Melvin Hazen Valley Branch</v>
+      </c>
+      <c r="E18" t="s">
         <v>42</v>
       </c>
-      <c r="B18">
+      <c r="F18">
         <v>7593623.5350000001</v>
       </c>
-      <c r="C18">
+      <c r="G18">
         <v>2576687.5819999999</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" t="str">
+        <f>VLOOKUP(E19,location!$A$2:$C$29,3,FALSE)</f>
+        <v>Nash Run</v>
+      </c>
+      <c r="E19" t="s">
         <v>44</v>
       </c>
-      <c r="B19">
+      <c r="F19">
         <v>28262408.210000001</v>
       </c>
-      <c r="C19">
+      <c r="G19">
         <v>10428891.060000001</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" t="str">
+        <f>VLOOKUP(E20,location!$A$2:$C$29,3,FALSE)</f>
+        <v>Normanstone Creek</v>
+      </c>
+      <c r="E20" t="s">
         <v>46</v>
       </c>
-      <c r="B20">
+      <c r="F20">
         <v>9486410.7420000006</v>
       </c>
-      <c r="C20">
+      <c r="G20">
         <v>3660210.128</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" t="str">
+        <f>VLOOKUP(E21,location!$A$2:$C$29,3,FALSE)</f>
+        <v>Oxon Run</v>
+      </c>
+      <c r="E21" t="s">
         <v>48</v>
       </c>
-      <c r="B21">
+      <c r="F21">
         <v>414641447.69999999</v>
       </c>
-      <c r="C21">
+      <c r="G21">
         <v>145300487.90000001</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" t="str">
+        <f>VLOOKUP(E22,location!$A$2:$C$29,3,FALSE)</f>
+        <v>Pope Branch</v>
+      </c>
+      <c r="E22" t="s">
         <v>50</v>
       </c>
-      <c r="B22">
+      <c r="F22">
         <v>12216430</v>
       </c>
-      <c r="C22">
+      <c r="G22">
         <v>3607941.4730000002</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" t="str">
+        <f>VLOOKUP(E23,location!$A$2:$C$29,3,FALSE)</f>
+        <v>Pinehurst Branch</v>
+      </c>
+      <c r="E23" t="s">
         <v>52</v>
       </c>
-      <c r="B23">
+      <c r="F23">
         <v>28934650.41</v>
       </c>
-      <c r="C23">
+      <c r="G23">
         <v>7336519.3689999999</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" t="str">
+        <f>VLOOKUP(E24,location!$A$2:$C$29,3,FALSE)</f>
+        <v>Portal Branch</v>
+      </c>
+      <c r="E24" t="s">
         <v>54</v>
       </c>
-      <c r="B24">
+      <c r="F24">
         <v>5906012.3820000002</v>
       </c>
-      <c r="C24">
+      <c r="G24">
         <v>2675408.4810000001</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" t="str">
+        <f>VLOOKUP(E25,location!$A$2:$C$29,3,FALSE)</f>
+        <v>Piney Branch</v>
+      </c>
+      <c r="E25" t="s">
         <v>56</v>
       </c>
-      <c r="B25">
+      <c r="F25">
         <v>109878251</v>
       </c>
-      <c r="C25">
+      <c r="G25">
         <v>57375195.619999997</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" t="str">
+        <f>VLOOKUP(E26,location!$A$2:$C$29,3,FALSE)</f>
+        <v>Soapstone Creek</v>
+      </c>
+      <c r="E26" t="s">
         <v>58</v>
       </c>
-      <c r="B26">
+      <c r="F26">
         <v>22493208.359999999</v>
       </c>
-      <c r="C26">
+      <c r="G26">
         <v>10075179</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" t="str">
+        <f>VLOOKUP(E27,location!$A$2:$C$29,3,FALSE)</f>
+        <v>Texas Avenue Tributary</v>
+      </c>
+      <c r="E27" t="s">
         <v>60</v>
       </c>
-      <c r="B27">
+      <c r="F27">
         <v>10859458.939999999</v>
       </c>
-      <c r="C27">
+      <c r="G27">
         <v>4057289.39</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" t="str">
+        <f>VLOOKUP(E28,location!$A$2:$C$29,3,FALSE)</f>
+        <v>Watts Branch</v>
+      </c>
+      <c r="E28" t="s">
         <v>69</v>
       </c>
-      <c r="B28">
+      <c r="F28">
         <v>108610836.7</v>
       </c>
-      <c r="C28">
+      <c r="G28">
         <v>38050077.590000004</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" t="str">
+        <f>VLOOKUP(E29,location!$A$2:$C$29,3,FALSE)</f>
+        <v>Watts Branch</v>
+      </c>
+      <c r="E29" t="s">
         <v>68</v>
       </c>
-      <c r="B29">
+      <c r="F29">
         <v>90723670.299999997</v>
       </c>
-      <c r="C29">
+      <c r="G29">
         <v>32039217.879999999</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Start compiling all scores into a single table
Still need to make sure each individual score table has "sci_subshed" as column name and the parameter name as the other column name
</commit_message>
<xml_diff>
--- a/data/lookup_tables.xlsx
+++ b/data/lookup_tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://limnotech-my.sharepoint.com/personal/srucker_limno_com/Documents/Documents/GitHub/SCI/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="322" documentId="13_ncr:1_{113EE769-9AD3-4243-97B3-520451D281E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DB145C5F-4E28-44E6-8A43-B83E52B0DE31}"/>
+  <xr:revisionPtr revIDLastSave="325" documentId="13_ncr:1_{113EE769-9AD3-4243-97B3-520451D281E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4127BB9D-607A-44B9-AFEA-8970B5B22C19}"/>
   <bookViews>
-    <workbookView xWindow="-14175" yWindow="-14415" windowWidth="23010" windowHeight="12360" firstSheet="7" activeTab="10" xr2:uid="{23697FDE-567D-4570-AE33-F8F65584BB36}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="7" activeTab="10" xr2:uid="{23697FDE-567D-4570-AE33-F8F65584BB36}"/>
   </bookViews>
   <sheets>
     <sheet name="location" sheetId="7" r:id="rId1"/>
@@ -304,9 +304,6 @@
     <t>SEWER_SYST</t>
   </si>
   <si>
-    <t>sci_watershed</t>
-  </si>
-  <si>
     <t>Normanstone Creek</t>
   </si>
   <si>
@@ -446,6 +443,9 @@
   </si>
   <si>
     <t>max_eia_percent</t>
+  </si>
+  <si>
+    <t>sci_subshed</t>
   </si>
 </sst>
 </file>
@@ -806,7 +806,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8059EA70-FEB1-4761-8449-3A8139D2BAE4}">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -824,7 +826,7 @@
         <v>70</v>
       </c>
       <c r="C1" t="s">
-        <v>85</v>
+        <v>132</v>
       </c>
       <c r="D1" t="s">
         <v>73</v>
@@ -1073,7 +1075,7 @@
         <v>45</v>
       </c>
       <c r="C19" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D19" t="s">
         <v>71</v>
@@ -1228,9 +1230,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FCF3A67-4696-4690-90E1-1249EF121DBC}">
   <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1248,40 +1248,40 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>85</v>
+        <v>132</v>
       </c>
       <c r="B1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C1" t="s">
         <v>87</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>88</v>
-      </c>
-      <c r="D1" t="s">
-        <v>89</v>
       </c>
       <c r="E1" t="s">
         <v>81</v>
       </c>
       <c r="F1" t="s">
+        <v>126</v>
+      </c>
+      <c r="G1" t="s">
         <v>127</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>128</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
+        <v>121</v>
+      </c>
+      <c r="J1" t="s">
+        <v>125</v>
+      </c>
+      <c r="K1" t="s">
         <v>129</v>
       </c>
-      <c r="I1" t="s">
-        <v>122</v>
-      </c>
-      <c r="J1" t="s">
-        <v>126</v>
-      </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>130</v>
-      </c>
-      <c r="L1" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
@@ -1292,10 +1292,10 @@
         <v>74</v>
       </c>
       <c r="C2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E2" t="str">
         <f>B2 &amp;" - "&amp;D2&amp;" - "&amp;C2</f>
@@ -1331,7 +1331,7 @@
         <v>74</v>
       </c>
       <c r="D3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E3" t="str">
         <f t="shared" ref="E3:E18" si="0">B3 &amp;" - "&amp;D3&amp;" - "&amp;C3</f>
@@ -1367,7 +1367,7 @@
         <v>74</v>
       </c>
       <c r="D4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E4" t="str">
         <f t="shared" si="0"/>
@@ -1403,7 +1403,7 @@
         <v>55</v>
       </c>
       <c r="D5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E5" t="str">
         <f t="shared" si="0"/>
@@ -1439,7 +1439,7 @@
         <v>37</v>
       </c>
       <c r="D6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E6" t="str">
         <f t="shared" si="0"/>
@@ -1475,7 +1475,7 @@
         <v>57</v>
       </c>
       <c r="D7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E7" t="str">
         <f t="shared" si="0"/>
@@ -1511,7 +1511,7 @@
         <v>41</v>
       </c>
       <c r="D8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E8" t="str">
         <f t="shared" si="0"/>
@@ -1547,7 +1547,7 @@
         <v>31</v>
       </c>
       <c r="D9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E9" t="str">
         <f t="shared" si="0"/>
@@ -1583,7 +1583,7 @@
         <v>53</v>
       </c>
       <c r="D10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E10" t="str">
         <f t="shared" si="0"/>
@@ -1619,7 +1619,7 @@
         <v>39</v>
       </c>
       <c r="D11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E11" t="str">
         <f t="shared" si="0"/>
@@ -1655,7 +1655,7 @@
         <v>51</v>
       </c>
       <c r="D12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E12" t="str">
         <f t="shared" si="0"/>
@@ -1688,10 +1688,10 @@
         <v>74</v>
       </c>
       <c r="C13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E13" t="str">
         <f t="shared" si="0"/>
@@ -1727,7 +1727,7 @@
         <v>16</v>
       </c>
       <c r="D14" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E14" t="str">
         <f t="shared" si="0"/>
@@ -1760,10 +1760,10 @@
         <v>74</v>
       </c>
       <c r="C15" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E15" t="str">
         <f t="shared" si="0"/>
@@ -1796,10 +1796,10 @@
         <v>74</v>
       </c>
       <c r="C16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E16" t="str">
         <f t="shared" si="0"/>
@@ -1835,7 +1835,7 @@
         <v>21</v>
       </c>
       <c r="D17" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E17" t="str">
         <f t="shared" si="0"/>
@@ -1868,10 +1868,10 @@
         <v>74</v>
       </c>
       <c r="C18" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E18" t="str">
         <f t="shared" si="0"/>
@@ -1906,7 +1906,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1916,7 +1916,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -2025,18 +2025,18 @@
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B2" t="s">
         <v>99</v>
-      </c>
-      <c r="B2" t="s">
-        <v>100</v>
       </c>
       <c r="C2" t="s">
         <v>81</v>
@@ -2051,16 +2051,16 @@
         <v>84</v>
       </c>
       <c r="G2" t="s">
+        <v>100</v>
+      </c>
+      <c r="H2" t="s">
         <v>101</v>
       </c>
-      <c r="H2" t="s">
-        <v>102</v>
-      </c>
       <c r="K2" t="s">
+        <v>98</v>
+      </c>
+      <c r="L2" t="s">
         <v>99</v>
-      </c>
-      <c r="L2" t="s">
-        <v>100</v>
       </c>
       <c r="M2" t="s">
         <v>81</v>
@@ -2075,16 +2075,16 @@
         <v>84</v>
       </c>
       <c r="Q2" t="s">
+        <v>100</v>
+      </c>
+      <c r="R2" t="s">
         <v>101</v>
       </c>
-      <c r="R2" t="s">
-        <v>102</v>
-      </c>
       <c r="U2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="V2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="W2" t="s">
         <v>81</v>
@@ -2099,7 +2099,7 @@
         <v>84</v>
       </c>
       <c r="AA2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.3">
@@ -2107,20 +2107,20 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C3" t="str">
         <f t="shared" ref="C3:C34" si="0">D3&amp;" - "&amp;F3&amp;" - "&amp;E3</f>
         <v>Anacostia River - CSS - Anacostia River</v>
       </c>
       <c r="D3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E3" t="s">
+        <v>91</v>
+      </c>
+      <c r="F3" t="s">
         <v>92</v>
-      </c>
-      <c r="E3" t="s">
-        <v>92</v>
-      </c>
-      <c r="F3" t="s">
-        <v>93</v>
       </c>
       <c r="G3">
         <v>52229.235499000002</v>
@@ -2132,20 +2132,20 @@
         <v>1</v>
       </c>
       <c r="L3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M3" t="str">
         <f>N3&amp;" - "&amp;P3&amp;" - "&amp;O3</f>
         <v>Anacostia River - CSS - Anacostia River</v>
       </c>
       <c r="N3" t="s">
+        <v>91</v>
+      </c>
+      <c r="O3" t="s">
+        <v>91</v>
+      </c>
+      <c r="P3" t="s">
         <v>92</v>
-      </c>
-      <c r="O3" t="s">
-        <v>92</v>
-      </c>
-      <c r="P3" t="s">
-        <v>93</v>
       </c>
       <c r="Q3">
         <v>3201774.381029</v>
@@ -2157,20 +2157,20 @@
         <v>1</v>
       </c>
       <c r="V3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="W3" t="str">
         <f>X3&amp;" - "&amp;Z3&amp;" - "&amp;Y3</f>
         <v>Anacostia River - CSS - Anacostia River</v>
       </c>
       <c r="X3" t="s">
+        <v>91</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>91</v>
+      </c>
+      <c r="Z3" t="s">
         <v>92</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>92</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>93</v>
       </c>
       <c r="AA3">
         <v>22372585.52138</v>
@@ -2181,20 +2181,20 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C4" t="str">
         <f t="shared" si="0"/>
         <v>Anacostia River - MS4 - Anacostia River</v>
       </c>
       <c r="D4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G4">
         <v>70918.854263999994</v>
@@ -2206,20 +2206,20 @@
         <v>2</v>
       </c>
       <c r="L4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M4" t="str">
         <f t="shared" ref="M4:M54" si="1">N4&amp;" - "&amp;P4&amp;" - "&amp;O4</f>
         <v>Anacostia River - MS4 - Anacostia River</v>
       </c>
       <c r="N4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="O4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="P4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q4">
         <v>395231.27515900001</v>
@@ -2231,20 +2231,20 @@
         <v>2</v>
       </c>
       <c r="V4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="W4" t="str">
         <f t="shared" ref="W4:W54" si="2">X4&amp;" - "&amp;Z4&amp;" - "&amp;Y4</f>
         <v>Anacostia River - MS4 - Anacostia River</v>
       </c>
       <c r="X4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="Y4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="Z4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AA4">
         <v>12287324.88528</v>
@@ -2255,20 +2255,20 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C5" t="str">
         <f t="shared" si="0"/>
         <v>Anacostia River - MS4 - Anacostia River / Benning-ECap</v>
       </c>
       <c r="D5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G5">
         <v>15567.19304</v>
@@ -2280,20 +2280,20 @@
         <v>3</v>
       </c>
       <c r="L5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M5" t="str">
         <f t="shared" si="1"/>
         <v>Anacostia River - MS4 - Anacostia River / Benning-ECap</v>
       </c>
       <c r="N5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="O5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="P5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q5">
         <v>493558.90466399997</v>
@@ -2305,20 +2305,20 @@
         <v>3</v>
       </c>
       <c r="V5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="W5" t="str">
         <f t="shared" si="2"/>
         <v>Anacostia River - MS4 - Anacostia River / Benning-ECap</v>
       </c>
       <c r="X5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="Y5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="Z5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AA5">
         <v>2029942.3796260001</v>
@@ -2329,20 +2329,20 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C6" t="str">
         <f t="shared" si="0"/>
         <v>Anacostia River - MS4 - Anacostia River / Naylor</v>
       </c>
       <c r="D6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G6">
         <v>6898.8047059999999</v>
@@ -2354,20 +2354,20 @@
         <v>4</v>
       </c>
       <c r="L6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M6" t="str">
         <f t="shared" si="1"/>
         <v>Anacostia River - MS4 - Anacostia River / Naylor</v>
       </c>
       <c r="N6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="O6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="P6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q6">
         <v>85233.205191000001</v>
@@ -2379,20 +2379,20 @@
         <v>4</v>
       </c>
       <c r="V6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="W6" t="str">
         <f t="shared" si="2"/>
         <v>Anacostia River - MS4 - Anacostia River / Naylor</v>
       </c>
       <c r="X6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="Y6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="Z6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AA6">
         <v>116119.34</v>
@@ -2403,20 +2403,20 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C7" t="str">
         <f t="shared" si="0"/>
         <v>Anacostia River - MS4 - Anacostia River / Northwest Anacostia</v>
       </c>
       <c r="D7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G7">
         <v>12164.09059</v>
@@ -2428,20 +2428,20 @@
         <v>5</v>
       </c>
       <c r="L7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M7" t="str">
         <f t="shared" si="1"/>
         <v>Anacostia River - MS4 - Anacostia River / Northwest Anacostia</v>
       </c>
       <c r="N7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="O7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="P7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q7">
         <v>47026.645927999998</v>
@@ -2453,20 +2453,20 @@
         <v>5</v>
       </c>
       <c r="V7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="W7" t="str">
         <f t="shared" si="2"/>
         <v>Anacostia River - MS4 - Anacostia River / Northwest Anacostia</v>
       </c>
       <c r="X7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="Y7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="Z7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AA7">
         <v>1537111.8</v>
@@ -2477,20 +2477,20 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" si="0"/>
         <v>Anacostia River - MS4 - Anacostia River / Ridge</v>
       </c>
       <c r="D8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G8">
         <v>6140.4891950000001</v>
@@ -2502,20 +2502,20 @@
         <v>6</v>
       </c>
       <c r="L8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M8" t="str">
         <f t="shared" si="1"/>
         <v>Anacostia River - MS4 - Anacostia River / Ridge</v>
       </c>
       <c r="N8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="O8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="P8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q8">
         <v>75320.481400999997</v>
@@ -2527,20 +2527,20 @@
         <v>6</v>
       </c>
       <c r="V8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="W8" t="str">
         <f t="shared" si="2"/>
         <v>Anacostia River - MS4 - Anacostia River / Ridge</v>
       </c>
       <c r="X8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="Y8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="Z8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AA8">
         <v>184753.5</v>
@@ -2551,20 +2551,20 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C9" t="str">
         <f t="shared" si="0"/>
         <v>Anacostia River - MS4 - Anacostia River / Sligo Creek</v>
       </c>
       <c r="D9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G9">
         <v>7988.540602</v>
@@ -2576,20 +2576,20 @@
         <v>7</v>
       </c>
       <c r="L9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M9" t="str">
         <f t="shared" si="1"/>
         <v>Anacostia River - MS4 - Anacostia River / Sligo Creek</v>
       </c>
       <c r="N9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="O9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="P9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q9">
         <v>124751.107412</v>
@@ -2601,20 +2601,20 @@
         <v>7</v>
       </c>
       <c r="V9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="W9" t="str">
         <f t="shared" si="2"/>
         <v>Anacostia River - MS4 - Anacostia River / Sligo Creek</v>
       </c>
       <c r="X9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="Y9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="Z9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AA9">
         <v>452698.47252000001</v>
@@ -2625,20 +2625,20 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" si="0"/>
         <v>Anacostia River - MS4 - Anacostia River / Suitland-Stickfoot</v>
       </c>
       <c r="D10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G10">
         <v>18514.055501999999</v>
@@ -2650,20 +2650,20 @@
         <v>8</v>
       </c>
       <c r="L10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M10" t="str">
         <f t="shared" si="1"/>
         <v>Anacostia River - MS4 - Anacostia River / Suitland-Stickfoot</v>
       </c>
       <c r="N10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="O10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="P10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q10">
         <v>380730.98753899999</v>
@@ -2675,20 +2675,20 @@
         <v>8</v>
       </c>
       <c r="V10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="W10" t="str">
         <f t="shared" si="2"/>
         <v>Anacostia River - MS4 - Anacostia River / Suitland-Stickfoot</v>
       </c>
       <c r="X10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="Y10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="Z10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AA10">
         <v>5428279.8678000001</v>
@@ -2699,20 +2699,20 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C11" t="str">
         <f t="shared" si="0"/>
         <v>Anacostia River - MS4 - Anacostia River / To MD - Anacostia</v>
       </c>
       <c r="D11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G11">
         <v>7844.2283550000002</v>
@@ -2724,20 +2724,20 @@
         <v>9</v>
       </c>
       <c r="L11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M11" t="str">
         <f t="shared" si="1"/>
         <v>Anacostia River - MS4 - Anacostia River / To MD - Anacostia</v>
       </c>
       <c r="N11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="O11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="P11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q11">
         <v>118351.62962599999</v>
@@ -2749,20 +2749,20 @@
         <v>9</v>
       </c>
       <c r="V11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="W11" t="str">
         <f t="shared" si="2"/>
         <v>Anacostia River - MS4 - Anacostia River / To MD - Anacostia</v>
       </c>
       <c r="X11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="Y11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="Z11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AA11">
         <v>150542.92154400001</v>
@@ -2773,20 +2773,20 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C12" t="str">
         <f t="shared" si="0"/>
         <v>Anacostia River - MS4 - Fort Chaplin Tributary</v>
       </c>
       <c r="D12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E12" t="s">
         <v>27</v>
       </c>
       <c r="F12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G12">
         <v>10033.585967000001</v>
@@ -2798,20 +2798,20 @@
         <v>10</v>
       </c>
       <c r="L12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M12" t="str">
         <f t="shared" si="1"/>
         <v>Anacostia River - MS4 - Fort Chaplin Tributary</v>
       </c>
       <c r="N12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="O12" t="s">
         <v>27</v>
       </c>
       <c r="P12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q12">
         <v>149145.92131199999</v>
@@ -2823,20 +2823,20 @@
         <v>10</v>
       </c>
       <c r="V12" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="W12" t="str">
         <f t="shared" si="2"/>
         <v>Anacostia River - MS4 - Fort Chaplin Tributary</v>
       </c>
       <c r="X12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="Y12" t="s">
         <v>27</v>
       </c>
       <c r="Z12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AA12">
         <v>768027.46</v>
@@ -2847,20 +2847,20 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C13" t="str">
         <f t="shared" si="0"/>
         <v>Anacostia River - MS4 - Fort Davis Tributary</v>
       </c>
       <c r="D13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E13" t="s">
         <v>29</v>
       </c>
       <c r="F13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G13">
         <v>8128.2598310000003</v>
@@ -2872,20 +2872,20 @@
         <v>11</v>
       </c>
       <c r="L13" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M13" t="str">
         <f t="shared" si="1"/>
         <v>Anacostia River - MS4 - Fort Davis Tributary</v>
       </c>
       <c r="N13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="O13" t="s">
         <v>29</v>
       </c>
       <c r="P13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q13">
         <v>109230.585076</v>
@@ -2897,20 +2897,20 @@
         <v>11</v>
       </c>
       <c r="V13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="W13" t="str">
         <f t="shared" si="2"/>
         <v>Anacostia River - MS4 - Fort Davis Tributary</v>
       </c>
       <c r="X13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="Y13" t="s">
         <v>29</v>
       </c>
       <c r="Z13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AA13">
         <v>237072.41034</v>
@@ -2921,20 +2921,20 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C14" t="str">
         <f t="shared" si="0"/>
         <v>Anacostia River - MS4 - Fort Dupont Tributary</v>
       </c>
       <c r="D14" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E14" t="s">
         <v>23</v>
       </c>
       <c r="F14" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G14">
         <v>8035.5652229999996</v>
@@ -2946,20 +2946,20 @@
         <v>12</v>
       </c>
       <c r="L14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M14" t="str">
         <f t="shared" si="1"/>
         <v>Anacostia River - MS4 - Fort Dupont Tributary</v>
       </c>
       <c r="N14" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="O14" t="s">
         <v>23</v>
       </c>
       <c r="P14" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q14">
         <v>52259.606752</v>
@@ -2971,20 +2971,20 @@
         <v>12</v>
       </c>
       <c r="V14" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="W14" t="str">
         <f t="shared" si="2"/>
         <v>Anacostia River - MS4 - Fort Dupont Tributary</v>
       </c>
       <c r="X14" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="Y14" t="s">
         <v>23</v>
       </c>
       <c r="Z14" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AA14">
         <v>177741.03056000001</v>
@@ -2995,20 +2995,20 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C15" t="str">
         <f t="shared" si="0"/>
         <v>Anacostia River - MS4 - Fort Stanton Tributary</v>
       </c>
       <c r="D15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E15" t="s">
         <v>33</v>
       </c>
       <c r="F15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G15">
         <v>8849.4169660000007</v>
@@ -3020,20 +3020,20 @@
         <v>13</v>
       </c>
       <c r="L15" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M15" t="str">
         <f t="shared" si="1"/>
         <v>Anacostia River - MS4 - Fort Stanton Tributary</v>
       </c>
       <c r="N15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="O15" t="s">
         <v>33</v>
       </c>
       <c r="P15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q15">
         <v>125898.988492</v>
@@ -3045,20 +3045,20 @@
         <v>13</v>
       </c>
       <c r="V15" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="W15" t="str">
         <f t="shared" si="2"/>
         <v>Anacostia River - MS4 - Fort Stanton Tributary</v>
       </c>
       <c r="X15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="Y15" t="s">
         <v>33</v>
       </c>
       <c r="Z15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AA15">
         <v>1001244.8</v>
@@ -3069,20 +3069,20 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C16" t="str">
         <f t="shared" si="0"/>
         <v>Anacostia River - MS4 - Hickey Run</v>
       </c>
       <c r="D16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E16" t="s">
         <v>35</v>
       </c>
       <c r="F16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G16">
         <v>13796.368617</v>
@@ -3094,20 +3094,20 @@
         <v>14</v>
       </c>
       <c r="L16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M16" t="str">
         <f t="shared" si="1"/>
         <v>Anacostia River - MS4 - Hickey Run</v>
       </c>
       <c r="N16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="O16" t="s">
         <v>35</v>
       </c>
       <c r="P16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q16">
         <v>334416.73605000001</v>
@@ -3119,20 +3119,20 @@
         <v>14</v>
       </c>
       <c r="V16" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="W16" t="str">
         <f t="shared" si="2"/>
         <v>Anacostia River - MS4 - Hickey Run</v>
       </c>
       <c r="X16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="Y16" t="s">
         <v>35</v>
       </c>
       <c r="Z16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AA16">
         <v>17219627.360909998</v>
@@ -3143,20 +3143,20 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C17" t="str">
         <f t="shared" si="0"/>
         <v>Anacostia River - MS4 - Kingman Lake</v>
       </c>
       <c r="D17" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E17" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F17" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G17">
         <v>10516.253885</v>
@@ -3168,20 +3168,20 @@
         <v>15</v>
       </c>
       <c r="L17" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M17" t="str">
         <f t="shared" si="1"/>
         <v>Anacostia River - MS4 - Kingman Lake</v>
       </c>
       <c r="N17" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="O17" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="P17" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q17">
         <v>150532.263236</v>
@@ -3193,20 +3193,20 @@
         <v>15</v>
       </c>
       <c r="V17" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="W17" t="str">
         <f t="shared" si="2"/>
         <v>Anacostia River - MS4 - Kingman Lake</v>
       </c>
       <c r="X17" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="Y17" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="Z17" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AA17">
         <v>1394451.68</v>
@@ -3217,20 +3217,20 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C18" t="str">
         <f t="shared" si="0"/>
         <v>Anacostia River - MS4 - Lower Beaverdam Creek</v>
       </c>
       <c r="D18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E18" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G18">
         <v>3005.5902019999999</v>
@@ -3242,20 +3242,20 @@
         <v>16</v>
       </c>
       <c r="L18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M18" t="str">
         <f t="shared" si="1"/>
         <v>Anacostia River - MS4 - Lower Beaverdam Creek</v>
       </c>
       <c r="N18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="O18" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="P18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q18">
         <v>6129.9075750000002</v>
@@ -3267,20 +3267,20 @@
         <v>16</v>
       </c>
       <c r="V18" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="W18" t="str">
         <f t="shared" si="2"/>
         <v>Anacostia River - MS4 - Lower Beaverdam Creek</v>
       </c>
       <c r="X18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="Y18" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="Z18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AA18">
         <v>58224</v>
@@ -3291,20 +3291,20 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C19" t="str">
         <f t="shared" si="0"/>
         <v>Anacostia River - MS4 - Nash Run</v>
       </c>
       <c r="D19" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E19" t="s">
         <v>43</v>
       </c>
       <c r="F19" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G19">
         <v>8546.0344420000001</v>
@@ -3316,20 +3316,20 @@
         <v>17</v>
       </c>
       <c r="L19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M19" t="str">
         <f t="shared" si="1"/>
         <v>Anacostia River - MS4 - Nash Run</v>
       </c>
       <c r="N19" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="O19" t="s">
         <v>43</v>
       </c>
       <c r="P19" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q19">
         <v>187316.89359200001</v>
@@ -3341,20 +3341,20 @@
         <v>17</v>
       </c>
       <c r="V19" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="W19" t="str">
         <f t="shared" si="2"/>
         <v>Anacostia River - MS4 - Nash Run</v>
       </c>
       <c r="X19" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="Y19" t="s">
         <v>43</v>
       </c>
       <c r="Z19" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AA19">
         <v>707857.25361599994</v>
@@ -3365,20 +3365,20 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C20" t="str">
         <f t="shared" si="0"/>
         <v>Anacostia River - MS4 - Northwest Branch</v>
       </c>
       <c r="D20" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E20" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F20" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G20">
         <v>16297.958084</v>
@@ -3390,20 +3390,20 @@
         <v>18</v>
       </c>
       <c r="L20" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M20" t="str">
         <f t="shared" si="1"/>
         <v>Anacostia River - MS4 - Northwest Branch</v>
       </c>
       <c r="N20" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="O20" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="P20" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q20">
         <v>1037350.52987</v>
@@ -3415,20 +3415,20 @@
         <v>18</v>
       </c>
       <c r="V20" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="W20" t="str">
         <f t="shared" si="2"/>
         <v>Anacostia River - MS4 - Northwest Branch</v>
       </c>
       <c r="X20" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="Y20" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="Z20" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AA20">
         <v>3904344.6596829998</v>
@@ -3439,20 +3439,20 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C21" t="str">
         <f t="shared" si="0"/>
         <v>Anacostia River - MS4 - Pope Branch</v>
       </c>
       <c r="D21" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E21" t="s">
         <v>49</v>
       </c>
       <c r="F21" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G21">
         <v>8976.1789700000008</v>
@@ -3464,20 +3464,20 @@
         <v>19</v>
       </c>
       <c r="L21" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M21" t="str">
         <f t="shared" si="1"/>
         <v>Anacostia River - MS4 - Pope Branch</v>
       </c>
       <c r="N21" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="O21" t="s">
         <v>49</v>
       </c>
       <c r="P21" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q21">
         <v>110849.163783</v>
@@ -3489,20 +3489,20 @@
         <v>19</v>
       </c>
       <c r="V21" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="W21" t="str">
         <f t="shared" si="2"/>
         <v>Anacostia River - MS4 - Pope Branch</v>
       </c>
       <c r="X21" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="Y21" t="s">
         <v>49</v>
       </c>
       <c r="Z21" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AA21">
         <v>108168.17</v>
@@ -3513,20 +3513,20 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C22" t="str">
         <f t="shared" si="0"/>
         <v>Anacostia River - MS4 - Texas Avenue Tributary</v>
       </c>
       <c r="D22" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E22" t="s">
         <v>59</v>
       </c>
       <c r="F22" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G22">
         <v>7328.0668809999997</v>
@@ -3538,20 +3538,20 @@
         <v>20</v>
       </c>
       <c r="L22" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M22" t="str">
         <f t="shared" si="1"/>
         <v>Anacostia River - MS4 - Texas Avenue Tributary</v>
       </c>
       <c r="N22" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="O22" t="s">
         <v>59</v>
       </c>
       <c r="P22" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q22">
         <v>117662.415549</v>
@@ -3563,20 +3563,20 @@
         <v>20</v>
       </c>
       <c r="V22" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="W22" t="str">
         <f t="shared" si="2"/>
         <v>Anacostia River - MS4 - Texas Avenue Tributary</v>
       </c>
       <c r="X22" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="Y22" t="s">
         <v>59</v>
       </c>
       <c r="Z22" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AA22">
         <v>1023406.87528</v>
@@ -3587,20 +3587,20 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C23" t="str">
         <f t="shared" si="0"/>
         <v>Anacostia River - MS4 - Watts Branch - Lower</v>
       </c>
       <c r="D23" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E23" t="s">
         <v>61</v>
       </c>
       <c r="F23" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G23">
         <v>6788.6184999999996</v>
@@ -3612,20 +3612,20 @@
         <v>21</v>
       </c>
       <c r="L23" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M23" t="str">
         <f t="shared" si="1"/>
         <v>Anacostia River - MS4 - Watts Branch - Lower</v>
       </c>
       <c r="N23" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="O23" t="s">
         <v>61</v>
       </c>
       <c r="P23" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q23">
         <v>153674.42840199999</v>
@@ -3637,20 +3637,20 @@
         <v>21</v>
       </c>
       <c r="V23" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="W23" t="str">
         <f t="shared" si="2"/>
         <v>Anacostia River - MS4 - Watts Branch - Lower</v>
       </c>
       <c r="X23" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="Y23" t="s">
         <v>61</v>
       </c>
       <c r="Z23" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AA23">
         <v>1867917.21056</v>
@@ -3661,20 +3661,20 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C24" t="str">
         <f t="shared" si="0"/>
         <v>Anacostia River - MS4 - Watts Branch - Upper</v>
       </c>
       <c r="D24" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E24" t="s">
         <v>76</v>
       </c>
       <c r="F24" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G24">
         <v>9944.8095880000001</v>
@@ -3686,20 +3686,20 @@
         <v>22</v>
       </c>
       <c r="L24" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M24" t="str">
         <f t="shared" si="1"/>
         <v>Anacostia River - MS4 - Watts Branch - Upper</v>
       </c>
       <c r="N24" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="O24" t="s">
         <v>76</v>
       </c>
       <c r="P24" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q24">
         <v>474384.54226299998</v>
@@ -3711,20 +3711,20 @@
         <v>22</v>
       </c>
       <c r="V24" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="W24" t="str">
         <f t="shared" si="2"/>
         <v>Anacostia River - MS4 - Watts Branch - Upper</v>
       </c>
       <c r="X24" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="Y24" t="s">
         <v>76</v>
       </c>
       <c r="Z24" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AA24">
         <v>1911943.256325</v>
@@ -3735,20 +3735,20 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C25" t="str">
         <f t="shared" si="0"/>
         <v>Potomac River - MS4 - Battery Kemble Creek</v>
       </c>
       <c r="D25" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E25" t="s">
         <v>14</v>
       </c>
       <c r="F25" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G25">
         <v>7791.1871849999998</v>
@@ -3760,20 +3760,20 @@
         <v>23</v>
       </c>
       <c r="L25" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M25" t="str">
         <f t="shared" si="1"/>
         <v>Potomac River - MS4 - Battery Kemble Creek</v>
       </c>
       <c r="N25" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="O25" t="s">
         <v>14</v>
       </c>
       <c r="P25" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q25">
         <v>65919.970967999994</v>
@@ -3785,20 +3785,20 @@
         <v>23</v>
       </c>
       <c r="V25" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="W25" t="str">
         <f t="shared" si="2"/>
         <v>Potomac River - MS4 - Battery Kemble Creek</v>
       </c>
       <c r="X25" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="Y25" t="s">
         <v>14</v>
       </c>
       <c r="Z25" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AA25">
         <v>380435</v>
@@ -3809,20 +3809,20 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C26" t="str">
         <f t="shared" si="0"/>
         <v>Potomac River - MS4 - C &amp; O Canal</v>
       </c>
       <c r="D26" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E26" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G26">
         <v>24075.785219000001</v>
@@ -3834,20 +3834,20 @@
         <v>24</v>
       </c>
       <c r="L26" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M26" t="str">
         <f t="shared" si="1"/>
         <v>Potomac River - MS4 - C &amp; O Canal</v>
       </c>
       <c r="N26" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="O26" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="P26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q26">
         <v>240031.94635700001</v>
@@ -3859,20 +3859,20 @@
         <v>24</v>
       </c>
       <c r="V26" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="W26" t="str">
         <f t="shared" si="2"/>
         <v>Potomac River - MS4 - C &amp; O Canal</v>
       </c>
       <c r="X26" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="Y26" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="Z26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AA26">
         <v>1454945.14056</v>
@@ -3883,20 +3883,20 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C27" t="str">
         <f t="shared" si="0"/>
         <v>Potomac River - MS4 - Dalecarlia Tributary</v>
       </c>
       <c r="D27" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E27" t="s">
         <v>18</v>
       </c>
       <c r="F27" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G27">
         <v>7023.5963279999996</v>
@@ -3908,20 +3908,20 @@
         <v>25</v>
       </c>
       <c r="L27" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M27" t="str">
         <f t="shared" si="1"/>
         <v>Potomac River - MS4 - Dalecarlia Tributary</v>
       </c>
       <c r="N27" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="O27" t="s">
         <v>18</v>
       </c>
       <c r="P27" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q27">
         <v>89745.101723</v>
@@ -3933,20 +3933,20 @@
         <v>25</v>
       </c>
       <c r="V27" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="W27" t="str">
         <f t="shared" si="2"/>
         <v>Potomac River - MS4 - Dalecarlia Tributary</v>
       </c>
       <c r="X27" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="Y27" t="s">
         <v>18</v>
       </c>
       <c r="Z27" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AA27">
         <v>255414</v>
@@ -3957,20 +3957,20 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C28" t="str">
         <f t="shared" si="0"/>
         <v>Potomac River - MS4 - Foundry Branch</v>
       </c>
       <c r="D28" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E28" t="s">
         <v>25</v>
       </c>
       <c r="F28" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G28">
         <v>14508.009964999999</v>
@@ -3982,20 +3982,20 @@
         <v>26</v>
       </c>
       <c r="L28" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M28" t="str">
         <f t="shared" si="1"/>
         <v>Potomac River - MS4 - Foundry Branch</v>
       </c>
       <c r="N28" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="O28" t="s">
         <v>25</v>
       </c>
       <c r="P28" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q28">
         <v>457643.41666300001</v>
@@ -4007,20 +4007,20 @@
         <v>26</v>
       </c>
       <c r="V28" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="W28" t="str">
         <f t="shared" si="2"/>
         <v>Potomac River - MS4 - Foundry Branch</v>
       </c>
       <c r="X28" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="Y28" t="s">
         <v>25</v>
       </c>
       <c r="Z28" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AA28">
         <v>2619097.3403039998</v>
@@ -4031,20 +4031,20 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C29" t="str">
         <f t="shared" si="0"/>
         <v>Potomac River - MS4 - Oxon Run</v>
       </c>
       <c r="D29" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E29" t="s">
         <v>47</v>
       </c>
       <c r="F29" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G29">
         <v>25322.430544999999</v>
@@ -4056,20 +4056,20 @@
         <v>27</v>
       </c>
       <c r="L29" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M29" t="str">
         <f t="shared" si="1"/>
         <v>Potomac River - MS4 - Oxon Run</v>
       </c>
       <c r="N29" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="O29" t="s">
         <v>47</v>
       </c>
       <c r="P29" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q29">
         <v>1116218.047125</v>
@@ -4081,20 +4081,20 @@
         <v>27</v>
       </c>
       <c r="V29" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="W29" t="str">
         <f t="shared" si="2"/>
         <v>Potomac River - MS4 - Oxon Run</v>
       </c>
       <c r="X29" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="Y29" t="s">
         <v>47</v>
       </c>
       <c r="Z29" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AA29">
         <v>5103945.4106769999</v>
@@ -4105,20 +4105,20 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C30" t="str">
         <f t="shared" si="0"/>
         <v>Potomac River - CSS - Potomac River</v>
       </c>
       <c r="D30" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E30" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F30" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G30">
         <v>28235.478543000001</v>
@@ -4130,20 +4130,20 @@
         <v>28</v>
       </c>
       <c r="L30" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M30" t="str">
         <f t="shared" si="1"/>
         <v>Potomac River - CSS - Potomac River</v>
       </c>
       <c r="N30" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="O30" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="P30" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="Q30">
         <v>509021.646358</v>
@@ -4155,20 +4155,20 @@
         <v>28</v>
       </c>
       <c r="V30" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="W30" t="str">
         <f t="shared" si="2"/>
         <v>Potomac River - CSS - Potomac River</v>
       </c>
       <c r="X30" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="Y30" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="Z30" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="AA30">
         <v>4741171.750461</v>
@@ -4179,20 +4179,20 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C31" t="str">
         <f t="shared" si="0"/>
         <v>Potomac River - MS4 - Potomac River</v>
       </c>
       <c r="D31" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E31" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F31" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G31">
         <v>72550.510769</v>
@@ -4204,20 +4204,20 @@
         <v>29</v>
       </c>
       <c r="L31" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M31" t="str">
         <f t="shared" si="1"/>
         <v>Potomac River - MS4 - Potomac River</v>
       </c>
       <c r="N31" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="O31" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="P31" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q31">
         <v>783467.23483700003</v>
@@ -4229,20 +4229,20 @@
         <v>29</v>
       </c>
       <c r="V31" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="W31" t="str">
         <f t="shared" si="2"/>
         <v>Potomac River - MS4 - Potomac River</v>
       </c>
       <c r="X31" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="Y31" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="Z31" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AA31">
         <v>4464167.6281199995</v>
@@ -4253,20 +4253,20 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C32" t="str">
         <f t="shared" si="0"/>
         <v>Potomac River - MS4 - Potomac River / Mill Creek</v>
       </c>
       <c r="D32" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E32" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F32" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G32">
         <v>9029.8248829999993</v>
@@ -4278,20 +4278,20 @@
         <v>30</v>
       </c>
       <c r="L32" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M32" t="str">
         <f t="shared" si="1"/>
         <v>Potomac River - MS4 - Potomac River / Mill Creek</v>
       </c>
       <c r="N32" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="O32" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="P32" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q32">
         <v>432160.081939</v>
@@ -4303,20 +4303,20 @@
         <v>30</v>
       </c>
       <c r="V32" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="W32" t="str">
         <f t="shared" si="2"/>
         <v>Potomac River - MS4 - Potomac River / Mill Creek</v>
       </c>
       <c r="X32" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="Y32" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="Z32" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AA32">
         <v>808390.92652600002</v>
@@ -4327,20 +4327,20 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C33" t="str">
         <f t="shared" si="0"/>
         <v>Potomac River - MS4 - Potomac River / Oxon Cove</v>
       </c>
       <c r="D33" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E33" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F33" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G33">
         <v>3558.1353389999999</v>
@@ -4352,20 +4352,20 @@
         <v>31</v>
       </c>
       <c r="L33" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M33" t="str">
         <f t="shared" si="1"/>
         <v>Potomac River - MS4 - Potomac River / Oxon Cove</v>
       </c>
       <c r="N33" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="O33" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="P33" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q33">
         <v>11359.981919</v>
@@ -4377,20 +4377,20 @@
         <v>31</v>
       </c>
       <c r="V33" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="W33" t="str">
         <f t="shared" si="2"/>
         <v>Potomac River - MS4 - Potomac River / Oxon Cove</v>
       </c>
       <c r="X33" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="Y33" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="Z33" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AA33">
         <v>1568704</v>
@@ -4401,20 +4401,20 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C34" t="str">
         <f t="shared" si="0"/>
         <v>Potomac River - MS4 - Potomac River / To Little Falls</v>
       </c>
       <c r="D34" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E34" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F34" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G34">
         <v>7063.8792830000002</v>
@@ -4426,20 +4426,20 @@
         <v>32</v>
       </c>
       <c r="L34" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M34" t="str">
         <f t="shared" si="1"/>
         <v>Potomac River - MS4 - Potomac River / To Little Falls</v>
       </c>
       <c r="N34" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="O34" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="P34" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q34">
         <v>103301.417221</v>
@@ -4451,20 +4451,20 @@
         <v>32</v>
       </c>
       <c r="V34" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="W34" t="str">
         <f t="shared" si="2"/>
         <v>Potomac River - MS4 - Potomac River / To Little Falls</v>
       </c>
       <c r="X34" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="Y34" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="Z34" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AA34">
         <v>212133.691238</v>
@@ -4475,20 +4475,20 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C35" t="str">
-        <f t="shared" ref="C35:C66" si="3">D35&amp;" - "&amp;F35&amp;" - "&amp;E35</f>
+        <f t="shared" ref="C35:C54" si="3">D35&amp;" - "&amp;F35&amp;" - "&amp;E35</f>
         <v>Potomac River - MS4 - Potomac River / Unknown Creek to Little Falls</v>
       </c>
       <c r="D35" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E35" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F35" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G35">
         <v>1965.728073</v>
@@ -4500,20 +4500,20 @@
         <v>33</v>
       </c>
       <c r="L35" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M35" t="str">
         <f t="shared" si="1"/>
         <v>Potomac River - MS4 - Potomac River / Unknown Creek to Little Falls</v>
       </c>
       <c r="N35" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="O35" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="P35" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q35">
         <v>13793.733683</v>
@@ -4525,20 +4525,20 @@
         <v>33</v>
       </c>
       <c r="V35" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="W35" t="str">
         <f t="shared" si="2"/>
         <v>Potomac River - MS4 - Potomac River / Unknown Creek to Little Falls</v>
       </c>
       <c r="X35" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="Y35" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="Z35" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AA35">
         <v>27529</v>
@@ -4549,20 +4549,20 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C36" t="str">
         <f t="shared" si="3"/>
         <v>Potomac River - MS4 - Tidal Basin</v>
       </c>
       <c r="D36" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E36" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F36" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G36">
         <v>9396.7228689999993</v>
@@ -4574,20 +4574,20 @@
         <v>34</v>
       </c>
       <c r="L36" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M36" t="str">
         <f t="shared" si="1"/>
         <v>Potomac River - MS4 - Tidal Basin</v>
       </c>
       <c r="N36" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="O36" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="P36" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q36">
         <v>89924.524558000005</v>
@@ -4599,20 +4599,20 @@
         <v>34</v>
       </c>
       <c r="V36" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="W36" t="str">
         <f t="shared" si="2"/>
         <v>Potomac River - MS4 - Tidal Basin</v>
       </c>
       <c r="X36" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="Y36" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="Z36" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AA36">
         <v>380525.64</v>
@@ -4623,20 +4623,20 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C37" t="str">
         <f t="shared" si="3"/>
         <v>Potomac River - MS4 - Washington Ship Channel</v>
       </c>
       <c r="D37" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E37" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F37" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G37">
         <v>14413.507315000001</v>
@@ -4648,20 +4648,20 @@
         <v>35</v>
       </c>
       <c r="L37" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M37" t="str">
         <f t="shared" si="1"/>
         <v>Potomac River - MS4 - Washington Ship Channel</v>
       </c>
       <c r="N37" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="O37" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="P37" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q37">
         <v>236295.435356</v>
@@ -4673,20 +4673,20 @@
         <v>35</v>
       </c>
       <c r="V37" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="W37" t="str">
         <f t="shared" si="2"/>
         <v>Potomac River - MS4 - Washington Ship Channel</v>
       </c>
       <c r="X37" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="Y37" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="Z37" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AA37">
         <v>2274319.9700000002</v>
@@ -4697,7 +4697,7 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C38" t="str">
         <f t="shared" si="3"/>
@@ -4707,10 +4707,10 @@
         <v>74</v>
       </c>
       <c r="E38" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F38" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G38">
         <v>4209.4905319999998</v>
@@ -4722,7 +4722,7 @@
         <v>36</v>
       </c>
       <c r="L38" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M38" t="str">
         <f t="shared" si="1"/>
@@ -4732,10 +4732,10 @@
         <v>74</v>
       </c>
       <c r="O38" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="P38" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q38">
         <v>42485.409610000002</v>
@@ -4747,7 +4747,7 @@
         <v>36</v>
       </c>
       <c r="V38" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="W38" t="str">
         <f t="shared" si="2"/>
@@ -4757,10 +4757,10 @@
         <v>74</v>
       </c>
       <c r="Y38" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="Z38" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AA38">
         <v>379316.2</v>
@@ -4771,7 +4771,7 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C39" t="str">
         <f t="shared" si="3"/>
@@ -4781,10 +4781,10 @@
         <v>74</v>
       </c>
       <c r="E39" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F39" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G39">
         <v>6010.7046879999998</v>
@@ -4796,7 +4796,7 @@
         <v>37</v>
       </c>
       <c r="L39" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M39" t="str">
         <f t="shared" si="1"/>
@@ -4806,10 +4806,10 @@
         <v>74</v>
       </c>
       <c r="O39" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="P39" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q39">
         <v>80175.560461999994</v>
@@ -4821,7 +4821,7 @@
         <v>37</v>
       </c>
       <c r="V39" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="W39" t="str">
         <f t="shared" si="2"/>
@@ -4831,10 +4831,10 @@
         <v>74</v>
       </c>
       <c r="Y39" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="Z39" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AA39">
         <v>387046.12</v>
@@ -4845,7 +4845,7 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C40" t="str">
         <f t="shared" si="3"/>
@@ -4858,7 +4858,7 @@
         <v>16</v>
       </c>
       <c r="F40" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G40">
         <v>12392.819351</v>
@@ -4870,7 +4870,7 @@
         <v>38</v>
       </c>
       <c r="L40" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M40" t="str">
         <f t="shared" si="1"/>
@@ -4883,7 +4883,7 @@
         <v>16</v>
       </c>
       <c r="P40" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q40">
         <v>567630.77776800003</v>
@@ -4895,7 +4895,7 @@
         <v>38</v>
       </c>
       <c r="V40" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="W40" t="str">
         <f t="shared" si="2"/>
@@ -4908,7 +4908,7 @@
         <v>16</v>
       </c>
       <c r="Z40" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AA40">
         <v>1117618.041373</v>
@@ -4919,7 +4919,7 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C41" t="str">
         <f t="shared" si="3"/>
@@ -4932,7 +4932,7 @@
         <v>21</v>
       </c>
       <c r="F41" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G41">
         <v>4448.8809250000004</v>
@@ -4944,7 +4944,7 @@
         <v>39</v>
       </c>
       <c r="L41" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M41" t="str">
         <f t="shared" si="1"/>
@@ -4957,7 +4957,7 @@
         <v>21</v>
       </c>
       <c r="P41" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q41">
         <v>31968.044718000001</v>
@@ -4969,7 +4969,7 @@
         <v>39</v>
       </c>
       <c r="V41" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="W41" t="str">
         <f t="shared" si="2"/>
@@ -4982,7 +4982,7 @@
         <v>21</v>
       </c>
       <c r="Z41" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AA41">
         <v>141034.4</v>
@@ -4993,7 +4993,7 @@
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C42" t="str">
         <f t="shared" si="3"/>
@@ -5006,7 +5006,7 @@
         <v>31</v>
       </c>
       <c r="F42" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G42">
         <v>8641.7816210000001</v>
@@ -5018,7 +5018,7 @@
         <v>40</v>
       </c>
       <c r="L42" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M42" t="str">
         <f t="shared" si="1"/>
@@ -5031,7 +5031,7 @@
         <v>31</v>
       </c>
       <c r="P42" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q42">
         <v>98130.810981999995</v>
@@ -5043,7 +5043,7 @@
         <v>40</v>
       </c>
       <c r="V42" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="W42" t="str">
         <f t="shared" si="2"/>
@@ -5056,7 +5056,7 @@
         <v>31</v>
       </c>
       <c r="Z42" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AA42">
         <v>100035.041018</v>
@@ -5067,7 +5067,7 @@
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C43" t="str">
         <f t="shared" si="3"/>
@@ -5080,7 +5080,7 @@
         <v>37</v>
       </c>
       <c r="F43" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G43">
         <v>8944.4209489999994</v>
@@ -5092,7 +5092,7 @@
         <v>41</v>
       </c>
       <c r="L43" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M43" t="str">
         <f t="shared" si="1"/>
@@ -5105,7 +5105,7 @@
         <v>37</v>
       </c>
       <c r="P43" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q43">
         <v>74481.859614999994</v>
@@ -5117,7 +5117,7 @@
         <v>41</v>
       </c>
       <c r="V43" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="W43" t="str">
         <f t="shared" si="2"/>
@@ -5130,7 +5130,7 @@
         <v>37</v>
       </c>
       <c r="Z43" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AA43">
         <v>365082.01527999999</v>
@@ -5141,7 +5141,7 @@
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C44" t="str">
         <f t="shared" si="3"/>
@@ -5154,7 +5154,7 @@
         <v>39</v>
       </c>
       <c r="F44" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G44">
         <v>12183.955723999999</v>
@@ -5166,7 +5166,7 @@
         <v>42</v>
       </c>
       <c r="L44" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M44" t="str">
         <f t="shared" si="1"/>
@@ -5179,7 +5179,7 @@
         <v>39</v>
       </c>
       <c r="P44" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q44">
         <v>345224.954218</v>
@@ -5191,7 +5191,7 @@
         <v>42</v>
       </c>
       <c r="V44" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="W44" t="str">
         <f t="shared" si="2"/>
@@ -5204,7 +5204,7 @@
         <v>39</v>
       </c>
       <c r="Z44" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AA44">
         <v>943535.51400199998</v>
@@ -5215,7 +5215,7 @@
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C45" t="str">
         <f t="shared" si="3"/>
@@ -5228,7 +5228,7 @@
         <v>41</v>
       </c>
       <c r="F45" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G45">
         <v>7061.6749559999998</v>
@@ -5240,7 +5240,7 @@
         <v>43</v>
       </c>
       <c r="L45" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M45" t="str">
         <f t="shared" si="1"/>
@@ -5253,7 +5253,7 @@
         <v>41</v>
       </c>
       <c r="P45" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q45">
         <v>61582.030580999999</v>
@@ -5265,7 +5265,7 @@
         <v>43</v>
       </c>
       <c r="V45" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="W45" t="str">
         <f t="shared" si="2"/>
@@ -5278,7 +5278,7 @@
         <v>41</v>
       </c>
       <c r="Z45" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AA45">
         <v>287341.69527999999</v>
@@ -5289,7 +5289,7 @@
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C46" t="str">
         <f t="shared" si="3"/>
@@ -5299,10 +5299,10 @@
         <v>74</v>
       </c>
       <c r="E46" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F46" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G46">
         <v>2687.2219700000001</v>
@@ -5314,7 +5314,7 @@
         <v>44</v>
       </c>
       <c r="L46" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M46" t="str">
         <f t="shared" si="1"/>
@@ -5324,10 +5324,10 @@
         <v>74</v>
       </c>
       <c r="O46" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="P46" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q46">
         <v>8563.0073900000007</v>
@@ -5339,7 +5339,7 @@
         <v>44</v>
       </c>
       <c r="V46" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="W46" t="str">
         <f t="shared" si="2"/>
@@ -5349,10 +5349,10 @@
         <v>74</v>
       </c>
       <c r="Y46" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="Z46" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AA46">
         <v>40207.339999999997</v>
@@ -5363,7 +5363,7 @@
         <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C47" t="str">
         <f t="shared" si="3"/>
@@ -5373,10 +5373,10 @@
         <v>74</v>
       </c>
       <c r="E47" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F47" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G47">
         <v>9859.9593829999994</v>
@@ -5388,7 +5388,7 @@
         <v>45</v>
       </c>
       <c r="L47" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M47" t="str">
         <f t="shared" si="1"/>
@@ -5398,10 +5398,10 @@
         <v>74</v>
       </c>
       <c r="O47" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="P47" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q47">
         <v>112011.83674499999</v>
@@ -5413,7 +5413,7 @@
         <v>45</v>
       </c>
       <c r="V47" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="W47" t="str">
         <f t="shared" si="2"/>
@@ -5423,10 +5423,10 @@
         <v>74</v>
       </c>
       <c r="Y47" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="Z47" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AA47">
         <v>353269</v>
@@ -5437,7 +5437,7 @@
         <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C48" t="str">
         <f t="shared" si="3"/>
@@ -5450,7 +5450,7 @@
         <v>51</v>
       </c>
       <c r="F48" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G48">
         <v>7940.9767030000003</v>
@@ -5462,7 +5462,7 @@
         <v>46</v>
       </c>
       <c r="L48" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M48" t="str">
         <f t="shared" si="1"/>
@@ -5475,7 +5475,7 @@
         <v>51</v>
       </c>
       <c r="P48" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q48">
         <v>138566.00618</v>
@@ -5487,7 +5487,7 @@
         <v>46</v>
       </c>
       <c r="V48" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="W48" t="str">
         <f t="shared" si="2"/>
@@ -5500,7 +5500,7 @@
         <v>51</v>
       </c>
       <c r="Z48" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AA48">
         <v>664773.17561999999</v>
@@ -5511,7 +5511,7 @@
         <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C49" t="str">
         <f t="shared" si="3"/>
@@ -5524,7 +5524,7 @@
         <v>55</v>
       </c>
       <c r="F49" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G49">
         <v>10181.275958</v>
@@ -5536,7 +5536,7 @@
         <v>47</v>
       </c>
       <c r="L49" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M49" t="str">
         <f t="shared" si="1"/>
@@ -5549,7 +5549,7 @@
         <v>55</v>
       </c>
       <c r="P49" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q49">
         <v>59810.91994</v>
@@ -5561,7 +5561,7 @@
         <v>47</v>
       </c>
       <c r="V49" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="W49" t="str">
         <f t="shared" si="2"/>
@@ -5574,7 +5574,7 @@
         <v>55</v>
       </c>
       <c r="Z49" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AA49">
         <v>96536.639999999999</v>
@@ -5585,7 +5585,7 @@
         <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C50" t="str">
         <f t="shared" si="3"/>
@@ -5598,7 +5598,7 @@
         <v>53</v>
       </c>
       <c r="F50" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G50">
         <v>2956.753044</v>
@@ -5610,7 +5610,7 @@
         <v>48</v>
       </c>
       <c r="L50" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M50" t="str">
         <f t="shared" si="1"/>
@@ -5623,7 +5623,7 @@
         <v>53</v>
       </c>
       <c r="P50" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q50">
         <v>28461.971171000001</v>
@@ -5635,7 +5635,7 @@
         <v>48</v>
       </c>
       <c r="V50" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="W50" t="str">
         <f t="shared" si="2"/>
@@ -5648,7 +5648,7 @@
         <v>53</v>
       </c>
       <c r="Z50" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AA50">
         <v>17157</v>
@@ -5659,7 +5659,7 @@
         <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C51" t="str">
         <f t="shared" si="3"/>
@@ -5672,7 +5672,7 @@
         <v>74</v>
       </c>
       <c r="F51" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G51">
         <v>32599.900953</v>
@@ -5684,7 +5684,7 @@
         <v>49</v>
       </c>
       <c r="L51" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M51" t="str">
         <f t="shared" si="1"/>
@@ -5697,7 +5697,7 @@
         <v>74</v>
       </c>
       <c r="P51" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="Q51">
         <v>798663.83966900001</v>
@@ -5709,7 +5709,7 @@
         <v>49</v>
       </c>
       <c r="V51" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="W51" t="str">
         <f t="shared" si="2"/>
@@ -5722,7 +5722,7 @@
         <v>74</v>
       </c>
       <c r="Z51" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="AA51">
         <v>3257267.9736270001</v>
@@ -5733,7 +5733,7 @@
         <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C52" t="str">
         <f t="shared" si="3"/>
@@ -5746,7 +5746,7 @@
         <v>74</v>
       </c>
       <c r="F52" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G52">
         <v>71774.352461000002</v>
@@ -5758,7 +5758,7 @@
         <v>50</v>
       </c>
       <c r="L52" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M52" t="str">
         <f t="shared" si="1"/>
@@ -5771,7 +5771,7 @@
         <v>74</v>
       </c>
       <c r="P52" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q52">
         <v>586000.84358900005</v>
@@ -5783,7 +5783,7 @@
         <v>50</v>
       </c>
       <c r="V52" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="W52" t="str">
         <f t="shared" si="2"/>
@@ -5796,7 +5796,7 @@
         <v>74</v>
       </c>
       <c r="Z52" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AA52">
         <v>1926145.1587739999</v>
@@ -5807,7 +5807,7 @@
         <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C53" t="str">
         <f t="shared" si="3"/>
@@ -5817,10 +5817,10 @@
         <v>74</v>
       </c>
       <c r="E53" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F53" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G53">
         <v>26360.728088</v>
@@ -5832,7 +5832,7 @@
         <v>51</v>
       </c>
       <c r="L53" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M53" t="str">
         <f t="shared" si="1"/>
@@ -5842,10 +5842,10 @@
         <v>74</v>
       </c>
       <c r="O53" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="P53" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="Q53">
         <v>1452134.9693410001</v>
@@ -5857,7 +5857,7 @@
         <v>51</v>
       </c>
       <c r="V53" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="W53" t="str">
         <f t="shared" si="2"/>
@@ -5867,10 +5867,10 @@
         <v>74</v>
       </c>
       <c r="Y53" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="Z53" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="AA53">
         <v>4796879.8973519998</v>
@@ -5881,7 +5881,7 @@
         <v>52</v>
       </c>
       <c r="B54" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C54" t="str">
         <f t="shared" si="3"/>
@@ -5894,7 +5894,7 @@
         <v>57</v>
       </c>
       <c r="F54" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G54">
         <v>9626.0710990000007</v>
@@ -5906,7 +5906,7 @@
         <v>52</v>
       </c>
       <c r="L54" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M54" t="str">
         <f t="shared" si="1"/>
@@ -5919,7 +5919,7 @@
         <v>57</v>
       </c>
       <c r="P54" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q54">
         <v>241791.126323</v>
@@ -5931,7 +5931,7 @@
         <v>52</v>
       </c>
       <c r="V54" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="W54" t="str">
         <f t="shared" si="2"/>
@@ -5944,7 +5944,7 @@
         <v>57</v>
       </c>
       <c r="Z54" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AA54">
         <v>1113950.1399999999</v>
@@ -6113,7 +6113,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BC52232-62A1-4046-A953-F434B4285A01}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -7690,9 +7690,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5527F1A5-7D36-461C-966C-101E89F52B4E}">
   <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -7709,40 +7707,40 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>85</v>
+        <v>132</v>
       </c>
       <c r="B1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C1" t="s">
         <v>87</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>88</v>
-      </c>
-      <c r="D1" t="s">
-        <v>89</v>
       </c>
       <c r="E1" t="s">
         <v>81</v>
       </c>
       <c r="F1" t="s">
+        <v>126</v>
+      </c>
+      <c r="G1" t="s">
         <v>127</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>128</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
+        <v>121</v>
+      </c>
+      <c r="J1" t="s">
+        <v>125</v>
+      </c>
+      <c r="K1" t="s">
         <v>129</v>
       </c>
-      <c r="I1" t="s">
-        <v>122</v>
-      </c>
-      <c r="J1" t="s">
-        <v>126</v>
-      </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>130</v>
-      </c>
-      <c r="L1" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
@@ -7750,13 +7748,13 @@
         <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E2" t="str">
         <f>B2 &amp;" - "&amp;D2&amp;" - "&amp;C2</f>
@@ -7792,7 +7790,7 @@
         <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E3" t="str">
         <f t="shared" ref="E3:E27" si="0">B3 &amp;" - "&amp;D3&amp;" - "&amp;C3</f>
@@ -7822,13 +7820,13 @@
         <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C4" t="s">
         <v>18</v>
       </c>
       <c r="D4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E4" t="str">
         <f t="shared" si="0"/>
@@ -7864,7 +7862,7 @@
         <v>21</v>
       </c>
       <c r="D5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E5" t="str">
         <f t="shared" si="0"/>
@@ -7900,7 +7898,7 @@
         <v>31</v>
       </c>
       <c r="D6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E6" t="str">
         <f t="shared" si="0"/>
@@ -7930,13 +7928,13 @@
         <v>27</v>
       </c>
       <c r="B7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C7" t="s">
         <v>27</v>
       </c>
       <c r="D7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E7" t="str">
         <f t="shared" si="0"/>
@@ -7966,13 +7964,13 @@
         <v>29</v>
       </c>
       <c r="B8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C8" t="s">
         <v>29</v>
       </c>
       <c r="D8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E8" t="str">
         <f t="shared" si="0"/>
@@ -8002,13 +8000,13 @@
         <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C9" t="s">
         <v>23</v>
       </c>
       <c r="D9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E9" t="str">
         <f t="shared" si="0"/>
@@ -8038,13 +8036,13 @@
         <v>33</v>
       </c>
       <c r="B10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C10" t="s">
         <v>33</v>
       </c>
       <c r="D10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E10" t="str">
         <f t="shared" si="0"/>
@@ -8074,13 +8072,13 @@
         <v>25</v>
       </c>
       <c r="B11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C11" t="s">
         <v>25</v>
       </c>
       <c r="D11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E11" t="str">
         <f t="shared" si="0"/>
@@ -8110,13 +8108,13 @@
         <v>35</v>
       </c>
       <c r="B12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C12" t="s">
         <v>35</v>
       </c>
       <c r="D12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E12" t="str">
         <f t="shared" si="0"/>
@@ -8152,7 +8150,7 @@
         <v>37</v>
       </c>
       <c r="D13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E13" t="str">
         <f t="shared" si="0"/>
@@ -8188,7 +8186,7 @@
         <v>39</v>
       </c>
       <c r="D14" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E14" t="str">
         <f t="shared" si="0"/>
@@ -8224,7 +8222,7 @@
         <v>41</v>
       </c>
       <c r="D15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E15" t="str">
         <f t="shared" si="0"/>
@@ -8254,13 +8252,13 @@
         <v>43</v>
       </c>
       <c r="B16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C16" t="s">
         <v>43</v>
       </c>
       <c r="D16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E16" t="str">
         <f t="shared" si="0"/>
@@ -8287,16 +8285,16 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B17" t="s">
         <v>74</v>
       </c>
       <c r="C17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D17" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E17" t="str">
         <f t="shared" si="0"/>
@@ -8326,13 +8324,13 @@
         <v>47</v>
       </c>
       <c r="B18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C18" t="s">
         <v>47</v>
       </c>
       <c r="D18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E18" t="str">
         <f t="shared" si="0"/>
@@ -8368,7 +8366,7 @@
         <v>51</v>
       </c>
       <c r="D19" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E19" t="str">
         <f t="shared" si="0"/>
@@ -8404,7 +8402,7 @@
         <v>55</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E20" t="str">
         <f t="shared" si="0"/>
@@ -8434,13 +8432,13 @@
         <v>49</v>
       </c>
       <c r="B21" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C21" t="s">
         <v>49</v>
       </c>
       <c r="D21" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E21" t="str">
         <f t="shared" si="0"/>
@@ -8476,7 +8474,7 @@
         <v>53</v>
       </c>
       <c r="D22" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E22" t="str">
         <f t="shared" si="0"/>
@@ -8509,10 +8507,10 @@
         <v>74</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E23" t="str">
         <f t="shared" si="0"/>
@@ -8548,7 +8546,7 @@
         <v>57</v>
       </c>
       <c r="D24" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E24" t="str">
         <f t="shared" si="0"/>
@@ -8578,13 +8576,13 @@
         <v>59</v>
       </c>
       <c r="B25" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C25" t="s">
         <v>59</v>
       </c>
       <c r="D25" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E25" t="str">
         <f t="shared" si="0"/>
@@ -8614,13 +8612,13 @@
         <v>75</v>
       </c>
       <c r="B26" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C26" t="s">
         <v>61</v>
       </c>
       <c r="D26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E26" t="str">
         <f t="shared" si="0"/>
@@ -8650,13 +8648,13 @@
         <v>75</v>
       </c>
       <c r="B27" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C27" t="s">
         <v>76</v>
       </c>
       <c r="D27" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E27" t="str">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
Format wq and wq_nutrient parameters for compiling
Aggregate by sci_subshed rather than location_id
</commit_message>
<xml_diff>
--- a/data/lookup_tables.xlsx
+++ b/data/lookup_tables.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://limnotech-my.sharepoint.com/personal/srucker_limno_com/Documents/Documents/GitHub/SCI/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\srucker\Git\SCI\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="346" documentId="13_ncr:1_{113EE769-9AD3-4243-97B3-520451D281E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D7D1C747-CB30-4FEE-8980-5C3D1EBA835A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD6EB2A4-1FD4-42E4-92E6-5C3A2A743EE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{23697FDE-567D-4570-AE33-F8F65584BB36}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{23697FDE-567D-4570-AE33-F8F65584BB36}"/>
   </bookViews>
   <sheets>
-    <sheet name="location" sheetId="7" r:id="rId1"/>
+    <sheet name="location_id" sheetId="7" r:id="rId1"/>
     <sheet name="location_name" sheetId="18" r:id="rId2"/>
     <sheet name="sci_subshed " sheetId="17" r:id="rId3"/>
     <sheet name="dumpsite_score" sheetId="1" r:id="rId4"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1397" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1340" uniqueCount="135">
   <si>
     <t>max_sites_per_mile</t>
   </si>
@@ -469,7 +469,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -479,12 +479,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -501,10 +495,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -819,421 +812,248 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8059EA70-FEB1-4761-8449-3A8139D2BAE4}">
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:B29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>63</v>
       </c>
       <c r="B1" t="s">
         <v>70</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>10</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>13</v>
       </c>
       <c r="B3" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>15</v>
       </c>
       <c r="B4" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>17</v>
       </c>
       <c r="B5" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>19</v>
       </c>
       <c r="B6" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>22</v>
       </c>
       <c r="B7" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>24</v>
       </c>
       <c r="B8" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>26</v>
       </c>
       <c r="B9" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>28</v>
       </c>
       <c r="B10" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>30</v>
       </c>
       <c r="B11" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>32</v>
       </c>
       <c r="B12" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>34</v>
       </c>
       <c r="B13" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>36</v>
       </c>
       <c r="B14" t="s">
         <v>35</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>38</v>
       </c>
       <c r="B15" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>40</v>
       </c>
       <c r="B16" t="s">
         <v>39</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>42</v>
       </c>
       <c r="B17" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>44</v>
       </c>
       <c r="B18" t="s">
         <v>43</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>46</v>
       </c>
       <c r="B19" t="s">
         <v>45</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>48</v>
       </c>
       <c r="B20" t="s">
         <v>47</v>
       </c>
-      <c r="C20" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>50</v>
       </c>
       <c r="B21" t="s">
         <v>49</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>52</v>
       </c>
       <c r="B22" t="s">
         <v>51</v>
       </c>
-      <c r="C22" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>54</v>
       </c>
       <c r="B23" t="s">
         <v>53</v>
       </c>
-      <c r="C23" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>56</v>
       </c>
       <c r="B24" t="s">
         <v>55</v>
       </c>
-      <c r="C24" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>58</v>
       </c>
       <c r="B25" t="s">
         <v>57</v>
       </c>
-      <c r="C25" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>60</v>
       </c>
       <c r="B26" t="s">
         <v>59</v>
       </c>
-      <c r="C26" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>62</v>
       </c>
       <c r="B27" t="s">
         <v>61</v>
       </c>
-      <c r="C27" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>69</v>
       </c>
       <c r="B28" t="s">
         <v>76</v>
       </c>
-      <c r="C28" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>68</v>
       </c>
       <c r="B29" t="s">
         <v>76</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -1247,15 +1067,15 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>64</v>
       </c>
@@ -1269,7 +1089,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>74</v>
       </c>
@@ -1283,7 +1103,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -1297,7 +1117,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -1311,7 +1131,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -1325,7 +1145,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -1339,7 +1159,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -1353,7 +1173,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -1361,7 +1181,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -1375,7 +1195,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -1389,7 +1209,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -1403,7 +1223,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>33</v>
       </c>
@@ -1417,7 +1237,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -1431,7 +1251,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>37</v>
       </c>
@@ -1445,7 +1265,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>39</v>
       </c>
@@ -1459,7 +1279,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>41</v>
       </c>
@@ -1473,7 +1293,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>43</v>
       </c>
@@ -1487,7 +1307,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>45</v>
       </c>
@@ -1501,7 +1321,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>47</v>
       </c>
@@ -1515,7 +1335,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>49</v>
       </c>
@@ -1529,7 +1349,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>51</v>
       </c>
@@ -1543,7 +1363,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>53</v>
       </c>
@@ -1557,7 +1377,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>55</v>
       </c>
@@ -1571,7 +1391,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>57</v>
       </c>
@@ -1585,7 +1405,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>59</v>
       </c>
@@ -1599,7 +1419,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>75</v>
       </c>
@@ -1624,20 +1444,20 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="42.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>132</v>
       </c>
@@ -1675,7 +1495,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -1711,7 +1531,7 @@
         <v>380435</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -1747,7 +1567,7 @@
         <v>1117618.041373</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -1783,7 +1603,7 @@
         <v>255414</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -1819,7 +1639,7 @@
         <v>141034.4</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>31</v>
       </c>
@@ -1855,7 +1675,7 @@
         <v>100035.041018</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>27</v>
       </c>
@@ -1891,7 +1711,7 @@
         <v>768027.46</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -1927,7 +1747,7 @@
         <v>237072.41034</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -1963,7 +1783,7 @@
         <v>177741.03056000001</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>33</v>
       </c>
@@ -1999,7 +1819,7 @@
         <v>1001244.8</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>25</v>
       </c>
@@ -2035,7 +1855,7 @@
         <v>2619097.3403039998</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>35</v>
       </c>
@@ -2071,7 +1891,7 @@
         <v>17219627.360909998</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>37</v>
       </c>
@@ -2107,7 +1927,7 @@
         <v>365082.01527999999</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>39</v>
       </c>
@@ -2143,7 +1963,7 @@
         <v>943535.51400199998</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>41</v>
       </c>
@@ -2179,7 +1999,7 @@
         <v>287341.69527999999</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>43</v>
       </c>
@@ -2215,7 +2035,7 @@
         <v>707857.25361599994</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>85</v>
       </c>
@@ -2251,7 +2071,7 @@
         <v>353269</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>47</v>
       </c>
@@ -2287,7 +2107,7 @@
         <v>5103945.4106769999</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>51</v>
       </c>
@@ -2323,7 +2143,7 @@
         <v>664773.17561999999</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>55</v>
       </c>
@@ -2359,7 +2179,7 @@
         <v>96536.639999999999</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>49</v>
       </c>
@@ -2395,7 +2215,7 @@
         <v>108168.17</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>53</v>
       </c>
@@ -2431,7 +2251,7 @@
         <v>17157</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>55</v>
       </c>
@@ -2467,7 +2287,7 @@
         <v>4796879.8973519998</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>57</v>
       </c>
@@ -2503,7 +2323,7 @@
         <v>1113950.1399999999</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>59</v>
       </c>
@@ -2539,7 +2359,7 @@
         <v>1023406.87528</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>75</v>
       </c>
@@ -2575,7 +2395,7 @@
         <v>1867917.21056</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>75</v>
       </c>
@@ -2622,21 +2442,21 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="41.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="41.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>132</v>
       </c>
@@ -2674,7 +2494,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>74</v>
       </c>
@@ -2710,7 +2530,7 @@
         <v>4796879.8973519998</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>74</v>
       </c>
@@ -2746,7 +2566,7 @@
         <v>3257267.9736270001</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>74</v>
       </c>
@@ -2782,7 +2602,7 @@
         <v>1926145.1587739999</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>74</v>
       </c>
@@ -2818,7 +2638,7 @@
         <v>96536.639999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>74</v>
       </c>
@@ -2854,7 +2674,7 @@
         <v>365082.01527999999</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>74</v>
       </c>
@@ -2890,7 +2710,7 @@
         <v>1113950.1399999999</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>74</v>
       </c>
@@ -2926,7 +2746,7 @@
         <v>287341.69527999999</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>74</v>
       </c>
@@ -2962,7 +2782,7 @@
         <v>100035.041018</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>74</v>
       </c>
@@ -2998,7 +2818,7 @@
         <v>17157</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>74</v>
       </c>
@@ -3034,7 +2854,7 @@
         <v>943535.51400199998</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>74</v>
       </c>
@@ -3070,7 +2890,7 @@
         <v>664773.17561999999</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>74</v>
       </c>
@@ -3106,7 +2926,7 @@
         <v>379316.2</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>74</v>
       </c>
@@ -3142,7 +2962,7 @@
         <v>1117618.041373</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>74</v>
       </c>
@@ -3178,7 +2998,7 @@
         <v>40207.339999999997</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>74</v>
       </c>
@@ -3214,7 +3034,7 @@
         <v>353269</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>74</v>
       </c>
@@ -3250,7 +3070,7 @@
         <v>141034.4</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>74</v>
       </c>
@@ -3299,9 +3119,9 @@
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -3309,7 +3129,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>10</v>
       </c>
@@ -3317,7 +3137,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>9</v>
       </c>
@@ -3325,7 +3145,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>8</v>
       </c>
@@ -3333,7 +3153,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>7</v>
       </c>
@@ -3341,7 +3161,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>6</v>
       </c>
@@ -3349,7 +3169,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -3357,7 +3177,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>4</v>
       </c>
@@ -3365,7 +3185,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>3</v>
       </c>
@@ -3373,7 +3193,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2</v>
       </c>
@@ -3381,7 +3201,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1</v>
       </c>
@@ -3402,18 +3222,18 @@
       <selection activeCell="V20" sqref="V20:V21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="58" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="39" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="58" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="58" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>97</v>
       </c>
@@ -3421,7 +3241,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>98</v>
       </c>
@@ -3492,7 +3312,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3566,7 +3386,7 @@
         <v>22372585.52138</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -3640,7 +3460,7 @@
         <v>12287324.88528</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -3714,7 +3534,7 @@
         <v>2029942.3796260001</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -3788,7 +3608,7 @@
         <v>116119.34</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -3862,7 +3682,7 @@
         <v>1537111.8</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -3936,7 +3756,7 @@
         <v>184753.5</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -4010,7 +3830,7 @@
         <v>452698.47252000001</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -4084,7 +3904,7 @@
         <v>5428279.8678000001</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
@@ -4158,7 +3978,7 @@
         <v>150542.92154400001</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
@@ -4232,7 +4052,7 @@
         <v>768027.46</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
@@ -4306,7 +4126,7 @@
         <v>237072.41034</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
@@ -4380,7 +4200,7 @@
         <v>177741.03056000001</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
@@ -4454,7 +4274,7 @@
         <v>1001244.8</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
@@ -4528,7 +4348,7 @@
         <v>17219627.360909998</v>
       </c>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15</v>
       </c>
@@ -4602,7 +4422,7 @@
         <v>1394451.68</v>
       </c>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>16</v>
       </c>
@@ -4676,7 +4496,7 @@
         <v>58224</v>
       </c>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>17</v>
       </c>
@@ -4750,7 +4570,7 @@
         <v>707857.25361599994</v>
       </c>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>18</v>
       </c>
@@ -4824,7 +4644,7 @@
         <v>3904344.6596829998</v>
       </c>
     </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>19</v>
       </c>
@@ -4898,7 +4718,7 @@
         <v>108168.17</v>
       </c>
     </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>20</v>
       </c>
@@ -4972,7 +4792,7 @@
         <v>1023406.87528</v>
       </c>
     </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>21</v>
       </c>
@@ -5046,7 +4866,7 @@
         <v>1867917.21056</v>
       </c>
     </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>22</v>
       </c>
@@ -5120,7 +4940,7 @@
         <v>1911943.256325</v>
       </c>
     </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>23</v>
       </c>
@@ -5194,7 +5014,7 @@
         <v>380435</v>
       </c>
     </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>24</v>
       </c>
@@ -5268,7 +5088,7 @@
         <v>1454945.14056</v>
       </c>
     </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>25</v>
       </c>
@@ -5342,7 +5162,7 @@
         <v>255414</v>
       </c>
     </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>26</v>
       </c>
@@ -5416,7 +5236,7 @@
         <v>2619097.3403039998</v>
       </c>
     </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>27</v>
       </c>
@@ -5490,7 +5310,7 @@
         <v>5103945.4106769999</v>
       </c>
     </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>28</v>
       </c>
@@ -5564,7 +5384,7 @@
         <v>4741171.750461</v>
       </c>
     </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>29</v>
       </c>
@@ -5638,7 +5458,7 @@
         <v>4464167.6281199995</v>
       </c>
     </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>30</v>
       </c>
@@ -5712,7 +5532,7 @@
         <v>808390.92652600002</v>
       </c>
     </row>
-    <row r="33" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>31</v>
       </c>
@@ -5786,7 +5606,7 @@
         <v>1568704</v>
       </c>
     </row>
-    <row r="34" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>32</v>
       </c>
@@ -5860,7 +5680,7 @@
         <v>212133.691238</v>
       </c>
     </row>
-    <row r="35" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>33</v>
       </c>
@@ -5934,7 +5754,7 @@
         <v>27529</v>
       </c>
     </row>
-    <row r="36" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>34</v>
       </c>
@@ -6008,7 +5828,7 @@
         <v>380525.64</v>
       </c>
     </row>
-    <row r="37" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>35</v>
       </c>
@@ -6082,7 +5902,7 @@
         <v>2274319.9700000002</v>
       </c>
     </row>
-    <row r="38" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>36</v>
       </c>
@@ -6156,7 +5976,7 @@
         <v>379316.2</v>
       </c>
     </row>
-    <row r="39" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>37</v>
       </c>
@@ -6230,7 +6050,7 @@
         <v>387046.12</v>
       </c>
     </row>
-    <row r="40" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>38</v>
       </c>
@@ -6304,7 +6124,7 @@
         <v>1117618.041373</v>
       </c>
     </row>
-    <row r="41" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>39</v>
       </c>
@@ -6378,7 +6198,7 @@
         <v>141034.4</v>
       </c>
     </row>
-    <row r="42" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>40</v>
       </c>
@@ -6452,7 +6272,7 @@
         <v>100035.041018</v>
       </c>
     </row>
-    <row r="43" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>41</v>
       </c>
@@ -6526,7 +6346,7 @@
         <v>365082.01527999999</v>
       </c>
     </row>
-    <row r="44" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>42</v>
       </c>
@@ -6600,7 +6420,7 @@
         <v>943535.51400199998</v>
       </c>
     </row>
-    <row r="45" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>43</v>
       </c>
@@ -6674,7 +6494,7 @@
         <v>287341.69527999999</v>
       </c>
     </row>
-    <row r="46" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>44</v>
       </c>
@@ -6748,7 +6568,7 @@
         <v>40207.339999999997</v>
       </c>
     </row>
-    <row r="47" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>45</v>
       </c>
@@ -6822,7 +6642,7 @@
         <v>353269</v>
       </c>
     </row>
-    <row r="48" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>46</v>
       </c>
@@ -6896,7 +6716,7 @@
         <v>664773.17561999999</v>
       </c>
     </row>
-    <row r="49" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>47</v>
       </c>
@@ -6970,7 +6790,7 @@
         <v>96536.639999999999</v>
       </c>
     </row>
-    <row r="50" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>48</v>
       </c>
@@ -7044,7 +6864,7 @@
         <v>17157</v>
       </c>
     </row>
-    <row r="51" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>49</v>
       </c>
@@ -7118,7 +6938,7 @@
         <v>3257267.9736270001</v>
       </c>
     </row>
-    <row r="52" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>50</v>
       </c>
@@ -7192,7 +7012,7 @@
         <v>1926145.1587739999</v>
       </c>
     </row>
-    <row r="53" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>51</v>
       </c>
@@ -7266,7 +7086,7 @@
         <v>4796879.8973519998</v>
       </c>
     </row>
-    <row r="54" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>52</v>
       </c>
@@ -7349,18 +7169,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74073812-F58D-4768-AC11-644789E06262}">
   <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>70</v>
       </c>
@@ -7371,7 +7191,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>74</v>
       </c>
@@ -7382,7 +7202,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -7393,7 +7213,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -7404,7 +7224,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -7415,7 +7235,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -7426,7 +7246,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -7437,7 +7257,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -7448,7 +7268,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -7459,7 +7279,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>25</v>
       </c>
@@ -7470,7 +7290,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -7481,7 +7301,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -7492,7 +7312,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>31</v>
       </c>
@@ -7503,7 +7323,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>33</v>
       </c>
@@ -7514,7 +7334,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>35</v>
       </c>
@@ -7525,7 +7345,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>37</v>
       </c>
@@ -7536,7 +7356,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>39</v>
       </c>
@@ -7544,7 +7364,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>41</v>
       </c>
@@ -7555,7 +7375,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>43</v>
       </c>
@@ -7566,7 +7386,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>85</v>
       </c>
@@ -7577,7 +7397,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>45</v>
       </c>
@@ -7588,7 +7408,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>47</v>
       </c>
@@ -7599,7 +7419,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>49</v>
       </c>
@@ -7610,7 +7430,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>51</v>
       </c>
@@ -7621,7 +7441,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>53</v>
       </c>
@@ -7632,7 +7452,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>55</v>
       </c>
@@ -7643,7 +7463,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>57</v>
       </c>
@@ -7654,7 +7474,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>59</v>
       </c>
@@ -7665,7 +7485,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>61</v>
       </c>
@@ -7676,7 +7496,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>76</v>
       </c>
@@ -7700,15 +7520,15 @@
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.85546875" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.88671875" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>70</v>
       </c>
@@ -7722,7 +7542,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -7733,7 +7553,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -7744,7 +7564,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -7755,7 +7575,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -7769,7 +7589,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -7780,7 +7600,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -7791,7 +7611,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -7802,7 +7622,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -7813,7 +7633,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -7824,7 +7644,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -7835,7 +7655,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>31</v>
       </c>
@@ -7846,7 +7666,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>33</v>
       </c>
@@ -7857,7 +7677,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>35</v>
       </c>
@@ -7868,7 +7688,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>37</v>
       </c>
@@ -7879,7 +7699,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>39</v>
       </c>
@@ -7887,7 +7707,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>41</v>
       </c>
@@ -7898,7 +7718,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>43</v>
       </c>
@@ -7909,7 +7729,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>45</v>
       </c>
@@ -7920,7 +7740,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>47</v>
       </c>
@@ -7931,7 +7751,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>49</v>
       </c>
@@ -7942,7 +7762,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>51</v>
       </c>
@@ -7953,7 +7773,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>53</v>
       </c>
@@ -7964,7 +7784,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>55</v>
       </c>
@@ -7975,7 +7795,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>57</v>
       </c>
@@ -7986,7 +7806,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>59</v>
       </c>
@@ -7997,7 +7817,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>61</v>
       </c>
@@ -8008,7 +7828,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>76</v>
       </c>
@@ -8030,12 +7850,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -8043,7 +7863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>10</v>
       </c>
@@ -8051,7 +7871,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>9</v>
       </c>
@@ -8059,7 +7879,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>8</v>
       </c>
@@ -8067,7 +7887,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>7</v>
       </c>
@@ -8075,7 +7895,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>6</v>
       </c>
@@ -8083,7 +7903,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -8091,7 +7911,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>4</v>
       </c>
@@ -8099,7 +7919,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>3</v>
       </c>
@@ -8107,7 +7927,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2</v>
       </c>
@@ -8115,7 +7935,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1</v>
       </c>
@@ -8131,9 +7951,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>66</v>
       </c>
@@ -8141,7 +7961,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -8149,7 +7969,7 @@
         <v>-3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -8157,7 +7977,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -8165,7 +7985,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>67</v>
       </c>
@@ -8184,9 +8004,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -8194,7 +8014,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -8202,7 +8022,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -8210,7 +8030,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -8218,7 +8038,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -8237,14 +8057,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>64</v>
       </c>
@@ -8258,7 +8078,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>74</v>
       </c>
@@ -8272,7 +8092,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -8286,7 +8106,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -8300,7 +8120,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -8314,7 +8134,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -8328,7 +8148,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -8342,7 +8162,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -8356,7 +8176,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -8370,7 +8190,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -8384,7 +8204,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -8398,7 +8218,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>33</v>
       </c>
@@ -8412,7 +8232,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -8426,7 +8246,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>37</v>
       </c>
@@ -8440,7 +8260,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>39</v>
       </c>
@@ -8454,7 +8274,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>41</v>
       </c>
@@ -8468,7 +8288,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>43</v>
       </c>
@@ -8482,7 +8302,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>45</v>
       </c>
@@ -8496,7 +8316,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>47</v>
       </c>
@@ -8510,7 +8330,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>49</v>
       </c>
@@ -8524,7 +8344,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>51</v>
       </c>
@@ -8538,7 +8358,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>53</v>
       </c>
@@ -8552,7 +8372,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>55</v>
       </c>
@@ -8566,7 +8386,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>57</v>
       </c>
@@ -8580,7 +8400,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>59</v>
       </c>
@@ -8594,7 +8414,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>75</v>
       </c>
@@ -8619,15 +8439,15 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>64</v>
       </c>
@@ -8641,7 +8461,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>74</v>
       </c>
@@ -8655,7 +8475,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -8669,7 +8489,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -8683,7 +8503,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -8697,7 +8517,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -8711,7 +8531,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -8725,7 +8545,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -8739,7 +8559,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -8753,7 +8573,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -8767,7 +8587,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -8781,7 +8601,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>33</v>
       </c>
@@ -8795,7 +8615,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -8809,7 +8629,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>37</v>
       </c>
@@ -8823,7 +8643,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>39</v>
       </c>
@@ -8837,7 +8657,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>41</v>
       </c>
@@ -8851,7 +8671,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>43</v>
       </c>
@@ -8865,7 +8685,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>45</v>
       </c>
@@ -8879,7 +8699,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>47</v>
       </c>
@@ -8893,7 +8713,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>49</v>
       </c>
@@ -8907,7 +8727,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>51</v>
       </c>
@@ -8921,7 +8741,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>53</v>
       </c>
@@ -8935,7 +8755,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>55</v>
       </c>
@@ -8949,7 +8769,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>57</v>
       </c>
@@ -8963,7 +8783,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>59</v>
       </c>
@@ -8977,7 +8797,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>75</v>
       </c>
@@ -9002,14 +8822,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>64</v>
       </c>
@@ -9023,7 +8843,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>74</v>
       </c>
@@ -9037,7 +8857,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -9051,7 +8871,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -9065,7 +8885,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -9079,7 +8899,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -9093,7 +8913,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -9107,7 +8927,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -9121,7 +8941,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -9135,7 +8955,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -9149,7 +8969,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -9163,7 +8983,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>33</v>
       </c>
@@ -9177,7 +8997,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -9191,7 +9011,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>37</v>
       </c>
@@ -9205,7 +9025,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>39</v>
       </c>
@@ -9219,7 +9039,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>41</v>
       </c>
@@ -9233,7 +9053,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>43</v>
       </c>
@@ -9247,7 +9067,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>45</v>
       </c>
@@ -9261,7 +9081,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>47</v>
       </c>
@@ -9275,7 +9095,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>49</v>
       </c>
@@ -9289,7 +9109,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>51</v>
       </c>
@@ -9303,7 +9123,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>53</v>
       </c>
@@ -9317,7 +9137,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>55</v>
       </c>
@@ -9331,7 +9151,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>57</v>
       </c>
@@ -9345,7 +9165,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>59</v>
       </c>
@@ -9359,7 +9179,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>75</v>
       </c>

</xml_diff>

<commit_message>
Add in TFB01 and THR02 in station lookup table
We are now combining all available data in a watershed, not just the most downstream station
</commit_message>
<xml_diff>
--- a/data/lookup_tables.xlsx
+++ b/data/lookup_tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\srucker\Git\SCI\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A8450DC-B6E6-4432-8E9F-37223AB51ADF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBDC4500-55F7-417D-B301-1BEB243CD2B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" firstSheet="5" activeTab="6" xr2:uid="{23697FDE-567D-4570-AE33-F8F65584BB36}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{23697FDE-567D-4570-AE33-F8F65584BB36}"/>
   </bookViews>
   <sheets>
     <sheet name="location_id" sheetId="7" r:id="rId1"/>
@@ -28,6 +28,9 @@
     <sheet name="eia_score" sheetId="16" r:id="rId13"/>
     <sheet name="eia_2023_TEMP" sheetId="15" r:id="rId14"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="13" hidden="1">eia_2023_TEMP!$K$2:$R$54</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -49,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1340" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1347" uniqueCount="139">
   <si>
     <t>max_sites_per_mile</t>
   </si>
@@ -451,16 +454,49 @@
   </si>
   <si>
     <t>We decided to combine all data available in awatershed. Does that include for Rock Creek too? That would mean fo r Rock Creek subsheds, data would be used both for the subshed and Rock Creek</t>
+  </si>
+  <si>
+    <t>subshed_sf</t>
+  </si>
+  <si>
+    <t>impervious_sf</t>
+  </si>
+  <si>
+    <t>imp_treated_sf</t>
+  </si>
+  <si>
+    <t>TFB02</t>
+  </si>
+  <si>
+    <t>THR02</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -489,14 +525,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -809,10 +849,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8059EA70-FEB1-4761-8449-3A8139D2BAE4}">
-  <dimension ref="A1:B29"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q17" sqref="Q17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -895,161 +935,177 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>137</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B13" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B14" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B15" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>40</v>
+        <v>138</v>
       </c>
       <c r="B16" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B17" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B18" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B19" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B20" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B21" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B22" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B23" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B24" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B25" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B26" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B27" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="B28" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
+        <v>62</v>
+      </c>
+      <c r="B29" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>68</v>
+      </c>
+      <c r="B30" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
         <v>67</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B31" t="s">
         <v>75</v>
       </c>
     </row>
@@ -1441,7 +1497,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5527F1A5-7D36-461C-966C-101E89F52B4E}">
   <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1451,8 +1509,9 @@
     <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="42.109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2437,9 +2496,11 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FCF3A67-4696-4690-90E1-1249EF121DBC}">
-  <dimension ref="A1:L18"/>
+  <dimension ref="A1:O18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2447,15 +2508,18 @@
     <col min="2" max="3" width="25.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="41.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.33203125" customWidth="1"/>
+    <col min="7" max="7" width="23.33203125" customWidth="1"/>
+    <col min="8" max="8" width="30.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.6640625" customWidth="1"/>
+    <col min="10" max="10" width="19.21875" customWidth="1"/>
     <col min="11" max="11" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="27.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.6640625" customWidth="1"/>
+    <col min="14" max="15" width="13.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>131</v>
       </c>
@@ -2492,8 +2556,17 @@
       <c r="L1" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M1" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>73</v>
       </c>
@@ -2528,8 +2601,20 @@
         <f>VLOOKUP(E2,eia_2023_TEMP!$W$3:$AA$54,5,FALSE)</f>
         <v>4796879.8973519998</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M2" s="3">
+        <f>F2*10.7639</f>
+        <v>102954268.64044008</v>
+      </c>
+      <c r="N2" s="3">
+        <f t="shared" ref="N2:O2" si="0">G2*10.7639</f>
+        <v>55238809.993116289</v>
+      </c>
+      <c r="O2" s="3">
+        <f t="shared" si="0"/>
+        <v>51633135.527107187</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>73</v>
       </c>
@@ -2543,7 +2628,7 @@
         <v>91</v>
       </c>
       <c r="E3" t="str">
-        <f t="shared" ref="E3:E18" si="0">B3 &amp;" - "&amp;D3&amp;" - "&amp;C3</f>
+        <f t="shared" ref="E3:E18" si="1">B3 &amp;" - "&amp;D3&amp;" - "&amp;C3</f>
         <v>Rock Creek - CSS - Rock Creek</v>
       </c>
       <c r="F3">
@@ -2564,8 +2649,20 @@
         <f>VLOOKUP(E3,eia_2023_TEMP!$W$3:$AA$54,5,FALSE)</f>
         <v>3257267.9736270001</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M3" s="3">
+        <f t="shared" ref="M3:M18" si="2">F3*10.7639</f>
+        <v>69836315.795694157</v>
+      </c>
+      <c r="N3" s="3">
+        <f t="shared" ref="N3:N18" si="3">G3*10.7639</f>
+        <v>49918964.170099445</v>
+      </c>
+      <c r="O3" s="3">
+        <f t="shared" ref="O3:O18" si="4">H3*10.7639</f>
+        <v>35060906.741323665</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>73</v>
       </c>
@@ -2579,7 +2676,7 @@
         <v>89</v>
       </c>
       <c r="E4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Rock Creek - MS4 - Rock Creek</v>
       </c>
       <c r="F4">
@@ -2600,8 +2697,20 @@
         <f>VLOOKUP(E4,eia_2023_TEMP!$W$3:$AA$54,5,FALSE)</f>
         <v>1926145.1587739999</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M4" s="3">
+        <f t="shared" si="2"/>
+        <v>98466785.054549903</v>
+      </c>
+      <c r="N4" s="3">
+        <f t="shared" si="3"/>
+        <v>19802045.308608543</v>
+      </c>
+      <c r="O4" s="3">
+        <f t="shared" si="4"/>
+        <v>20732833.874527458</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>73</v>
       </c>
@@ -2615,7 +2724,7 @@
         <v>89</v>
       </c>
       <c r="E5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Rock Creek - MS4 - Piney Branch</v>
       </c>
       <c r="F5">
@@ -2636,8 +2745,20 @@
         <f>VLOOKUP(E5,eia_2023_TEMP!$W$3:$AA$54,5,FALSE)</f>
         <v>96536.639999999999</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M5" s="3">
+        <f t="shared" si="2"/>
+        <v>6924367.8393698735</v>
+      </c>
+      <c r="N5" s="3">
+        <f t="shared" si="3"/>
+        <v>2044592.8622564033</v>
+      </c>
+      <c r="O5" s="3">
+        <f t="shared" si="4"/>
+        <v>1039110.739296</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>73</v>
       </c>
@@ -2651,7 +2772,7 @@
         <v>89</v>
       </c>
       <c r="E6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Rock Creek - MS4 - Klingle Valley Run</v>
       </c>
       <c r="F6">
@@ -2672,8 +2793,20 @@
         <f>VLOOKUP(E6,eia_2023_TEMP!$W$3:$AA$54,5,FALSE)</f>
         <v>365082.01527999999</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M6" s="3">
+        <f t="shared" si="2"/>
+        <v>7485883.3067554366</v>
+      </c>
+      <c r="N6" s="3">
+        <f t="shared" si="3"/>
+        <v>2820711.9128589891</v>
+      </c>
+      <c r="O6" s="3">
+        <f t="shared" si="4"/>
+        <v>3929706.3042723918</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>73</v>
       </c>
@@ -2687,7 +2820,7 @@
         <v>89</v>
       </c>
       <c r="E7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Rock Creek - MS4 - Soapstone Creek</v>
       </c>
       <c r="F7">
@@ -2708,8 +2841,20 @@
         <f>VLOOKUP(E7,eia_2023_TEMP!$W$3:$AA$54,5,FALSE)</f>
         <v>1113950.1399999999</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M7" s="3">
+        <f t="shared" si="2"/>
+        <v>22493267.358961131</v>
+      </c>
+      <c r="N7" s="3">
+        <f t="shared" si="3"/>
+        <v>10104122.319692302</v>
+      </c>
+      <c r="O7" s="3">
+        <f t="shared" si="4"/>
+        <v>11990447.911945999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>73</v>
       </c>
@@ -2723,7 +2868,7 @@
         <v>89</v>
       </c>
       <c r="E8" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Rock Creek - MS4 - Melvin Hazen Valley Branch</v>
       </c>
       <c r="F8">
@@ -2744,8 +2889,20 @@
         <f>VLOOKUP(E8,eia_2023_TEMP!$W$3:$AA$54,5,FALSE)</f>
         <v>287341.69527999999</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M8" s="3">
+        <f t="shared" si="2"/>
+        <v>7593641.7658308325</v>
+      </c>
+      <c r="N8" s="3">
+        <f t="shared" si="3"/>
+        <v>2606850.9993030364</v>
+      </c>
+      <c r="O8" s="3">
+        <f t="shared" si="4"/>
+        <v>3092917.2738243919</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>73</v>
       </c>
@@ -2759,7 +2916,7 @@
         <v>89</v>
       </c>
       <c r="E9" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Rock Creek - MS4 - Fenwick Branch</v>
       </c>
       <c r="F9">
@@ -2780,8 +2937,20 @@
         <f>VLOOKUP(E9,eia_2023_TEMP!$W$3:$AA$54,5,FALSE)</f>
         <v>100035.041018</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M9" s="3">
+        <f t="shared" si="2"/>
+        <v>9618301.0132363159</v>
+      </c>
+      <c r="N9" s="3">
+        <f t="shared" si="3"/>
+        <v>3062834.3398283641</v>
+      </c>
+      <c r="O9" s="3">
+        <f t="shared" si="4"/>
+        <v>1076767.1780136502</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>73</v>
       </c>
@@ -2795,7 +2964,7 @@
         <v>89</v>
       </c>
       <c r="E10" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Rock Creek - MS4 - Portal Branch</v>
       </c>
       <c r="F10">
@@ -2816,8 +2985,20 @@
         <f>VLOOKUP(E10,eia_2023_TEMP!$W$3:$AA$54,5,FALSE)</f>
         <v>17157</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M10" s="3">
+        <f t="shared" si="2"/>
+        <v>3112114.49119259</v>
+      </c>
+      <c r="N10" s="3">
+        <f t="shared" si="3"/>
+        <v>955107.1947344892</v>
+      </c>
+      <c r="O10" s="3">
+        <f t="shared" si="4"/>
+        <v>184676.2323</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>73</v>
       </c>
@@ -2831,7 +3012,7 @@
         <v>89</v>
       </c>
       <c r="E11" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Rock Creek - MS4 - Luzon Branch</v>
       </c>
       <c r="F11">
@@ -2852,8 +3033,20 @@
         <f>VLOOKUP(E11,eia_2023_TEMP!$W$3:$AA$54,5,FALSE)</f>
         <v>943535.51400199998</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M11" s="3">
+        <f t="shared" si="2"/>
+        <v>28032155.584225256</v>
+      </c>
+      <c r="N11" s="3">
+        <f t="shared" si="3"/>
+        <v>13120277.754532568</v>
+      </c>
+      <c r="O11" s="3">
+        <f t="shared" si="4"/>
+        <v>10156121.919166127</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>73</v>
       </c>
@@ -2867,7 +3060,7 @@
         <v>89</v>
       </c>
       <c r="E12" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Rock Creek - MS4 - Pinehurst Branch</v>
       </c>
       <c r="F12">
@@ -2888,8 +3081,20 @@
         <f>VLOOKUP(E12,eia_2023_TEMP!$W$3:$AA$54,5,FALSE)</f>
         <v>664773.17561999999</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M12" s="3">
+        <f t="shared" si="2"/>
+        <v>19573676.777167626</v>
+      </c>
+      <c r="N12" s="3">
+        <f t="shared" si="3"/>
+        <v>4243937.1085025333</v>
+      </c>
+      <c r="O12" s="3">
+        <f t="shared" si="4"/>
+        <v>7155551.9850561181</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>73</v>
       </c>
@@ -2903,7 +3108,7 @@
         <v>89</v>
       </c>
       <c r="E13" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Rock Creek - MS4 - Bingham Run</v>
       </c>
       <c r="F13">
@@ -2924,8 +3129,20 @@
         <f>VLOOKUP(E13,eia_2023_TEMP!$W$3:$AA$54,5,FALSE)</f>
         <v>379316.2</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M13" s="3">
+        <f t="shared" si="2"/>
+        <v>7260169.3516161824</v>
+      </c>
+      <c r="N13" s="3">
+        <f t="shared" si="3"/>
+        <v>1374354.2781989756</v>
+      </c>
+      <c r="O13" s="3">
+        <f t="shared" si="4"/>
+        <v>4082921.64518</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>73</v>
       </c>
@@ -2939,7 +3156,7 @@
         <v>89</v>
       </c>
       <c r="E14" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Rock Creek - MS4 - Broad Branch</v>
       </c>
       <c r="F14">
@@ -2960,8 +3177,20 @@
         <f>VLOOKUP(E14,eia_2023_TEMP!$W$3:$AA$54,5,FALSE)</f>
         <v>1117618.041373</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M14" s="3">
+        <f t="shared" si="2"/>
+        <v>50026467.955882095</v>
+      </c>
+      <c r="N14" s="3">
+        <f t="shared" si="3"/>
+        <v>17521868.042866062</v>
+      </c>
+      <c r="O14" s="3">
+        <f t="shared" si="4"/>
+        <v>12029928.835534835</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>73</v>
       </c>
@@ -2975,7 +3204,7 @@
         <v>89</v>
       </c>
       <c r="E15" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Rock Creek - MS4 - Milkhouse Run</v>
       </c>
       <c r="F15">
@@ -2996,8 +3225,20 @@
         <f>VLOOKUP(E15,eia_2023_TEMP!$W$3:$AA$54,5,FALSE)</f>
         <v>40207.339999999997</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M15" s="3">
+        <f t="shared" si="2"/>
+        <v>2877121.8564989651</v>
+      </c>
+      <c r="N15" s="3">
+        <f t="shared" si="3"/>
+        <v>615038.05919713282</v>
+      </c>
+      <c r="O15" s="3">
+        <f t="shared" si="4"/>
+        <v>432787.78702599992</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>73</v>
       </c>
@@ -3011,7 +3252,7 @@
         <v>89</v>
       </c>
       <c r="E16" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Rock Creek - MS4 - Normanstone Creek</v>
       </c>
       <c r="F16">
@@ -3032,8 +3273,20 @@
         <f>VLOOKUP(E16,eia_2023_TEMP!$W$3:$AA$54,5,FALSE)</f>
         <v>353269</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="M16" s="3">
+        <f t="shared" si="2"/>
+        <v>9486436.5269554295</v>
+      </c>
+      <c r="N16" s="3">
+        <f t="shared" si="3"/>
+        <v>3696813.0731316544</v>
+      </c>
+      <c r="O16" s="3">
+        <f t="shared" si="4"/>
+        <v>3802552.1891000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>73</v>
       </c>
@@ -3047,7 +3300,7 @@
         <v>89</v>
       </c>
       <c r="E17" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Rock Creek - MS4 - Dumbarton Oaks</v>
       </c>
       <c r="F17">
@@ -3068,8 +3321,20 @@
         <f>VLOOKUP(E17,eia_2023_TEMP!$W$3:$AA$54,5,FALSE)</f>
         <v>141034.4</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="M17" s="3">
+        <f t="shared" si="2"/>
+        <v>5927346.3455916252</v>
+      </c>
+      <c r="N17" s="3">
+        <f t="shared" si="3"/>
+        <v>1650497.1020503798</v>
+      </c>
+      <c r="O17" s="3">
+        <f t="shared" si="4"/>
+        <v>1518080.1781599999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>73</v>
       </c>
@@ -3083,7 +3348,7 @@
         <v>89</v>
       </c>
       <c r="E18" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Rock Creek - MS4 - Blagden Run</v>
       </c>
       <c r="F18">
@@ -3103,6 +3368,18 @@
       <c r="J18">
         <f>VLOOKUP(E18,eia_2023_TEMP!$W$3:$AA$54,5,FALSE)</f>
         <v>387046.12</v>
+      </c>
+      <c r="M18" s="3">
+        <f t="shared" si="2"/>
+        <v>8877133.8801231608</v>
+      </c>
+      <c r="N18" s="3">
+        <f t="shared" si="3"/>
+        <v>3002010.5346595799</v>
+      </c>
+      <c r="O18" s="3">
+        <f t="shared" si="4"/>
+        <v>4166125.7310679997</v>
       </c>
     </row>
   </sheetData>
@@ -3215,10 +3492,11 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9958D10-7702-442F-9409-F4700B4DEC04}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:AA54"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="V20" sqref="V20:V21"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="P63" sqref="P63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3311,7 +3589,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:27" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3385,7 +3663,7 @@
         <v>22372585.52138</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:27" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -3459,7 +3737,7 @@
         <v>12287324.88528</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:27" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -3533,7 +3811,7 @@
         <v>2029942.3796260001</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:27" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -3607,7 +3885,7 @@
         <v>116119.34</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:27" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -3681,7 +3959,7 @@
         <v>1537111.8</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:27" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -3755,7 +4033,7 @@
         <v>184753.5</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:27" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -3829,7 +4107,7 @@
         <v>452698.47252000001</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:27" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -3903,7 +4181,7 @@
         <v>5428279.8678000001</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:27" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
@@ -3977,7 +4255,7 @@
         <v>150542.92154400001</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:27" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
@@ -4051,7 +4329,7 @@
         <v>768027.46</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:27" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
@@ -4125,7 +4403,7 @@
         <v>237072.41034</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:27" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
@@ -4199,7 +4477,7 @@
         <v>177741.03056000001</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:27" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
@@ -4273,7 +4551,7 @@
         <v>1001244.8</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:27" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
@@ -4347,7 +4625,7 @@
         <v>17219627.360909998</v>
       </c>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:27" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15</v>
       </c>
@@ -4421,7 +4699,7 @@
         <v>1394451.68</v>
       </c>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:27" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>16</v>
       </c>
@@ -4495,7 +4773,7 @@
         <v>58224</v>
       </c>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:27" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>17</v>
       </c>
@@ -4569,7 +4847,7 @@
         <v>707857.25361599994</v>
       </c>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:27" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>18</v>
       </c>
@@ -4643,7 +4921,7 @@
         <v>3904344.6596829998</v>
       </c>
     </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:27" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>19</v>
       </c>
@@ -4717,7 +4995,7 @@
         <v>108168.17</v>
       </c>
     </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:27" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>20</v>
       </c>
@@ -4791,7 +5069,7 @@
         <v>1023406.87528</v>
       </c>
     </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:27" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>21</v>
       </c>
@@ -4865,7 +5143,7 @@
         <v>1867917.21056</v>
       </c>
     </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:27" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>22</v>
       </c>
@@ -4939,7 +5217,7 @@
         <v>1911943.256325</v>
       </c>
     </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:27" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>23</v>
       </c>
@@ -5013,7 +5291,7 @@
         <v>380435</v>
       </c>
     </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:27" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>24</v>
       </c>
@@ -5087,7 +5365,7 @@
         <v>1454945.14056</v>
       </c>
     </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:27" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>25</v>
       </c>
@@ -5161,7 +5439,7 @@
         <v>255414</v>
       </c>
     </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:27" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>26</v>
       </c>
@@ -5235,7 +5513,7 @@
         <v>2619097.3403039998</v>
       </c>
     </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:27" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>27</v>
       </c>
@@ -5309,7 +5587,7 @@
         <v>5103945.4106769999</v>
       </c>
     </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:27" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>28</v>
       </c>
@@ -5383,7 +5661,7 @@
         <v>4741171.750461</v>
       </c>
     </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:27" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>29</v>
       </c>
@@ -5457,7 +5735,7 @@
         <v>4464167.6281199995</v>
       </c>
     </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:27" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>30</v>
       </c>
@@ -5531,7 +5809,7 @@
         <v>808390.92652600002</v>
       </c>
     </row>
-    <row r="33" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:27" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>31</v>
       </c>
@@ -5605,7 +5883,7 @@
         <v>1568704</v>
       </c>
     </row>
-    <row r="34" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:27" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>32</v>
       </c>
@@ -5679,7 +5957,7 @@
         <v>212133.691238</v>
       </c>
     </row>
-    <row r="35" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:27" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>33</v>
       </c>
@@ -5753,7 +6031,7 @@
         <v>27529</v>
       </c>
     </row>
-    <row r="36" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:27" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>34</v>
       </c>
@@ -5827,7 +6105,7 @@
         <v>380525.64</v>
       </c>
     </row>
-    <row r="37" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:27" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>35</v>
       </c>
@@ -7160,6 +7438,13 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="K2:R54" xr:uid="{A9958D10-7702-442F-9409-F4700B4DEC04}">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="Rock Creek"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -8054,8 +8339,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B281CBBA-5423-42AE-9693-0C69866CF5CE}">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Add data filter for trash and dumpsite functions
</commit_message>
<xml_diff>
--- a/data/lookup_tables.xlsx
+++ b/data/lookup_tables.xlsx
@@ -8,28 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\srucker\Git\SCI\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBDC4500-55F7-417D-B301-1BEB243CD2B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9216B83E-AC55-4F2D-9FE4-B5F56D2CA152}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{23697FDE-567D-4570-AE33-F8F65584BB36}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{23697FDE-567D-4570-AE33-F8F65584BB36}"/>
   </bookViews>
   <sheets>
-    <sheet name="location_id" sheetId="7" r:id="rId1"/>
+    <sheet name="location_id" sheetId="19" r:id="rId1"/>
     <sheet name="location_name" sheetId="18" r:id="rId2"/>
-    <sheet name="sci_subshed " sheetId="17" r:id="rId3"/>
-    <sheet name="dumpsite_score" sheetId="1" r:id="rId4"/>
-    <sheet name="dumpsite_weight" sheetId="2" r:id="rId5"/>
-    <sheet name="trash_score" sheetId="3" r:id="rId6"/>
-    <sheet name="connectivity_summary" sheetId="4" r:id="rId7"/>
-    <sheet name="fish_summary" sheetId="8" r:id="rId8"/>
-    <sheet name="habitat_summary" sheetId="11" r:id="rId9"/>
-    <sheet name="macroinvertebrate_summary" sheetId="12" r:id="rId10"/>
-    <sheet name="eia_subsheds" sheetId="13" r:id="rId11"/>
-    <sheet name="eia_rock_creek" sheetId="14" r:id="rId12"/>
-    <sheet name="eia_score" sheetId="16" r:id="rId13"/>
-    <sheet name="eia_2023_TEMP" sheetId="15" r:id="rId14"/>
+    <sheet name="dumpsite_score" sheetId="1" r:id="rId3"/>
+    <sheet name="dumpsite_weight" sheetId="2" r:id="rId4"/>
+    <sheet name="trash_score" sheetId="3" r:id="rId5"/>
+    <sheet name="connectivity_summary" sheetId="4" r:id="rId6"/>
+    <sheet name="fish_summary" sheetId="8" r:id="rId7"/>
+    <sheet name="habitat_summary" sheetId="11" r:id="rId8"/>
+    <sheet name="macroinvertebrate_summary" sheetId="12" r:id="rId9"/>
+    <sheet name="eia_subsheds" sheetId="13" r:id="rId10"/>
+    <sheet name="eia_rock_creek" sheetId="14" r:id="rId11"/>
+    <sheet name="eia_score" sheetId="16" r:id="rId12"/>
+    <sheet name="eia_2023_TEMP" sheetId="15" r:id="rId13"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="13" hidden="1">eia_2023_TEMP!$K$2:$R$54</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">eia_2023_TEMP!$K$2:$R$54</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -52,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1347" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1262" uniqueCount="137">
   <si>
     <t>max_sites_per_mile</t>
   </si>
@@ -448,12 +447,6 @@
   </si>
   <si>
     <t>sci_subshed</t>
-  </si>
-  <si>
-    <t>sci_watershed</t>
-  </si>
-  <si>
-    <t>We decided to combine all data available in awatershed. Does that include for Rock Creek too? That would mean fo r Rock Creek subsheds, data would be used both for the subshed and Rock Creek</t>
   </si>
   <si>
     <t>subshed_sf</t>
@@ -477,7 +470,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -533,7 +526,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -848,20 +841,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8059EA70-FEB1-4761-8449-3A8139D2BAE4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35A9A15C-8D95-4037-950D-70E415250836}">
   <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q17" sqref="Q17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>63</v>
       </c>
@@ -869,7 +862,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -877,7 +870,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -885,7 +878,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -893,7 +886,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -901,7 +894,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -909,7 +902,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -917,7 +910,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -925,7 +918,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -933,15 +926,15 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B10" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -949,7 +942,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>30</v>
       </c>
@@ -957,7 +950,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>32</v>
       </c>
@@ -965,7 +958,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>34</v>
       </c>
@@ -973,7 +966,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>36</v>
       </c>
@@ -981,15 +974,15 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B16" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>38</v>
       </c>
@@ -997,7 +990,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>40</v>
       </c>
@@ -1005,7 +998,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>42</v>
       </c>
@@ -1013,7 +1006,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>44</v>
       </c>
@@ -1021,7 +1014,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>46</v>
       </c>
@@ -1029,7 +1022,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>48</v>
       </c>
@@ -1037,7 +1030,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>50</v>
       </c>
@@ -1045,7 +1038,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>52</v>
       </c>
@@ -1053,7 +1046,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>54</v>
       </c>
@@ -1061,7 +1054,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>56</v>
       </c>
@@ -1069,7 +1062,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>58</v>
       </c>
@@ -1077,7 +1070,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>60</v>
       </c>
@@ -1085,7 +1078,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>62</v>
       </c>
@@ -1093,7 +1086,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>68</v>
       </c>
@@ -1101,7 +1094,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>67</v>
       </c>
@@ -1115,385 +1108,6 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{200F6E0C-51C0-4CFC-8295-6BC9A0CB5165}">
-  <dimension ref="A1:D26"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="25.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>131</v>
-      </c>
-      <c r="B1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C1" t="s">
-        <v>79</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2">
-        <v>6.86</v>
-      </c>
-      <c r="D2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3">
-        <v>5.28</v>
-      </c>
-      <c r="D3">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4">
-        <v>6.41</v>
-      </c>
-      <c r="D4">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5">
-        <v>5.88</v>
-      </c>
-      <c r="D5">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6">
-        <v>5</v>
-      </c>
-      <c r="D6">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7">
-        <v>6.24</v>
-      </c>
-      <c r="D7">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9">
-        <v>9.14</v>
-      </c>
-      <c r="D9">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10" t="s">
-        <v>30</v>
-      </c>
-      <c r="C10">
-        <v>7.39</v>
-      </c>
-      <c r="D10">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B11" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11">
-        <v>6.28</v>
-      </c>
-      <c r="D11">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>33</v>
-      </c>
-      <c r="B12" t="s">
-        <v>34</v>
-      </c>
-      <c r="C12">
-        <v>5.39</v>
-      </c>
-      <c r="D12">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>35</v>
-      </c>
-      <c r="B13" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13">
-        <v>7.9</v>
-      </c>
-      <c r="D13">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>37</v>
-      </c>
-      <c r="B14" t="s">
-        <v>38</v>
-      </c>
-      <c r="C14">
-        <v>5.99</v>
-      </c>
-      <c r="D14">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>39</v>
-      </c>
-      <c r="B15" t="s">
-        <v>40</v>
-      </c>
-      <c r="C15">
-        <v>6.49</v>
-      </c>
-      <c r="D15">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>41</v>
-      </c>
-      <c r="B16" t="s">
-        <v>42</v>
-      </c>
-      <c r="C16">
-        <v>5.32</v>
-      </c>
-      <c r="D16">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>43</v>
-      </c>
-      <c r="B17" t="s">
-        <v>44</v>
-      </c>
-      <c r="C17">
-        <v>8.06</v>
-      </c>
-      <c r="D17">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>84</v>
-      </c>
-      <c r="B18" t="s">
-        <v>46</v>
-      </c>
-      <c r="C18">
-        <v>5.88</v>
-      </c>
-      <c r="D18">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>47</v>
-      </c>
-      <c r="B19" t="s">
-        <v>48</v>
-      </c>
-      <c r="C19">
-        <v>7.67</v>
-      </c>
-      <c r="D19">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>49</v>
-      </c>
-      <c r="B20" t="s">
-        <v>50</v>
-      </c>
-      <c r="C20">
-        <v>4.45</v>
-      </c>
-      <c r="D20">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>51</v>
-      </c>
-      <c r="B21" t="s">
-        <v>52</v>
-      </c>
-      <c r="C21">
-        <v>6.82</v>
-      </c>
-      <c r="D21">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>53</v>
-      </c>
-      <c r="B22" t="s">
-        <v>54</v>
-      </c>
-      <c r="C22">
-        <v>5.93</v>
-      </c>
-      <c r="D22">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>55</v>
-      </c>
-      <c r="B23" t="s">
-        <v>56</v>
-      </c>
-      <c r="C23">
-        <v>7.6</v>
-      </c>
-      <c r="D23">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>57</v>
-      </c>
-      <c r="B24" t="s">
-        <v>58</v>
-      </c>
-      <c r="C24">
-        <v>6.22</v>
-      </c>
-      <c r="D24">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>59</v>
-      </c>
-      <c r="B25" t="s">
-        <v>60</v>
-      </c>
-      <c r="C25">
-        <v>9.3800000000000008</v>
-      </c>
-      <c r="D25">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>74</v>
-      </c>
-      <c r="B26" t="s">
-        <v>62</v>
-      </c>
-      <c r="C26">
-        <v>6.46</v>
-      </c>
-      <c r="D26">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5527F1A5-7D36-461C-966C-101E89F52B4E}">
   <dimension ref="A1:L27"/>
   <sheetViews>
@@ -1501,21 +1115,21 @@
       <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="42.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="27.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>131</v>
       </c>
@@ -1553,7 +1167,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -1589,7 +1203,7 @@
         <v>380435</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -1625,7 +1239,7 @@
         <v>1117618.041373</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -1661,7 +1275,7 @@
         <v>255414</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -1697,7 +1311,7 @@
         <v>141034.4</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>31</v>
       </c>
@@ -1733,7 +1347,7 @@
         <v>100035.041018</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>27</v>
       </c>
@@ -1769,7 +1383,7 @@
         <v>768027.46</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -1805,7 +1419,7 @@
         <v>237072.41034</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -1841,7 +1455,7 @@
         <v>177741.03056000001</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>33</v>
       </c>
@@ -1877,7 +1491,7 @@
         <v>1001244.8</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>25</v>
       </c>
@@ -1913,7 +1527,7 @@
         <v>2619097.3403039998</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>35</v>
       </c>
@@ -1949,7 +1563,7 @@
         <v>17219627.360909998</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>37</v>
       </c>
@@ -1985,7 +1599,7 @@
         <v>365082.01527999999</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>39</v>
       </c>
@@ -2021,7 +1635,7 @@
         <v>943535.51400199998</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>41</v>
       </c>
@@ -2057,7 +1671,7 @@
         <v>287341.69527999999</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>43</v>
       </c>
@@ -2093,7 +1707,7 @@
         <v>707857.25361599994</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>84</v>
       </c>
@@ -2129,7 +1743,7 @@
         <v>353269</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>47</v>
       </c>
@@ -2165,7 +1779,7 @@
         <v>5103945.4106769999</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>51</v>
       </c>
@@ -2201,7 +1815,7 @@
         <v>664773.17561999999</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>55</v>
       </c>
@@ -2237,7 +1851,7 @@
         <v>96536.639999999999</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>49</v>
       </c>
@@ -2273,7 +1887,7 @@
         <v>108168.17</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>53</v>
       </c>
@@ -2309,7 +1923,7 @@
         <v>17157</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>55</v>
       </c>
@@ -2345,7 +1959,7 @@
         <v>4796879.8973519998</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>57</v>
       </c>
@@ -2381,7 +1995,7 @@
         <v>1113950.1399999999</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>59</v>
       </c>
@@ -2417,7 +2031,7 @@
         <v>1023406.87528</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>74</v>
       </c>
@@ -2453,7 +2067,7 @@
         <v>1867917.21056</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>74</v>
       </c>
@@ -2494,7 +2108,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FCF3A67-4696-4690-90E1-1249EF121DBC}">
   <dimension ref="A1:O18"/>
   <sheetViews>
@@ -2502,24 +2116,24 @@
       <selection activeCell="E2" sqref="E2:E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="25.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="41.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.33203125" customWidth="1"/>
-    <col min="7" max="7" width="23.33203125" customWidth="1"/>
-    <col min="8" max="8" width="30.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.6640625" customWidth="1"/>
-    <col min="10" max="10" width="19.21875" customWidth="1"/>
-    <col min="11" max="11" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="27.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.6640625" customWidth="1"/>
-    <col min="14" max="15" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="41.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.28515625" customWidth="1"/>
+    <col min="7" max="7" width="23.28515625" customWidth="1"/>
+    <col min="8" max="8" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.7109375" customWidth="1"/>
+    <col min="10" max="10" width="19.28515625" customWidth="1"/>
+    <col min="11" max="11" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.7109375" customWidth="1"/>
+    <col min="14" max="15" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>131</v>
       </c>
@@ -2557,16 +2171,16 @@
         <v>129</v>
       </c>
       <c r="M1" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="O1" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="N1" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>73</v>
       </c>
@@ -2614,7 +2228,7 @@
         <v>51633135.527107187</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>73</v>
       </c>
@@ -2662,7 +2276,7 @@
         <v>35060906.741323665</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>73</v>
       </c>
@@ -2710,7 +2324,7 @@
         <v>20732833.874527458</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>73</v>
       </c>
@@ -2758,7 +2372,7 @@
         <v>1039110.739296</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>73</v>
       </c>
@@ -2806,7 +2420,7 @@
         <v>3929706.3042723918</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>73</v>
       </c>
@@ -2854,7 +2468,7 @@
         <v>11990447.911945999</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>73</v>
       </c>
@@ -2902,7 +2516,7 @@
         <v>3092917.2738243919</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>73</v>
       </c>
@@ -2950,7 +2564,7 @@
         <v>1076767.1780136502</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>73</v>
       </c>
@@ -2998,7 +2612,7 @@
         <v>184676.2323</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>73</v>
       </c>
@@ -3046,7 +2660,7 @@
         <v>10156121.919166127</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>73</v>
       </c>
@@ -3094,7 +2708,7 @@
         <v>7155551.9850561181</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>73</v>
       </c>
@@ -3142,7 +2756,7 @@
         <v>4082921.64518</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>73</v>
       </c>
@@ -3190,7 +2804,7 @@
         <v>12029928.835534835</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>73</v>
       </c>
@@ -3238,7 +2852,7 @@
         <v>432787.78702599992</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>73</v>
       </c>
@@ -3286,7 +2900,7 @@
         <v>3802552.1891000001</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>73</v>
       </c>
@@ -3334,7 +2948,7 @@
         <v>1518080.1781599999</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>73</v>
       </c>
@@ -3387,7 +3001,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A15AB59E-477A-404D-9A36-733C66688157}">
   <dimension ref="A1:B11"/>
   <sheetViews>
@@ -3395,9 +3009,9 @@
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -3405,7 +3019,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>10</v>
       </c>
@@ -3413,7 +3027,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>9</v>
       </c>
@@ -3421,7 +3035,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>8</v>
       </c>
@@ -3429,7 +3043,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>7</v>
       </c>
@@ -3437,7 +3051,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>6</v>
       </c>
@@ -3445,7 +3059,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -3453,7 +3067,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4</v>
       </c>
@@ -3461,7 +3075,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>3</v>
       </c>
@@ -3469,7 +3083,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2</v>
       </c>
@@ -3477,7 +3091,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1</v>
       </c>
@@ -3490,7 +3104,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9958D10-7702-442F-9409-F4700B4DEC04}">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:AA54"/>
@@ -3499,18 +3113,18 @@
       <selection activeCell="P63" sqref="P63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="58" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="39" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="58" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="58" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>96</v>
       </c>
@@ -3518,7 +3132,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>97</v>
       </c>
@@ -3589,7 +3203,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="3" spans="1:27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3663,7 +3277,7 @@
         <v>22372585.52138</v>
       </c>
     </row>
-    <row r="4" spans="1:27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -3737,7 +3351,7 @@
         <v>12287324.88528</v>
       </c>
     </row>
-    <row r="5" spans="1:27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -3811,7 +3425,7 @@
         <v>2029942.3796260001</v>
       </c>
     </row>
-    <row r="6" spans="1:27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -3885,7 +3499,7 @@
         <v>116119.34</v>
       </c>
     </row>
-    <row r="7" spans="1:27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -3959,7 +3573,7 @@
         <v>1537111.8</v>
       </c>
     </row>
-    <row r="8" spans="1:27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -4033,7 +3647,7 @@
         <v>184753.5</v>
       </c>
     </row>
-    <row r="9" spans="1:27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -4107,7 +3721,7 @@
         <v>452698.47252000001</v>
       </c>
     </row>
-    <row r="10" spans="1:27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -4181,7 +3795,7 @@
         <v>5428279.8678000001</v>
       </c>
     </row>
-    <row r="11" spans="1:27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -4255,7 +3869,7 @@
         <v>150542.92154400001</v>
       </c>
     </row>
-    <row r="12" spans="1:27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -4329,7 +3943,7 @@
         <v>768027.46</v>
       </c>
     </row>
-    <row r="13" spans="1:27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -4403,7 +4017,7 @@
         <v>237072.41034</v>
       </c>
     </row>
-    <row r="14" spans="1:27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -4477,7 +4091,7 @@
         <v>177741.03056000001</v>
       </c>
     </row>
-    <row r="15" spans="1:27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -4551,7 +4165,7 @@
         <v>1001244.8</v>
       </c>
     </row>
-    <row r="16" spans="1:27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -4625,7 +4239,7 @@
         <v>17219627.360909998</v>
       </c>
     </row>
-    <row r="17" spans="1:27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
@@ -4699,7 +4313,7 @@
         <v>1394451.68</v>
       </c>
     </row>
-    <row r="18" spans="1:27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
@@ -4773,7 +4387,7 @@
         <v>58224</v>
       </c>
     </row>
-    <row r="19" spans="1:27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
@@ -4847,7 +4461,7 @@
         <v>707857.25361599994</v>
       </c>
     </row>
-    <row r="20" spans="1:27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
@@ -4921,7 +4535,7 @@
         <v>3904344.6596829998</v>
       </c>
     </row>
-    <row r="21" spans="1:27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
@@ -4995,7 +4609,7 @@
         <v>108168.17</v>
       </c>
     </row>
-    <row r="22" spans="1:27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20</v>
       </c>
@@ -5069,7 +4683,7 @@
         <v>1023406.87528</v>
       </c>
     </row>
-    <row r="23" spans="1:27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>21</v>
       </c>
@@ -5143,7 +4757,7 @@
         <v>1867917.21056</v>
       </c>
     </row>
-    <row r="24" spans="1:27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>22</v>
       </c>
@@ -5217,7 +4831,7 @@
         <v>1911943.256325</v>
       </c>
     </row>
-    <row r="25" spans="1:27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>23</v>
       </c>
@@ -5291,7 +4905,7 @@
         <v>380435</v>
       </c>
     </row>
-    <row r="26" spans="1:27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>24</v>
       </c>
@@ -5365,7 +4979,7 @@
         <v>1454945.14056</v>
       </c>
     </row>
-    <row r="27" spans="1:27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>25</v>
       </c>
@@ -5439,7 +5053,7 @@
         <v>255414</v>
       </c>
     </row>
-    <row r="28" spans="1:27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>26</v>
       </c>
@@ -5513,7 +5127,7 @@
         <v>2619097.3403039998</v>
       </c>
     </row>
-    <row r="29" spans="1:27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>27</v>
       </c>
@@ -5587,7 +5201,7 @@
         <v>5103945.4106769999</v>
       </c>
     </row>
-    <row r="30" spans="1:27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>28</v>
       </c>
@@ -5661,7 +5275,7 @@
         <v>4741171.750461</v>
       </c>
     </row>
-    <row r="31" spans="1:27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>29</v>
       </c>
@@ -5735,7 +5349,7 @@
         <v>4464167.6281199995</v>
       </c>
     </row>
-    <row r="32" spans="1:27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>30</v>
       </c>
@@ -5809,7 +5423,7 @@
         <v>808390.92652600002</v>
       </c>
     </row>
-    <row r="33" spans="1:27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>31</v>
       </c>
@@ -5883,7 +5497,7 @@
         <v>1568704</v>
       </c>
     </row>
-    <row r="34" spans="1:27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>32</v>
       </c>
@@ -5957,7 +5571,7 @@
         <v>212133.691238</v>
       </c>
     </row>
-    <row r="35" spans="1:27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>33</v>
       </c>
@@ -6031,7 +5645,7 @@
         <v>27529</v>
       </c>
     </row>
-    <row r="36" spans="1:27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>34</v>
       </c>
@@ -6105,7 +5719,7 @@
         <v>380525.64</v>
       </c>
     </row>
-    <row r="37" spans="1:27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>35</v>
       </c>
@@ -6179,7 +5793,7 @@
         <v>2274319.9700000002</v>
       </c>
     </row>
-    <row r="38" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>36</v>
       </c>
@@ -6253,7 +5867,7 @@
         <v>379316.2</v>
       </c>
     </row>
-    <row r="39" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>37</v>
       </c>
@@ -6327,7 +5941,7 @@
         <v>387046.12</v>
       </c>
     </row>
-    <row r="40" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>38</v>
       </c>
@@ -6401,7 +6015,7 @@
         <v>1117618.041373</v>
       </c>
     </row>
-    <row r="41" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>39</v>
       </c>
@@ -6475,7 +6089,7 @@
         <v>141034.4</v>
       </c>
     </row>
-    <row r="42" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>40</v>
       </c>
@@ -6549,7 +6163,7 @@
         <v>100035.041018</v>
       </c>
     </row>
-    <row r="43" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>41</v>
       </c>
@@ -6623,7 +6237,7 @@
         <v>365082.01527999999</v>
       </c>
     </row>
-    <row r="44" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>42</v>
       </c>
@@ -6697,7 +6311,7 @@
         <v>943535.51400199998</v>
       </c>
     </row>
-    <row r="45" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>43</v>
       </c>
@@ -6771,7 +6385,7 @@
         <v>287341.69527999999</v>
       </c>
     </row>
-    <row r="46" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>44</v>
       </c>
@@ -6845,7 +6459,7 @@
         <v>40207.339999999997</v>
       </c>
     </row>
-    <row r="47" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>45</v>
       </c>
@@ -6919,7 +6533,7 @@
         <v>353269</v>
       </c>
     </row>
-    <row r="48" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>46</v>
       </c>
@@ -6993,7 +6607,7 @@
         <v>664773.17561999999</v>
       </c>
     </row>
-    <row r="49" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>47</v>
       </c>
@@ -7067,7 +6681,7 @@
         <v>96536.639999999999</v>
       </c>
     </row>
-    <row r="50" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>48</v>
       </c>
@@ -7141,7 +6755,7 @@
         <v>17157</v>
       </c>
     </row>
-    <row r="51" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>49</v>
       </c>
@@ -7215,7 +6829,7 @@
         <v>3257267.9736270001</v>
       </c>
     </row>
-    <row r="52" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>50</v>
       </c>
@@ -7289,7 +6903,7 @@
         <v>1926145.1587739999</v>
       </c>
     </row>
-    <row r="53" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>51</v>
       </c>
@@ -7363,7 +6977,7 @@
         <v>4796879.8973519998</v>
       </c>
     </row>
-    <row r="54" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>52</v>
       </c>
@@ -7453,18 +7067,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74073812-F58D-4768-AC11-644789E06262}">
   <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>69</v>
       </c>
@@ -7475,7 +7089,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>73</v>
       </c>
@@ -7486,7 +7100,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -7497,7 +7111,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -7508,7 +7122,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -7519,7 +7133,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -7530,7 +7144,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -7541,7 +7155,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -7552,7 +7166,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -7563,7 +7177,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>25</v>
       </c>
@@ -7574,7 +7188,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -7585,7 +7199,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -7596,7 +7210,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>31</v>
       </c>
@@ -7607,7 +7221,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>33</v>
       </c>
@@ -7618,7 +7232,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>35</v>
       </c>
@@ -7629,7 +7243,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>37</v>
       </c>
@@ -7640,7 +7254,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>39</v>
       </c>
@@ -7648,7 +7262,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>41</v>
       </c>
@@ -7659,7 +7273,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>43</v>
       </c>
@@ -7670,7 +7284,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>84</v>
       </c>
@@ -7681,7 +7295,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>45</v>
       </c>
@@ -7692,7 +7306,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>47</v>
       </c>
@@ -7703,7 +7317,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>49</v>
       </c>
@@ -7714,7 +7328,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>51</v>
       </c>
@@ -7725,7 +7339,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>53</v>
       </c>
@@ -7736,7 +7350,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>55</v>
       </c>
@@ -7747,7 +7361,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>57</v>
       </c>
@@ -7758,7 +7372,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>59</v>
       </c>
@@ -7769,7 +7383,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>61</v>
       </c>
@@ -7780,7 +7394,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>75</v>
       </c>
@@ -7797,330 +7411,99 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6F6C565-1382-4E82-B436-2627A22CB456}">
-  <dimension ref="A1:H28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEE4E2E0-88CD-471E-9F5A-AB0C2722050D}">
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.88671875" customWidth="1"/>
-    <col min="4" max="4" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>69</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>131</v>
-      </c>
-      <c r="C1" t="s">
-        <v>132</v>
-      </c>
-      <c r="D1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
         <v>9</v>
       </c>
-      <c r="B2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" t="s">
-        <v>73</v>
-      </c>
-      <c r="D3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" t="s">
-        <v>70</v>
-      </c>
-      <c r="H5" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" t="s">
-        <v>29</v>
-      </c>
-      <c r="D11" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12" t="s">
-        <v>31</v>
-      </c>
-      <c r="D12" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>33</v>
-      </c>
-      <c r="B13" t="s">
-        <v>33</v>
-      </c>
-      <c r="D13" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>35</v>
-      </c>
-      <c r="B14" t="s">
-        <v>35</v>
-      </c>
-      <c r="D14" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>37</v>
-      </c>
-      <c r="B15" t="s">
-        <v>37</v>
-      </c>
-      <c r="D15" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>39</v>
-      </c>
-      <c r="B16" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>41</v>
-      </c>
-      <c r="B17" t="s">
-        <v>41</v>
-      </c>
-      <c r="D17" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>43</v>
-      </c>
-      <c r="B18" t="s">
-        <v>43</v>
-      </c>
-      <c r="D18" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>45</v>
-      </c>
-      <c r="B19" t="s">
-        <v>84</v>
-      </c>
-      <c r="D19" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>47</v>
-      </c>
-      <c r="B20" t="s">
-        <v>47</v>
-      </c>
-      <c r="D20" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>49</v>
-      </c>
-      <c r="B21" t="s">
-        <v>49</v>
-      </c>
-      <c r="D21" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>51</v>
-      </c>
-      <c r="B22" t="s">
-        <v>51</v>
-      </c>
-      <c r="D22" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>53</v>
-      </c>
-      <c r="B23" t="s">
-        <v>53</v>
-      </c>
-      <c r="D23" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>55</v>
-      </c>
-      <c r="B24" t="s">
-        <v>55</v>
-      </c>
-      <c r="D24" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>57</v>
-      </c>
-      <c r="B25" t="s">
-        <v>57</v>
-      </c>
-      <c r="D25" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>59</v>
-      </c>
-      <c r="B26" t="s">
-        <v>59</v>
-      </c>
-      <c r="D26" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>61</v>
-      </c>
-      <c r="B27" t="s">
-        <v>74</v>
-      </c>
-      <c r="D27" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>75</v>
-      </c>
-      <c r="B28" t="s">
-        <v>74</v>
-      </c>
-      <c r="D28" t="s">
-        <v>71</v>
+      <c r="B3">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>4</v>
+      </c>
+      <c r="B8">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>3</v>
+      </c>
+      <c r="B9">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>2</v>
+      </c>
+      <c r="B10">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -8129,99 +7512,51 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEE4E2E0-88CD-471E-9F5A-AB0C2722050D}">
-  <dimension ref="A1:B11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF0D815C-FD9D-4123-9D9D-AD3295A2835E}">
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="17.44140625" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>65</v>
       </c>
       <c r="B1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5">
         <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>10</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>9</v>
-      </c>
-      <c r="B3">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>8</v>
-      </c>
-      <c r="B4">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>7</v>
-      </c>
-      <c r="B5">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>6</v>
-      </c>
-      <c r="B6">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>5</v>
-      </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>4</v>
-      </c>
-      <c r="B8">
-        <v>1.2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>3</v>
-      </c>
-      <c r="B9">
-        <v>1.4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>2</v>
-      </c>
-      <c r="B10">
-        <v>1.6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -8230,51 +7565,51 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF0D815C-FD9D-4123-9D9D-AD3295A2835E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BC52232-62A1-4046-A953-F434B4285A01}">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>65</v>
+        <v>8</v>
       </c>
       <c r="B1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B2">
-        <v>-3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B3">
-        <v>-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="B4">
         <v>4</v>
       </c>
-      <c r="B4">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>66</v>
+        <v>7</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -8283,59 +7618,6 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BC52232-62A1-4046-A953-F434B4285A01}">
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B281CBBA-5423-42AE-9693-0C69866CF5CE}">
   <dimension ref="A1:D26"/>
   <sheetViews>
@@ -8343,14 +7625,14 @@
       <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>131</v>
       </c>
@@ -8364,7 +7646,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>73</v>
       </c>
@@ -8378,7 +7660,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -8392,7 +7674,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -8406,7 +7688,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -8420,7 +7702,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -8434,7 +7716,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -8448,7 +7730,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -8462,7 +7744,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -8476,7 +7758,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -8490,7 +7772,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -8504,7 +7786,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>33</v>
       </c>
@@ -8518,7 +7800,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -8532,7 +7814,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>37</v>
       </c>
@@ -8546,7 +7828,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>39</v>
       </c>
@@ -8560,7 +7842,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>41</v>
       </c>
@@ -8574,7 +7856,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>43</v>
       </c>
@@ -8588,7 +7870,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>84</v>
       </c>
@@ -8602,7 +7884,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>47</v>
       </c>
@@ -8616,7 +7898,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>49</v>
       </c>
@@ -8630,7 +7912,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>51</v>
       </c>
@@ -8644,7 +7926,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>53</v>
       </c>
@@ -8658,7 +7940,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>55</v>
       </c>
@@ -8672,7 +7954,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>57</v>
       </c>
@@ -8686,7 +7968,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>59</v>
       </c>
@@ -8700,7 +7982,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>74</v>
       </c>
@@ -8719,7 +8001,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AE2FD76-BC91-45B2-B5B8-525E322D787E}">
   <dimension ref="A1:D26"/>
   <sheetViews>
@@ -8727,15 +8009,15 @@
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>131</v>
       </c>
@@ -8749,7 +8031,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>73</v>
       </c>
@@ -8763,7 +8045,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -8777,7 +8059,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -8791,7 +8073,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -8805,7 +8087,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -8819,7 +8101,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -8833,7 +8115,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -8847,7 +8129,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -8861,7 +8143,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -8875,7 +8157,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -8889,7 +8171,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>33</v>
       </c>
@@ -8903,7 +8185,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -8917,7 +8199,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>37</v>
       </c>
@@ -8931,7 +8213,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>39</v>
       </c>
@@ -8945,7 +8227,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>41</v>
       </c>
@@ -8959,7 +8241,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>43</v>
       </c>
@@ -8973,7 +8255,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>84</v>
       </c>
@@ -8987,7 +8269,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>47</v>
       </c>
@@ -9001,7 +8283,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>49</v>
       </c>
@@ -9015,7 +8297,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>51</v>
       </c>
@@ -9029,7 +8311,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>53</v>
       </c>
@@ -9043,7 +8325,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>55</v>
       </c>
@@ -9057,7 +8339,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>57</v>
       </c>
@@ -9071,7 +8353,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>59</v>
       </c>
@@ -9085,7 +8367,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>74</v>
       </c>
@@ -9104,7 +8386,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B442153-1068-48BB-9E2A-4ABB5CD9BD58}">
   <dimension ref="A1:D26"/>
   <sheetViews>
@@ -9112,14 +8394,14 @@
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>131</v>
       </c>
@@ -9133,7 +8415,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>73</v>
       </c>
@@ -9147,7 +8429,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -9161,7 +8443,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -9175,7 +8457,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -9189,7 +8471,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -9203,7 +8485,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -9217,7 +8499,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -9231,7 +8513,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -9245,7 +8527,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -9259,7 +8541,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -9273,7 +8555,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>33</v>
       </c>
@@ -9287,7 +8569,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -9301,7 +8583,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>37</v>
       </c>
@@ -9315,7 +8597,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>39</v>
       </c>
@@ -9329,7 +8611,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>41</v>
       </c>
@@ -9343,7 +8625,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>43</v>
       </c>
@@ -9357,7 +8639,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>84</v>
       </c>
@@ -9371,7 +8653,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>47</v>
       </c>
@@ -9385,7 +8667,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>49</v>
       </c>
@@ -9399,7 +8681,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>51</v>
       </c>
@@ -9413,7 +8695,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>53</v>
       </c>
@@ -9427,7 +8709,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>55</v>
       </c>
@@ -9441,7 +8723,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>57</v>
       </c>
@@ -9455,7 +8737,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>59</v>
       </c>
@@ -9469,7 +8751,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>74</v>
       </c>
@@ -9481,6 +8763,385 @@
       </c>
       <c r="D26">
         <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{200F6E0C-51C0-4CFC-8295-6BC9A0CB5165}">
+  <dimension ref="A1:D26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2">
+        <v>6.86</v>
+      </c>
+      <c r="D2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3">
+        <v>5.28</v>
+      </c>
+      <c r="D3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4">
+        <v>6.41</v>
+      </c>
+      <c r="D4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5">
+        <v>5.88</v>
+      </c>
+      <c r="D5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7">
+        <v>6.24</v>
+      </c>
+      <c r="D7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9">
+        <v>9.14</v>
+      </c>
+      <c r="D9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10">
+        <v>7.39</v>
+      </c>
+      <c r="D10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11">
+        <v>6.28</v>
+      </c>
+      <c r="D11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12">
+        <v>5.39</v>
+      </c>
+      <c r="D12">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13">
+        <v>7.9</v>
+      </c>
+      <c r="D13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14">
+        <v>5.99</v>
+      </c>
+      <c r="D14">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15">
+        <v>6.49</v>
+      </c>
+      <c r="D15">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16">
+        <v>5.32</v>
+      </c>
+      <c r="D16">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17">
+        <v>8.06</v>
+      </c>
+      <c r="D17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>84</v>
+      </c>
+      <c r="B18" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18">
+        <v>5.88</v>
+      </c>
+      <c r="D18">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19">
+        <v>7.67</v>
+      </c>
+      <c r="D19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>49</v>
+      </c>
+      <c r="B20" t="s">
+        <v>50</v>
+      </c>
+      <c r="C20">
+        <v>4.45</v>
+      </c>
+      <c r="D20">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>51</v>
+      </c>
+      <c r="B21" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21">
+        <v>6.82</v>
+      </c>
+      <c r="D21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22" t="s">
+        <v>54</v>
+      </c>
+      <c r="C22">
+        <v>5.93</v>
+      </c>
+      <c r="D22">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>55</v>
+      </c>
+      <c r="B23" t="s">
+        <v>56</v>
+      </c>
+      <c r="C23">
+        <v>7.6</v>
+      </c>
+      <c r="D23">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>57</v>
+      </c>
+      <c r="B24" t="s">
+        <v>58</v>
+      </c>
+      <c r="C24">
+        <v>6.22</v>
+      </c>
+      <c r="D24">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>59</v>
+      </c>
+      <c r="B25" t="s">
+        <v>60</v>
+      </c>
+      <c r="C25">
+        <v>9.3800000000000008</v>
+      </c>
+      <c r="D25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>74</v>
+      </c>
+      <c r="B26" t="s">
+        <v>62</v>
+      </c>
+      <c r="C26">
+        <v>6.46</v>
+      </c>
+      <c r="D26">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adjust dumpsite function to handle variable field name prefixes. Updated lookup to include "Watts Branch" as location_name
</commit_message>
<xml_diff>
--- a/data/lookup_tables.xlsx
+++ b/data/lookup_tables.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\srucker\Git\SCI\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9216B83E-AC55-4F2D-9FE4-B5F56D2CA152}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A58E5B4-18F9-46D6-98DC-5FEA9AFC8138}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{23697FDE-567D-4570-AE33-F8F65584BB36}"/>
   </bookViews>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1262" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1265" uniqueCount="137">
   <si>
     <t>max_sites_per_mile</t>
   </si>
@@ -7065,10 +7065,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74073812-F58D-4768-AC11-644789E06262}">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7385,7 +7385,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>61</v>
+        <v>74</v>
       </c>
       <c r="B29" t="s">
         <v>74</v>
@@ -7396,12 +7396,23 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="B30" t="s">
         <v>74</v>
       </c>
       <c r="C30" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>75</v>
+      </c>
+      <c r="B31" t="s">
+        <v>74</v>
+      </c>
+      <c r="C31" t="s">
         <v>71</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated lookups to replace Melvin Hazen Valley Branch with Reservation 630.
Still need to make update for EIA
</commit_message>
<xml_diff>
--- a/data/lookup_tables.xlsx
+++ b/data/lookup_tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\srucker\Git\SCI\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A58E5B4-18F9-46D6-98DC-5FEA9AFC8138}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23563AAD-BC0F-407A-88FB-6A7900914E7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{23697FDE-567D-4570-AE33-F8F65584BB36}"/>
   </bookViews>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1265" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1268" uniqueCount="138">
   <si>
     <t>max_sites_per_mile</t>
   </si>
@@ -462,6 +462,9 @@
   </si>
   <si>
     <t>THR02</t>
+  </si>
+  <si>
+    <t>Reservation 630</t>
   </si>
 </sst>
 </file>
@@ -845,7 +848,7 @@
   <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q17" sqref="Q17"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1003,7 +1006,7 @@
         <v>42</v>
       </c>
       <c r="B19" t="s">
-        <v>41</v>
+        <v>137</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -1112,7 +1115,7 @@
   <dimension ref="A1:L27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2112,8 +2115,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FCF3A67-4696-4690-90E1-1249EF121DBC}">
   <dimension ref="A1:O18"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3109,7 +3112,7 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:AA54"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P63" sqref="P63"/>
     </sheetView>
   </sheetViews>
@@ -7065,10 +7068,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74073812-F58D-4768-AC11-644789E06262}">
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7267,7 +7270,7 @@
         <v>41</v>
       </c>
       <c r="B18" t="s">
-        <v>41</v>
+        <v>137</v>
       </c>
       <c r="C18" t="s">
         <v>70</v>
@@ -7275,29 +7278,29 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>43</v>
+        <v>137</v>
       </c>
       <c r="B19" t="s">
-        <v>43</v>
+        <v>137</v>
       </c>
       <c r="C19" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>84</v>
+        <v>43</v>
       </c>
       <c r="B20" t="s">
-        <v>84</v>
+        <v>43</v>
       </c>
       <c r="C20" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>45</v>
+        <v>84</v>
       </c>
       <c r="B21" t="s">
         <v>84</v>
@@ -7308,21 +7311,21 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B22" t="s">
-        <v>47</v>
+        <v>84</v>
       </c>
       <c r="C22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B23" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C23" t="s">
         <v>71</v>
@@ -7330,21 +7333,21 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B24" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C24" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B25" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C25" t="s">
         <v>70</v>
@@ -7352,10 +7355,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B26" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C26" t="s">
         <v>70</v>
@@ -7363,10 +7366,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B27" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C27" t="s">
         <v>70</v>
@@ -7374,21 +7377,21 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B28" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C28" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="B29" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="C29" t="s">
         <v>71</v>
@@ -7396,7 +7399,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>61</v>
+        <v>74</v>
       </c>
       <c r="B30" t="s">
         <v>74</v>
@@ -7407,12 +7410,23 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="B31" t="s">
         <v>74</v>
       </c>
       <c r="C31" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>75</v>
+      </c>
+      <c r="B32" t="s">
+        <v>74</v>
+      </c>
+      <c r="C32" t="s">
         <v>71</v>
       </c>
     </row>
@@ -7633,7 +7647,7 @@
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7855,7 +7869,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>41</v>
+        <v>137</v>
       </c>
       <c r="B16" t="s">
         <v>42</v>
@@ -8017,7 +8031,7 @@
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8240,7 +8254,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>41</v>
+        <v>137</v>
       </c>
       <c r="B16" t="s">
         <v>42</v>
@@ -8402,7 +8416,7 @@
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8624,7 +8638,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>41</v>
+        <v>137</v>
       </c>
       <c r="B16" t="s">
         <v>42</v>
@@ -8786,7 +8800,7 @@
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9003,7 +9017,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>41</v>
+        <v>137</v>
       </c>
       <c r="B16" t="s">
         <v>42</v>

</xml_diff>

<commit_message>
Update readme and vignettes
</commit_message>
<xml_diff>
--- a/data/lookup_tables.xlsx
+++ b/data/lookup_tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\srucker\Git\SCI\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9032371B-CD04-4049-BD41-70906A1FF635}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{119A69C2-4C13-4068-B699-2E7808ADCA3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-12225" windowWidth="25440" windowHeight="15390" firstSheet="6" activeTab="11" xr2:uid="{23697FDE-567D-4570-AE33-F8F65584BB36}"/>
+    <workbookView xWindow="28680" yWindow="-12225" windowWidth="25440" windowHeight="15390" firstSheet="6" activeTab="10" xr2:uid="{23697FDE-567D-4570-AE33-F8F65584BB36}"/>
   </bookViews>
   <sheets>
     <sheet name="location_id" sheetId="19" r:id="rId1"/>
@@ -27,6 +27,7 @@
     <sheet name="eia_score" sheetId="16" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1967,8 +1968,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FCF3A67-4696-4690-90E1-1249EF121DBC}">
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:H18"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2620,7 +2621,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A15AB59E-477A-404D-9A36-733C66688157}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
@@ -4076,6 +4077,7 @@
   <cols>
     <col min="1" max="1" width="25.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.88671875" customWidth="1"/>
     <col min="4" max="4" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
Specify Luzon Branch ecoregion. Save all_scores as CSV in output folder.
</commit_message>
<xml_diff>
--- a/data/lookup_tables.xlsx
+++ b/data/lookup_tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\srucker\Git\SCI\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{119A69C2-4C13-4068-B699-2E7808ADCA3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05677B0F-C594-4AB1-90CA-C4D8C53B08C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-12225" windowWidth="25440" windowHeight="15390" firstSheet="6" activeTab="10" xr2:uid="{23697FDE-567D-4570-AE33-F8F65584BB36}"/>
+    <workbookView xWindow="28740" yWindow="-16005" windowWidth="25440" windowHeight="15270" activeTab="1" xr2:uid="{23697FDE-567D-4570-AE33-F8F65584BB36}"/>
   </bookViews>
   <sheets>
     <sheet name="location_id" sheetId="19" r:id="rId1"/>
@@ -27,7 +27,6 @@
     <sheet name="eia_score" sheetId="16" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -48,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="103">
   <si>
     <t>max_sites_per_mile</t>
   </si>
@@ -736,13 +735,13 @@
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>63</v>
       </c>
@@ -750,7 +749,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -758,7 +757,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -766,7 +765,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -774,7 +773,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -782,7 +781,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -790,7 +789,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -798,7 +797,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -806,7 +805,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -814,7 +813,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>99</v>
       </c>
@@ -822,7 +821,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -830,7 +829,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>30</v>
       </c>
@@ -838,7 +837,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>32</v>
       </c>
@@ -846,7 +845,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>34</v>
       </c>
@@ -854,7 +853,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>36</v>
       </c>
@@ -862,7 +861,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>100</v>
       </c>
@@ -870,7 +869,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>38</v>
       </c>
@@ -878,7 +877,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>40</v>
       </c>
@@ -886,7 +885,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>42</v>
       </c>
@@ -894,7 +893,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>44</v>
       </c>
@@ -902,7 +901,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>46</v>
       </c>
@@ -910,7 +909,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>48</v>
       </c>
@@ -918,7 +917,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>50</v>
       </c>
@@ -926,7 +925,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>52</v>
       </c>
@@ -934,7 +933,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>54</v>
       </c>
@@ -942,7 +941,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>56</v>
       </c>
@@ -950,7 +949,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>58</v>
       </c>
@@ -958,7 +957,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>60</v>
       </c>
@@ -966,7 +965,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>62</v>
       </c>
@@ -974,7 +973,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>68</v>
       </c>
@@ -982,7 +981,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>67</v>
       </c>
@@ -1003,21 +1002,21 @@
       <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="42.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.109375" customWidth="1"/>
-    <col min="9" max="9" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="27.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.08984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.90625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.08984375" customWidth="1"/>
+    <col min="9" max="9" width="19.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>98</v>
       </c>
@@ -1049,7 +1048,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>14</v>
       </c>
@@ -1084,7 +1083,7 @@
         <v>26487.214122240002</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
@@ -1119,7 +1118,7 @@
         <v>76874.450765425325</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
@@ -1154,7 +1153,7 @@
         <v>23139.45307584</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>21</v>
       </c>
@@ -1189,7 +1188,7 @@
         <v>11828.730923136</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>31</v>
       </c>
@@ -1224,7 +1223,7 @@
         <v>6249.2345953731656</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>27</v>
       </c>
@@ -1259,7 +1258,7 @@
         <v>30926.7215270784</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>29</v>
       </c>
@@ -1294,7 +1293,7 @@
         <v>12328.301321980302</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>23</v>
       </c>
@@ -1329,7 +1328,7 @@
         <v>15534.227254476902</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>33</v>
       </c>
@@ -1364,7 +1363,7 @@
         <v>64799.294401152009</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>25</v>
       </c>
@@ -1399,7 +1398,7 @@
         <v>198108.23926903613</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>35</v>
       </c>
@@ -1434,7 +1433,7 @@
         <v>1582820.0720122508</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>37</v>
       </c>
@@ -1469,7 +1468,7 @@
         <v>29429.919333798451</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>39</v>
       </c>
@@ -1504,7 +1503,7 @@
         <v>85543.649502339729</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>101</v>
       </c>
@@ -1539,7 +1538,7 @@
         <v>23970.50377523205</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>43</v>
       </c>
@@ -1574,7 +1573,7 @@
         <v>66905.076848097378</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>81</v>
       </c>
@@ -1609,7 +1608,7 @@
         <v>27347.774981760002</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>47</v>
       </c>
@@ -1644,7 +1643,7 @@
         <v>436011.69874767505</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>51</v>
       </c>
@@ -1679,7 +1678,7 @@
         <v>69298.720686307235</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>55</v>
       </c>
@@ -1714,7 +1713,7 @@
         <v>6639.0035993856</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>49</v>
       </c>
@@ -1749,7 +1748,7 @@
         <v>6755.6461531968007</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>53</v>
       </c>
@@ -1784,7 +1783,7 @@
         <v>1318.94445888</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>55</v>
       </c>
@@ -1819,7 +1818,7 @@
         <v>364009.03523212724</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>57</v>
       </c>
@@ -1854,7 +1853,7 @@
         <v>91720.743835564819</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>59</v>
       </c>
@@ -1889,7 +1888,7 @@
         <v>94237.666040523225</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>74</v>
       </c>
@@ -1924,7 +1923,7 @@
         <v>149667.65312902408</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>74</v>
       </c>
@@ -1968,24 +1967,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FCF3A67-4696-4690-90E1-1249EF121DBC}">
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="25.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="41.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.33203125" customWidth="1"/>
-    <col min="7" max="7" width="23.33203125" customWidth="1"/>
-    <col min="8" max="8" width="30.109375" customWidth="1"/>
-    <col min="9" max="9" width="23.6640625" customWidth="1"/>
-    <col min="10" max="10" width="27.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="25.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="41.90625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.36328125" customWidth="1"/>
+    <col min="7" max="7" width="23.36328125" customWidth="1"/>
+    <col min="8" max="8" width="30.08984375" customWidth="1"/>
+    <col min="9" max="9" width="23.6328125" customWidth="1"/>
+    <col min="10" max="10" width="27.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>98</v>
       </c>
@@ -2017,7 +2016,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>73</v>
       </c>
@@ -2052,7 +2051,7 @@
         <v>364009.03523212724</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>73</v>
       </c>
@@ -2087,7 +2086,7 @@
         <v>242715.20037653751</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>73</v>
       </c>
@@ -2122,7 +2121,7 @@
         <v>209289.48596387706</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>73</v>
       </c>
@@ -2157,7 +2156,7 @@
         <v>6639.0035993856</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>73</v>
       </c>
@@ -2192,7 +2191,7 @@
         <v>29429.919333798451</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>73</v>
       </c>
@@ -2227,7 +2226,7 @@
         <v>91720.743835564819</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>73</v>
       </c>
@@ -2262,7 +2261,7 @@
         <v>23970.50377523205</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>73</v>
       </c>
@@ -2297,7 +2296,7 @@
         <v>6249.2345953731656</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>73</v>
       </c>
@@ -2332,7 +2331,7 @@
         <v>1318.94445888</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>73</v>
       </c>
@@ -2367,7 +2366,7 @@
         <v>85543.649502339729</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>73</v>
       </c>
@@ -2402,7 +2401,7 @@
         <v>69298.720686307235</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>73</v>
       </c>
@@ -2437,7 +2436,7 @@
         <v>41437.078416000004</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>73</v>
       </c>
@@ -2472,7 +2471,7 @@
         <v>76874.450765425325</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>73</v>
       </c>
@@ -2507,7 +2506,7 @@
         <v>6897.1216895999996</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>73</v>
       </c>
@@ -2542,7 +2541,7 @@
         <v>27347.774981760002</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>73</v>
       </c>
@@ -2577,7 +2576,7 @@
         <v>11828.730923136</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>73</v>
       </c>
@@ -2625,9 +2624,9 @@
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -2635,7 +2634,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>10</v>
       </c>
@@ -2643,7 +2642,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>9</v>
       </c>
@@ -2651,7 +2650,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>8</v>
       </c>
@@ -2659,7 +2658,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>7</v>
       </c>
@@ -2667,7 +2666,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>6</v>
       </c>
@@ -2675,7 +2674,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>5</v>
       </c>
@@ -2683,7 +2682,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>4</v>
       </c>
@@ -2691,7 +2690,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>3</v>
       </c>
@@ -2699,7 +2698,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>2</v>
       </c>
@@ -2707,7 +2706,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>1</v>
       </c>
@@ -2724,18 +2723,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74073812-F58D-4768-AC11-644789E06262}">
   <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>69</v>
       </c>
@@ -2746,7 +2745,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>73</v>
       </c>
@@ -2757,7 +2756,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -2768,7 +2767,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -2779,7 +2778,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -2790,7 +2789,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -2801,7 +2800,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -2812,7 +2811,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -2823,7 +2822,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -2834,7 +2833,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>25</v>
       </c>
@@ -2845,7 +2844,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -2856,7 +2855,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -2867,7 +2866,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>31</v>
       </c>
@@ -2878,7 +2877,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>33</v>
       </c>
@@ -2889,7 +2888,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>35</v>
       </c>
@@ -2900,7 +2899,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>37</v>
       </c>
@@ -2911,15 +2910,18 @@
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>39</v>
       </c>
       <c r="B17" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C17" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>41</v>
       </c>
@@ -2930,7 +2932,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>101</v>
       </c>
@@ -2941,7 +2943,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>43</v>
       </c>
@@ -2952,7 +2954,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>81</v>
       </c>
@@ -2963,7 +2965,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>45</v>
       </c>
@@ -2974,7 +2976,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>47</v>
       </c>
@@ -2985,7 +2987,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>49</v>
       </c>
@@ -2996,7 +2998,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>51</v>
       </c>
@@ -3007,7 +3009,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>53</v>
       </c>
@@ -3018,7 +3020,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>55</v>
       </c>
@@ -3029,7 +3031,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>57</v>
       </c>
@@ -3040,7 +3042,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>59</v>
       </c>
@@ -3051,7 +3053,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>74</v>
       </c>
@@ -3062,7 +3064,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>61</v>
       </c>
@@ -3073,7 +3075,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>75</v>
       </c>
@@ -3095,12 +3097,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -3108,7 +3110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>10</v>
       </c>
@@ -3116,7 +3118,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>9</v>
       </c>
@@ -3124,7 +3126,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>8</v>
       </c>
@@ -3132,7 +3134,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>7</v>
       </c>
@@ -3140,7 +3142,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>6</v>
       </c>
@@ -3148,7 +3150,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>5</v>
       </c>
@@ -3156,7 +3158,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>4</v>
       </c>
@@ -3164,7 +3166,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>3</v>
       </c>
@@ -3172,7 +3174,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>2</v>
       </c>
@@ -3180,7 +3182,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>1</v>
       </c>
@@ -3196,9 +3198,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>65</v>
       </c>
@@ -3206,7 +3208,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -3214,7 +3216,7 @@
         <v>-3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -3222,7 +3224,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -3230,7 +3232,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>66</v>
       </c>
@@ -3249,9 +3251,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -3259,7 +3261,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -3267,7 +3269,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -3275,7 +3277,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -3283,7 +3285,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -3304,14 +3306,14 @@
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>98</v>
       </c>
@@ -3325,7 +3327,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>73</v>
       </c>
@@ -3339,7 +3341,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -3353,7 +3355,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -3367,7 +3369,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -3381,7 +3383,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -3395,7 +3397,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -3409,7 +3411,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -3423,7 +3425,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -3437,7 +3439,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -3451,7 +3453,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -3465,7 +3467,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>33</v>
       </c>
@@ -3479,7 +3481,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -3493,7 +3495,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>37</v>
       </c>
@@ -3507,7 +3509,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>39</v>
       </c>
@@ -3521,7 +3523,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>101</v>
       </c>
@@ -3535,7 +3537,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>43</v>
       </c>
@@ -3549,7 +3551,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>81</v>
       </c>
@@ -3563,7 +3565,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>47</v>
       </c>
@@ -3577,7 +3579,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>49</v>
       </c>
@@ -3591,7 +3593,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>51</v>
       </c>
@@ -3605,7 +3607,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>53</v>
       </c>
@@ -3619,7 +3621,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>55</v>
       </c>
@@ -3633,7 +3635,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>57</v>
       </c>
@@ -3647,7 +3649,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>59</v>
       </c>
@@ -3661,7 +3663,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>74</v>
       </c>
@@ -3688,15 +3690,15 @@
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>98</v>
       </c>
@@ -3710,7 +3712,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>73</v>
       </c>
@@ -3724,7 +3726,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -3738,7 +3740,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -3752,7 +3754,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -3766,7 +3768,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -3780,7 +3782,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -3794,7 +3796,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -3808,7 +3810,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -3822,7 +3824,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -3836,7 +3838,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -3850,7 +3852,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>33</v>
       </c>
@@ -3864,7 +3866,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -3878,7 +3880,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>37</v>
       </c>
@@ -3892,7 +3894,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>39</v>
       </c>
@@ -3906,7 +3908,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>101</v>
       </c>
@@ -3920,7 +3922,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>43</v>
       </c>
@@ -3934,7 +3936,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>81</v>
       </c>
@@ -3948,7 +3950,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>47</v>
       </c>
@@ -3962,7 +3964,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>49</v>
       </c>
@@ -3976,7 +3978,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>51</v>
       </c>
@@ -3990,7 +3992,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>53</v>
       </c>
@@ -4004,7 +4006,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>55</v>
       </c>
@@ -4018,7 +4020,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>57</v>
       </c>
@@ -4032,7 +4034,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>59</v>
       </c>
@@ -4046,7 +4048,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>74</v>
       </c>
@@ -4073,15 +4075,15 @@
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.88671875" customWidth="1"/>
-    <col min="4" max="4" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.90625" customWidth="1"/>
+    <col min="4" max="4" width="10.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>98</v>
       </c>
@@ -4095,7 +4097,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>73</v>
       </c>
@@ -4109,7 +4111,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -4123,7 +4125,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -4137,7 +4139,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -4151,7 +4153,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -4165,7 +4167,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -4179,7 +4181,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -4193,7 +4195,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -4207,7 +4209,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -4221,7 +4223,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -4235,7 +4237,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>33</v>
       </c>
@@ -4249,7 +4251,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -4263,7 +4265,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>37</v>
       </c>
@@ -4277,7 +4279,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>39</v>
       </c>
@@ -4291,7 +4293,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>101</v>
       </c>
@@ -4305,7 +4307,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>43</v>
       </c>
@@ -4319,7 +4321,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>81</v>
       </c>
@@ -4333,7 +4335,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>47</v>
       </c>
@@ -4347,7 +4349,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>49</v>
       </c>
@@ -4361,7 +4363,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>51</v>
       </c>
@@ -4375,7 +4377,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>53</v>
       </c>
@@ -4389,7 +4391,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>55</v>
       </c>
@@ -4403,7 +4405,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>57</v>
       </c>
@@ -4417,7 +4419,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>59</v>
       </c>
@@ -4431,7 +4433,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>74</v>
       </c>
@@ -4458,15 +4460,15 @@
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>98</v>
       </c>
@@ -4480,7 +4482,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>73</v>
       </c>
@@ -4494,7 +4496,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -4508,7 +4510,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -4522,7 +4524,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -4536,7 +4538,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -4550,7 +4552,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -4564,7 +4566,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -4572,7 +4574,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -4586,7 +4588,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -4600,7 +4602,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -4614,7 +4616,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>33</v>
       </c>
@@ -4628,7 +4630,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -4642,7 +4644,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>37</v>
       </c>
@@ -4656,7 +4658,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>39</v>
       </c>
@@ -4670,7 +4672,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>101</v>
       </c>
@@ -4684,7 +4686,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>43</v>
       </c>
@@ -4698,7 +4700,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>81</v>
       </c>
@@ -4712,7 +4714,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>47</v>
       </c>
@@ -4726,7 +4728,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>49</v>
       </c>
@@ -4740,7 +4742,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>51</v>
       </c>
@@ -4754,7 +4756,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>53</v>
       </c>
@@ -4768,7 +4770,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>55</v>
       </c>
@@ -4782,7 +4784,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>57</v>
       </c>
@@ -4796,7 +4798,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>59</v>
       </c>
@@ -4810,7 +4812,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>74</v>
       </c>

</xml_diff>

<commit_message>
Update aquatic life score ranges
</commit_message>
<xml_diff>
--- a/data/lookup_tables.xlsx
+++ b/data/lookup_tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\srucker\Git\SCI\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05677B0F-C594-4AB1-90CA-C4D8C53B08C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AE23ADF-2C79-43AA-896C-680376F2DCD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28740" yWindow="-16005" windowWidth="25440" windowHeight="15270" activeTab="1" xr2:uid="{23697FDE-567D-4570-AE33-F8F65584BB36}"/>
+    <workbookView xWindow="-15060" yWindow="-16320" windowWidth="29040" windowHeight="15720" firstSheet="4" activeTab="8" xr2:uid="{23697FDE-567D-4570-AE33-F8F65584BB36}"/>
   </bookViews>
   <sheets>
     <sheet name="location_id" sheetId="19" r:id="rId1"/>
@@ -2621,7 +2621,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2723,7 +2723,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74073812-F58D-4768-AC11-644789E06262}">
   <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
@@ -3687,7 +3687,7 @@
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4072,7 +4072,7 @@
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4360,7 +4360,7 @@
         <v>73.84</v>
       </c>
       <c r="D20">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
@@ -4430,7 +4430,7 @@
         <v>65.17</v>
       </c>
       <c r="D25">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
@@ -4456,8 +4456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{200F6E0C-51C0-4CFC-8295-6BC9A0CB5165}">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>